<commit_message>
Improve JSON filename comparison logic to avoid double '.json' extensions
Fixes the logic for converting PDF filenames to JSON for output comparison, preventing double .json extensions and improving the accuracy of the script’s output.
</commit_message>
<xml_diff>
--- a/inputExcel/CAO_Frequencies_2014.xlsx
+++ b/inputExcel/CAO_Frequencies_2014.xlsx
@@ -503,19 +503,11 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
         <v>0</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
@@ -541,19 +533,11 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
@@ -577,19 +561,15 @@
         <v>39</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>CAO%20UZK%20april%202011%20integraal.pdf, ABU%20CAO%20voor%20Uitzendkrachten%202024.pdf, CAO_voor_Uitzendkrachten_dec__2012_integraal.pdf, Cao%20voor%20Uitzendkrachten%202026-2028.pdf, ABU%20CAO%20voor%20Uitzendkrachten%2030-12-2019%20integraal%20dec.pdf, ABU%20CAO%20voor%20Uitzendkrachten%202022%20integraal.pdf, CAO_voor_uzk_16_9_2015_integraal.pdf, CAO_voor_uzk_14_10_2015_integraal.pdf, CAO_1_november_integraal.pdf, ABU%20CAO%20voor%20Uitzendkrachten%2030-12-2019.pdf, ABU%20CAO%20voor%20Uitzendkrachten%202023%20integraal.pdf, CAO_voor_Uitzendkrachten_1_4__2012_integraal.pdf, ABU%20CAO%20voor%20Uitzendkrachten%201-1-2021%20wijz.%20bijhouden.doc.pdf, Uitzendkrachten_tekst.pdf, CAO_voor_uzk_29_6_2015_integraal.pdf, ABU%20CAO%20voor%20Uitzendkrachten%2030-12-2019%20integraal%20mei.pdf, CAO_voor_uzk_29_12_14_integraal.pdf, CAO_integrale_tekst.pdf, Cao_integraal_1_7_2018.pdf, CAO_mei_2011_integraal.pdf, Cao%201-7-2019%20integraal.pdf, CAO_voor_Uitzendkrachten_integraal.pdf, Cao_integraal_1_7_2017.pdf, Cao_integraal.pdf, CAO_voor_Uitzendkrachten_5_11_2012_integraal.pdf, CAO%20UZK%20januari%202011%20integraal.pdf, Cao_integraal_1_1_2019_integraal.pdf, ABU%20CAO%20voor%20Uitzendkrachten%202023%20integraal%209-03-23.pdf, ABU%20CAO%20voor%20Uitzendkrachten%202021%20-%202023%20versie%20januari%202023%20met%20integraal.pdf, ABU%20CAO%20voor%20Uitzendkrachten%202021%20-%202023%20versie%20juli%202022%20integraal.pdf, CAO_voor_Uitzendkrachten_maart_2013_integraal.pdf, Cao_integraal_5_11_2017.pdf, ABU-LBV%20CAO%20voor%20Uitzendkrachten%202021%20integraal%207-22.pdf, ABU%20CAO%20voor%20Uitzendkrachten%2030-12-2019%20integraal%202020.doc.pdf, CAO_voor_Uitzendkrachten_juli_2013_integraal.pdf</t>
-        </is>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>1</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>ABU-LBV CAO voor Uitzendkrachten 2021 integraal 7-22.json, Cao_integraal_1_7_2017.json, Cao_integraal_5_11_2017.json, Cao_integraal.json, ABU CAO voor Uitzendkrachten 2023 integraal 9-03-23.json, CAO_integrale_tekst.json, CAO_voor_uzk_14_10_2015_integraal.json, CAO_mei_2011_integraal.json, Cao_integraal_1_1_2019_integraal.json, CAO_1_november_integraal.json, ABU CAO voor Uitzendkrachten 2022 integraal.json, ABU CAO voor Uitzendkrachten 30-12-2019.json, ABU CAO voor Uitzendkrachten 2021 - 2023 versie juli 2022 integraal.json, CAO UZK januari 2011 integraal.json, ABU CAO voor Uitzendkrachten 2021 - 2023 versie januari 2023 met integraal.json, Cao_integraal_5_11_2017_1.json, ABU CAO voor Uitzendkrachten 2023 integraal_1.json, CAO_voor_uzk_16_9_2015_integraal.json, ABU CAO voor Uitzendkrachten 30-12-2019 integraal mei.json, ABU CAO voor Uitzendkrachten 2023 integraal.json, CAO_voor_Uitzendkrachten_dec__2012_integraal.json, CAO_voor_Uitzendkrachten_5_11_2012_integraal.json, ABU CAO voor Uitzendkrachten 30-12-2019 integraal 2020.doc.json, CAO_voor_Uitzendkrachten_juli_2013_integraal.json, CAO_voor_Uitzendkrachten_maart_2013_integraal.json, CAO_voor_Uitzendkrachten_1_4__2012_integraal.json, Cao voor Uitzendkrachten 2026-2028.json, CAO UZK april 2011 integraal.json, Uitzendkrachten_tekst.json, ABU CAO voor Uitzendkrachten 30-12-2019 integraal dec.json, Cao 1-7-2019 integraal.json, CAO_voor_Uitzendkrachten_integraal_1.json, CAO_voor_uzk_29_6_2015_integraal.json, ABU CAO voor Uitzendkrachten 1-1-2021 wijz. bijhouden.doc.json, CAO_voor_Uitzendkrachten_integraal.json, CAO_voor_uzk_29_12_14_integraal.json, Cao_integraal_1_7_2018.json, ABU CAO voor Uitzendkrachten 2024.json</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -614,22 +594,18 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
         <v>1</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>KHN_cao_2018_2019.json, 20200310 cao_horeca_2020_wijziging_op_kvo.docx.json, 20221124 cao_horeca_2022-2023 na 2020_wijziging bijlage loontabellen schoon.json, 202404~2.json, Horeca_CAO_.json, 20240103 cao_horeca_2024 - tussentijdse wijziging - schone versie.json, Cao Horeca 2025-2026 incl handboek.json, cao_horeca_2018_2019_na_ttw2.json, 20200101 cao_horeca_2020_wijziging_op_ttw2_schone versie.docx.json, 20220524 cao_horeca_2022-2023 na 2020_wijziging bijlage loontabellen schoon.json, 20220101 cao_horeca_2022-2023 na 2020_wijziging_op_kvo_avv versie bronbestand.do.json, 20131221 cao_horeca_2024 - schone versie.json, 20220520 cao_horeca_2022-2023 na 2020_wijziging mei-avv.json</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -657,19 +633,15 @@
         <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
         <v>1</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO VGL 2024 tot en met 2026 .json, CAO VGL 2017-2019 v4 schoon 300418 incl loonschalen def. 090518.docx .json, VGL_Cao_2013___2017_getekend.json, CAO VGL 2019-2020 definitief schoon 010420.docx.json, 211229 CAO VGL 2020 tot en met 2023 met aangepaste loonschalen - 23-12-2021 V.json, 240105 VGL-cao 2023 tot en met 2024 met aangepaste loonschalen - DEF. (schoon).json</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -699,19 +671,11 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>0</v>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
@@ -732,22 +696,18 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>1</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>NVZ CAO 2021 2023 schone versie.json, Cao Ziekenhuizen 2023-2025.json, NLVRZH067_CAO_Ziekenhuizen_14PM.json, CAO_Ziekenhuizen_totaal.json, NVZ CAO 2021 2023 schone versie compleet.json, Tekst_Cao_Ziekenhuizen_2011_2014_definitief.json, Ziekenhuizen_2011_2014_zonder_renvooi.json, CAO_ziekenhuizen_2017_2019_DEF.json</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -775,19 +735,15 @@
         <v>13</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>1</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO LMB 2019 - 2020 V 210220 def .docx.json, CAO LMB 2020 2023 schone versie feb 22.json, CAO_LMB_2013_2017_SZW_schoon_V3_20160530.json, CAO LMB incl fuwa 2020 2023 schone versie feb 22.json, CAO_LMB_2013_2017_SZW_schoon.json, CAO LMB incl fuwa 2023 - schoon getekend.json, Vakcentrum CAO 2024-2026 .json, CAO LMB 2020 2023 schone versie.json, CAO LMB incl fuwa 2023 - schoon v 20231808 ongetekend.json, CAO_LMB_2013_2017_SZW_V4_schoon.json, CAO_LMB_2017____2019_def_01_02_2018_schone_versie.json, CAO LMB 2019 - 2020 V 210220 def.docx.json</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -812,22 +768,18 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>1</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO 2021 definitief.json, CAO 2019-2021 definitief.docx.json, CAO 2022-2024 defintief_2.json, CAO 2022-2024 (met wijzigingen 6-7-2023).json, CAO 2024 (1-1-2024 tm 30-6-2024)_1.json, CAO_2017_2018_definitief.json, CAO 2019 tot 2021 definitief.docx.json, CAO_2014_2016_2.json, CAO 2022-2024 defintief.json, CAO 2019 2021 definitief.docx.json, CAO_2017_2019_definitief.json, CAO 2021 definitief_1.json, CAO 2024 (1-1-2024 tm 30-6-2024).json, CAO_2017_2019_definitief___met_renvooi___20_7_2018.json, CAO_2014_2016.json, CAO_2017_2019_definitief_1.json, CAO 2024-2026 definitief met alle bijlagen cao.json, CAO.json, CAO 2019-2021 nota van wijziging 8-7-2019.docx.json, Schoonmaak__en_Glazenwassers_cao_stat__en_regl_.json, CAO 2024-2026 definitief met bijlagen.json, CAO 2024 (1-1-2024 tm 30-6-2024)_2.json, CAO_2014_2016_1.json, CAO 2022-2024 defintief_1.json, CAO 2019-2021 -definitief.docx .json, CAO 2022-2024 definitief 1 10 2022.json, schoonmaak_en_glazenwassersbedrijf.json</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -855,19 +807,15 @@
         <v>18</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>1</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Versie 20250114 Teksten CAO PO 2024-2025.json, Def CAO-PO 2023-2024 23012024.json, cao_po_2013_verlengd_2014_140107_handtek.json, 20180719_cao_po_2018_2019_def_getekend.json, 20160711_cao_po_2016_2017_versie_iia.json, 201600701_cao_po_2016_2017_DEFINITIEF_1_juli_2017.json, Def cao po 2021 schoon 6dec2021.json, 20190222_CAO_PO_2018_2019_gewijzigd_feb_2019.json, cao_po_2013_def_versie.json, 20141217_cao_po_2014_2015_tekenversie_REE_EvB_copy.json, 20170427_cao_po_opnieuw_gewijzigd_tbv_AVV_.json, CAO_Appo_en_GOVak_2018_2023.json, cao_po_2013_verlengd_2014_140107_handtek_1.json, CAO-PO 2023-2024.json, 20161230_cao_po_gewijzigd_per_1_jan_2017.json, Def cao 2019-2020 nav aanvullende afspraken .json, Def cao primair onderwijs 2019-2020.json</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -892,22 +840,18 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>337</v>
+        <v>32</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>CAO_2011_aanmelding_TTW_11_2011.pdf</t>
-        </is>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao Bouw en Infra - versie 23 oktober 2023.json, Cao Bouw en Infra 2024 - TTW 12 februari 2024.pdf.json, Cao Bouw en Infra 2024.json, Bouwnijverheid_cao_tekst_docx.json, cao_Bouw_en_Infra_2017_2018_def.json, cao_Bouw_en_Infra_2018_2019_TTW_okt18.json, Cao Bouw en Infra 2023.json, TTW_CAO_2014_aanmelding_juli_2014.json, cao Bouw en Infra 2021-2022_1.json, TTW_cao_Bouw_en_Infra_10_2017.json, Cao Bouw en Infra 2025 - 2027.pdf.json, cao Bouw en Infra 2018-2019 TTW mrt19.pdf .json, TTW_CAO_1_7_2013.json, CAO_2011_aanmelding_TTW_11_2011.json, Bouw CAO 2011 aanmelding TTW 1-2011.json, cao Bouw en Infra 2021-2022.json, cao_Bouw_en_Infra_2018_2019_TTW_dec18.json, CAO BOUW EN INFRA 2023 - INTERACTIEF DEF.json, TTW_cao_Bouw___Infra_integraal.json, CAO_2014_aanmelding_20_3_2014.json, TTW_cao_Bouw_en_Infra_2017_2018_def.json, TTW_CAO_15_10_2013.json, Cao Bouw en Infra 2025 - 2027.json, cao Bouw en Infra 2021-2022_2.json, TTW_CAO_2014_4.json, cao_Bouw_en_Infra_2018_2019_def.json, cao Bouw en Infra 2020.json, CAO BOUW EN INFRA 2023 - INTERACTIEF mei 2023.json, CAO BOUW EN INFRA 2021-2022 INTERACTIEF.json, TTW_CAO_1_5_2013.json, TTW_CAO_definitief_12_november_2012.json, cao_Bouw__Infra_2015_2017_def.json</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
@@ -930,22 +874,18 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>gehandicaptenzorg%20integrale%20tekst.pdf</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Def_tekst_CAO_GHZ_2014_2015_vs20140709.json, CAO2021-2024_Augustus2023def_0_0.json, Tekst CAO GHZ 2021-2024_DEFGEW.json, gehandicaptenzorg integrale tekst.json, Tekst CAO GHZ 2021-2024 schone versie V2.json, CAO GHZ 2019-2021 versie oktober 2020 zonder wijzigingen bijhouden.docx.json, Tekst CAO Gehandicaptenzorg 2025-2026 (ID 161822).json, Tekst CAO GHZ 2021-2024.json, CAO GHZ 2019-2021 definitief zonder wijzigingen 20200107.docx.json, CAO_Gehandicaptenzorg_2017_2019_def.json, CAO Gehandicaptenzorg 2021-2024 tweede ronde.json, CAO_GHZ_2016_def_29_2_2016.json, CAO_Gehandicaptenzorg_2011_2014.json, Definitieve_tekst_CAO_GHZ_2014_2015.json</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
@@ -971,19 +911,15 @@
         <v>18</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>CAO_MB_TTW_juli.pdf</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_MB_arcering___wijz_AOW_LT.json, CAO MB 2021 2024_1.json, HB 5e editie 2024_2.json, CAO_MB_17_19.json, CAO_MB_2017_2019_TTW_GP_nov_2017.json, MenT_Metaalbewerkingsbedr__CAO_tot_.json, HB 5e editie 2024.json, CAO MB 2019 2021SZW TTW Wagweu en art 64.docx.json, CAO_MB_2017_2019_TTW_juli_2017.json, CAO MB 2021 2024b.json, MT_Metaalbew__CAO___handb_.json, CAO_MB_2017_2019_TTW_LL_nov_2018.json, cao_mb_aangepast_n_a_v_bed.json, CAO_MB.json, CAO MB 2019 2021SZW TTW V2 Wagweu.docx.json, CAO MB 2021 2024.json, CAO_MB_TTW_juli.json, HB 5e editie 2024_1.json</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1006,22 +942,18 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>297</v>
+        <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Cao_akkoord_Grond_HV_13_16_def.pdf</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_tekst_2019_basis_1.json, CAO tekst 2021-2022 basis_1.json, CAO_tekst_2017_2020.json, CAO 2010 aanmelding.json, CAO_2012_aanmelding.json, CAO_tekst_2017__2020_inclusief_FNV.json, CAO tekst 2024 basis_1.json, CAO_tekst_2019_basis.json, CAO tekst 2023 basis.json, CAO tekst 2020 basis.docx.json, CAO tekst 2020 basis aangepast.docx.json, CAO tekst 2021-2022 basis.json, CAO tekst 2024 basis.json, CAO_tekst_2014_2017.json</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
@@ -1044,22 +976,18 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>1</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao_2014_2016_aanmelding.json, CAO VVT 2022-2024 verlengde cao ttw2.json, CAO_VVT_2016_2018_def.json, CAO VVT 2022-2023 ttwnov22b.json, CAO VVT 2022-2023 ttwnov22c.json, cao_VVT_tot_1_januari_2015.json, CAO VVT 2025-2026_versie april 2025.json, CAO VVT 2022-2023 ttwnov22.json, cao_2018.json, CAO_VVT_2010_2012_2_.json, gewijzigde_cao_2016_2018.json, CAO VVT 2022-2024 verlengde cao def.json, CAO_VVT_2010_2012_nieuwe_aanmelding_okt_.json, cao 2019-2021 .docx.json, cao_VVT_2018_2019.json, CAO VVT 2022-2024 verlengde cao ttw.json, CAO 2021 aanmelding_1.json, CAO VVT 2022-2023 tussentijdse wijziging.json, cao 2019-2021 tussentijdse wijziging .docx.json, CAO VVT 2022-2023 ttw april23.json, gewijzigde_cao_2016_2018_artikel_1_1_.json, cao 2019-2021 tussentijdse wijziging versie 18 febr.docx.json, CAO VVT 2022-2023 ttwnov.json, CAO 2021 aanmelding.json, gewijzigde_cao_VVT.json, cao 2019-2021 tussentijdse wijziging.docx.json, cao_teksten_2013_2014_aanmelding.json, CAO VVT 2025-2026_TTW 1.json, cao_t_b_v__avv2.json, wijziging_art_1_1__cao_aanmelding.json, cao_VVT.json, CAO_VVT_2012_2013_docx.json, Tekst_aanmelding_CAO_VVT_2013_2014.json, CAO VVT 2022-2023 aanmelding.json, CAO VVT 2022-2023 ttwnov22a.json, gewijzigde_cao_2016_2018_artikel_12_2.json, CAO VVT 2022-2024 verlengde cao ttw_1.json</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1087,19 +1015,15 @@
         <v>16</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Basis_CAO_Metalektro_2011_2013.pdf</t>
-        </is>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_Metalektro_2013_2015_Basis.json, Cao Basis 2022-2024 dd 25-1.json, Basis_CAO_Metalektro_versie_voor_website.json, Basis_CAO_Metalektro_2011_2013_1.json, Basis_CAO_ME_2011_2013__versie_121008.json, Basis_CAO_Metalektro_2011_2013.json, Basis-cao Metalektro aanmelding ttw 21-8-19.docx.json, Cao Basis def. versie 15-7-24 markeringen en statuten.json, Basis 20-22 aanmelding 18-1-22.json, Cao Basis schone versie 9-9-2024 en statuten.json, Cao Basis schone versie 09-12-2024 en statuten.json, Cao Basis def. versie 29-11-22 met statuten ROM en SSF.json, CAO_Metalektro_Basis__met_statuten_.json, Basis-cao Metalektro hertaald - def. versie schoon 23-7-19OB.docx.json, Def. versie aanmelding 15-11 Basis-cao Metalektro 20-22.json, Basis_CAO_Metalektro_met_statutenfondsen.json</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
@@ -1125,19 +1049,15 @@
         <v>25</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>NBBUCAO_wijzigingen_geaccepteerd_SZW.pdf</t>
-        </is>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>definitieve_cao_tekst.json, NBBU cao voor uitzendkrachten - 30122019 - DEFINITIEF.doc.json, Cao_uzk_1_7_2016.json, NBBU_CAO_Uitzendkrachten-NL 2023 def..json, NBBU_CAO_uitzendkrachten_2017.json, NBBU-cao voor uitzendkrachten per 1 juni 2021 def ondertekend.json, NBBU_CAO_Uitzendkrachten-NL 2024.def.json, NBBU cao tussentijdse wijzigingen januari 2023.json, NBBU cao per 1-1-2022 defintief wijziging accept.json, NBBU_Uitzendkrachten_1060.json, NBBU Cao UK 2009-2013 SZW niet gemarkeerd.json, NBBU_CAO_Uitzendkrachten_2016_V3.json, 2180679_NBBU_CAO_Uitzendkrachten_2018_OTFp.json, NBBU_CAO_Uitzendkrachten_2015_per_1_juli_DEF.json, NBBU_CAO_Uitzendkrachten_2015-2019_versie 2019 NL OTF.pdf .json, NBBUCAO_wijzigingen_geaccepteerd_SZW.json, Cao uitzendkrachten LBV onwerkbaar weer dec 2021 wijzigingen geaccpteerd.json, c1032_f9599_fp2852_2011654_NBBU_Uitzend_versie_2.json, NBBU_CAO_Uitzendkrachten 2015-2019_versie 2019 NL OTF.docx.json, NBBU cao tussentijdse wijzigingen def.json, NBBU_CAO_Uitzendkrachten-NL_2021.json, NBBU_CAO_Uitzendkrachten_2015.json, NBBU_CAO_Uitzendkrachten-NL_JUN 2023_v1.json, NBBU_CAO_Uitzendkrachten_2018.json, NBBU_CAO_Uitzendkrachten_2015_2019_def_.json</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
@@ -1165,19 +1085,11 @@
       <c r="E19" t="n">
         <v>0</v>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
         <v>0</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
@@ -1201,19 +1113,15 @@
         <v>9</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>VOR_CAO_web_2020_03%20beveiligd.pdf</t>
-        </is>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO PDF DEF.json, CAO VO 2023-2024 (def 14.12.23).json, CAO VO 2022 2023 spreads def voor aanmelding SZW (nov 22).json, CAO_VO_2014__2015.json, CAO VO 2024 2025 zonder handtekeningen en namen (tbv aanmelding) PDF.json, CAO_VO_2018_2019_voor_aanmelding_SZW.json, CAO_VO_2016_2017_ondertekend_DEFPDF.json, VOR_CAO_web_2020_03 beveiligd.json, CAO_VO_2011_2012_def.json</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
@@ -1239,19 +1147,15 @@
         <v>11</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Tekst_CAO_GGZ_2011_2013_juli_2012.pdf</t>
-        </is>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
         <v>0</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao ggz tekst 05-02-2024.json, GGZ cao met wijziging salarisschaal.json, Word_werkbestand_CAO_GGZ_2017_2019.json, Tekst_CAO_GGZ_2011_2013_juli_2012.json, GGZ_CAOgids_gewijzigd3dec2015.json, CAO_GGZ_2015_2017.json, tekst CAO GGZ 2021-2024.json, cao 2019-2021 min SZW.json, Werkversie_CAO_GGZ_2011.json, GGZ1504_01_binnenwerkCAOgids.json, Wijzigingen CAO GGZ 2019-2021 excl bijlage VI - 31 december 2020 definitief.docx.json</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -1277,19 +1181,15 @@
         <v>7</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>CAOP_CAO_boek_A5_def_24_8_9uur.pdf</t>
-        </is>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAOP_CAO_boek_A5_def_24_8_9uur.json, 130214_gehelecao1_versienatosw_4_AP.json, Tekst Cao SW 2020.json, Web-versie-SW-CAO-boekje-2021-2025.json, 20191208_Cao tekst 2019.docx.json, 20211015__Tekst Cao SW 2021-2025_def.json, cao sociale werkvoorziening.json</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
@@ -1315,19 +1215,15 @@
         <v>18</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>CAO_TI_deel.pdf</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
         <v>0</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>HB 5e editie 2024_2.json, CAO_TI_arcering___wijz_AOW_LT.json, CAO_TI_deel.json, CAO TI 2019 2021 TTW V2 Wagweu.docx.json, CAO TI 2021 2024.json, M_en_T_Technisch_Installatiebedrijf_cao_en_handb_.json, CAO_TI_2017_2019_TTW_LL_nov_2018.json, CAO TI 2021 2024_1.json, CAO_TI_2017_2019_TTW_juli_2017.json, HB 5e editie 2024.json, CAO_TI_2011_2013_incl_wijz_4c_aangepast_n_a_v_bed.json, MenT_Technisch_Install_tot_cao_2297.json, c2255_f14208_fp3241_CAO_TI_17_19_arcering.json, CAO TI 2019 2021 TTW Wagweu en art 64 .docx.json, CAO TI 2021 2024b.json, CAO_TI_2017_2019_TTW_GP_nov_2017.json, CAO_TI_TTW_juli.json, HB 5e editie 2024_1.json</t>
         </is>
       </c>
       <c r="I23" t="inlineStr"/>
@@ -1350,22 +1246,18 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
         <v>1</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao_Fashion_en_Sport_Inretail.json, 230418 cao Retail Non-Food def.json, 171115_Cao_F_S__L_2016_2018_definitief_hvb_2.json, 170118_Cao_F_S__L_2016_2018_hvb.json, cao_Mode__Sport_1_7_2010_tot_1_7_2012.json, 220629 cao Retail Non-Food def.json, 220208 cao Retail Non-Food schone versie.json, 221214 cao Retail Non-Food schone versie.json, 230630 cao Retail Non-Food def.json, 150824_Cao_Fashion__Sport_en_Lifestyle.json, 211130 Cao Retail Non-Food 1-1-2022 def..json, 210805 Cao Retail Non-Food 1-7-21 def.json, Cao_Fashion_en_Sport_Inretail_21_8_2013.json, cao_Mode__Sport_1_7_2010_tot_1_7_2012_22_8_2011.json, 190730 cao Retail Non-Food per 1 juli 2019 definitief.docx.json, 241218 Cao Retail Non-Food jan 2025 definitief.json, 190730 cao Retail Non-Food per 1 juli 2019.docx.json, 250617 Cao Retail Non-Food juli 2025 def.json, 150824_Cao_Fashion__Sport___Lifestyle_hvb.json, 240206 cao Retail Non-Food def..json, 170313_Cao_F_S__L_2016_2018_incl_Wonen_def_hvb.json, 201207 Cao Retail Non-Food 1-1-21 definitief.docx.json, 180921_cao_Retail_Non_Food_definitief_hvb.json, 191227 cao Retail Non-Food per 1 januari 2020 definitief.docx.json, 170214_Cao_F_S__L_2016_2018_hvb.json, 210811 Cao Retail Non-Food 1-7-21 def.json, 240508 Cao Retail Non-Food definitief.json, 151020_Cao_Fashion__Sport___Lifestyle_hvb.json, 170630_Cao_F_S__L_2016_2018_definitief_hvb.json, 210128 Cao Retail Non-Food 1-1-21 definitief.docx.json, 190128_cao_Retail_Non_Food_definitief_hvb_bg.json, 240625 Cao Retail Non-Food definitief.json, 171115_Cao_F_S__L_2016_2018_definitief_hvb_1.json, 160715_Cao_F__S___L_2016_2018_gewijzigd_hvb.json, 171115_Cao_F_S__L_2016_2018_definitief_hvb.json, 161031_Cao_F_S__L_2016_2018_hvb.json</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -1393,19 +1285,15 @@
         <v>16</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>2025-07-01 CAO MVT 2025 - 2027 - incl HFI DEF.json, Concept cao MVT - incl HFI DEF.json, CAO MvT 2020-2021 DEFversie 19 januari 2021.docx.json, CAO_MvT_2014_2018_11_september.json, CAO_tekst_2011_2012_compleet_versie_2_augustus.json, Cao MVT - incl HFI 8 juni 2022.json, CAO_tekst_2011_2012_compleet_versie_19_juli.json, Cao MVT - incl HFI 31 januari 2024.json, CAO MvT 2020-2021 versie 23 dec 2020.docx.json, CAO MvT 2018-2020 DEF 2 oktober 2019.docx.json, Cao MVT - zonder HFI DEF 6 feb 2023.json, 2024-04 Cao MVT 2023 - 2025 - incl HFI vs 2.json, CAO MvT 2018-2020 DEF 29 mei19.docx .json, CAO_tekst_2012_2014_definitief.json, CAO_tekst_2011_2012_compleet_versie_28_juli.json, CAO_MvT_2014_2018_29_november_2016.json</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -1431,19 +1319,15 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao_umc_2013___2015_officiele_tekst.json, Officiele_versie_NL_Cao_UMC_2011_2013.json, SZW_15_14272_Cao_umc_2015_2017.json, Cao umc 2018-2020 def versie maart 2019.pdf .json, 19.9945 Umcs Cao umc 2018-2020 per 1-1-2020.json, 15_11628_Cao_umc_2015_2017_DEF.json, Cao_umc_2015_2017_versie_8_2017.json, Cao UMC wijzigingen per januari 2023.json, Cao umc 2022 2023 pdf.json, NFU-24.01131 CAO NL v08 def.json</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
@@ -1469,19 +1353,15 @@
         <v>21</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Integrale Cao Kinderopvang 2021-2022.json, CAO_Kinderopvang_difi.json, CAOKINDEROPVANG 1011 (ttw160311).json, Integrale cao Kinderopvang 2020 - 2021 - gewijzigd.json, Integrale Cao Kinderopvang 2025-2026.json, CAO_Kinderopvang_2012_2014_basistekst060214.json, CAO_Kinderopvang.json, Integrale Cao Kinderopvang 2021-2022 - 280721.json, CAO_Kinderopvang_2012_2014_aanmeld150813.json, Integrale Cao Kinderopvang 2024.json, CAO_Kinderopvang_2012_2014_basistekst101114.json, CAO_Kinderopvang_2012_2014_def.json, CAO_Kinderopvang_2018_2019.json, CAO_Kinderopvang_2016_2017.json, Integrale Cao Kinderopvang 2024 16-07-2024.json, Integrale gewijzigde Cao Kinderopvang 2023-2024.json, Integrale Cao Kinderopvang 2023-2024.json, Integrale gewijzigde cao Kinderopvang 2020-2021 (schone versie).docx.json, Integrale Cao Kinderopvang 2023-2024 (21-12-2023).json, Integrale cao Kinderopvang 2020 - 2021.json, Integrale Cao Kinderopvang 2024 20-12-2024.json</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -1504,22 +1384,18 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="n">
         <v>1</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao Sociaal Werk 2021-2023_definitief231122.json, Cao Sociaal Werk 2021 2023_280422definitief.json, CAO W&amp;MD 2008-2012 compleet 10_3.json, caosociaalwerk20172019_def191017_inclfuboek.json, welzijn_en_maatschappelijke__tekst.json, CAO_W_MD_2008_2012_AVV_zichtb_renv_17_05_2011.json, CAOWMD20082011aanmelding2012.json, CAOWMD20142016_definitief_301214_.json, Cao Sociaal Werk 2023-2025(ttw031224opttw010724)definitief.json, CAOSOCIAALWERK1921definitief_030120.json, CAOWMD20142016_ttw220615_definitiefgewijzigd.json, CAO_WMD_2008_2011_aanmeldversie.json, Cao Sociaal Werk 2023-2025(gewijzigdper091023).json, Cao Sociaal Werk 2023-2025(gewijzigdper091023)def.json, CAOSOCIAALWERK1921gewijzigdivmpsz_290720_def.json, CAOWMD_VERLENGING_2012_ttw_ivm_avv.json, CAOWMD_2012_TTW_ivm_AOW_datum.json, Cao Sociaal Werk 2023-2025(metcorrectie150224).json, CAOWMD_aanmelding_VERLENGING_2012_ttw_ivm_avv.json, Cao Sociaal Werk 2023-2025(definitief_tussentijdsgewijzigdper010724).json, Cao Sociaal Werk 2023-2025(definitief240723)def.json, welzijn_maatschappelijk_dienstverlenning.json, CAOSOCIAALWERK1719_070218__ttw_corr_avv_def.json, CAOSOCIAALWERK1719_completetekst_def_030419schoon.docx .json, ttwnov15_CAOWMD1416_def_exb2b15_wijzws_151215_def.json</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -1547,19 +1423,15 @@
         <v>13</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
         <v>0</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_2011_2014_def.json, CAO Nederlandse Universiteiten 31 december 2019 tm 31 december 2020.json, Cao Nederlandse Universiteiten 1 juli 2017 - 31 december 2019.pdf .json, CAO NU 1 juli 2024 - 30 juni 2025 eerste webversie.json, Collectieve Arbeids Overeenkomst 1 januari - 31 december 2020 webversie CAO NU.p.json, 16066-12 VSNU-CAO Nederlandse Universiteiten 2020.json, CAO NU 20222-2023 definitieve tekst schoon.json, VSNU-CAO Nederlandse Universiteiten 2021-2022-NL definitieve versie 10-11-21.json, Ned_Universiteiten_1536.json, CAONU_1_januari_2015___1_juli_2016.json, CAONU_1_januari_2015___1_juli_2016_1.json, CAO_NU_2_juli_2016___30_juni_2017.json, CAO NU 2023-2024 definitief.json</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -1585,19 +1457,15 @@
         <v>15</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
       <c r="G30" t="n">
         <v>1</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO MBO 2022-2023.json, CAO_MBO_2016_2017____Nieuwe_versie_25042018.json, CAO_MBO_2018_2020_in_Word.json, CAO MBO 2023-2024.json, Beroepsonderwijs_en_Volwasseneneducatie_BVE_1022.json, CAO_MBO_2016_2017_definitief.json, cao_mbo_2014_singlepage_def.json, CAO MBO 2021-2022 - wijzigingen doorgevoerd 17122021.json, CAO MBO 2021 - wijzigingen geaccepteerd 09072021.json, CAO_MBO_2016_2017___Nieuwe_versie.json, CAO MBO 2024.json, CAO MBO 2020-2021 - wijzigingen geaccepteerd 29062020 def.json, CAO MBO 2018-2020 - wijzigingen geaccepteerd 712020.json, CAO_MBO_2014_2015_in_Word___nieuwe_versie.json</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -1625,19 +1493,15 @@
         <v>27</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F31" t="inlineStr"/>
       <c r="G31" t="n">
         <v>1</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>01_CAO_BAKKERSBEDRIJF_1_MAART_2012.json, cao Bakkersbedrijf, definitief versie 03062024 (5).docx.json, cao tekst .json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016.json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016_1.json, 01_CAO_BAKKERSBEDRIJF_1_AUGUSTUS_2011_1.json, Cao Bakkersbedrijf 1 juni 2021 - 1 juni 2023 definitief 08072022.json, 01 CAO BAKKERSBEDRIJF 1 APRIL 2019.docx .json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2014.json, Cao Bakkersbedrijf 1 juni 2021 - 1 juni 2023 definitief 12082022.json, cao Bakkersbedrijf definitief versie 15082024.json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2015.json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2015_1.json, CAO BAKKERSBEDRIJF 1 AUGUSTUS 2020 incl Bijlagen.docx.json, Cao Bakkersbedrijf 1 juni 2021 - 1 juni 2023 definitief 25072022.json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016_2.json, BAKKERSBEDRIJF_1_AUGUSTUS_2011_incl_bijlagen.json, 01_CAO_BAKKERSBEDRIJF_1_AUGUSTUS_2011.json, CAO BAKKERSBEDRIJF 1 AUGUSTUS 2020 incl Bijlagen_1.json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016___def_.json, 01_CAO_BAKKERSBEDRIJF_1_MAART_2012___definitief.json, BAKKERSBEDRIJF_cao_tekst_en_bijlagen.json, CAO BAKKERSBEDRIJF 1 AUGUSTUS 2020 incl Bijlagen.json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2014_1.json, CAO tekst.json, cao Bakkersbedrijf, definitief versie 26072024.json</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -1665,19 +1529,15 @@
         <v>11</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F32" t="inlineStr"/>
       <c r="G32" t="n">
         <v>0</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao_hbo_2014_2016.json, 085_021_CAO_2018_2020_PAGINA_S.json, 085_021_CAO_2020_DEFDEF.json, CAO_2024_2025def.json, cao20162017_definitief.json, CAO_DEF_2017_2018___.json, caohbo_2012_2013_definitief.json, CAO_2021-2022_DEF.json, cao_hbo_2014_2016_1.json, 085_021_CAO_2022_2023DEF.json, CAOHBO_2023_2024.json</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
@@ -1703,19 +1563,15 @@
         <v>25</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F33" t="inlineStr"/>
       <c r="G33" t="n">
         <v>0</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao 1 juli 2018 - 30 juni 2023 definitief mei 2020.docx.json, cao_1_juli_2012___30_september_2013_definitief.json, Cao Particuliere beveiliging Versie 3- april 2021.json, CAO PB 18 dec 2024- 27 dec 2026.json, cao_2014_2015_definitief.json, Cao Particuliere beveiliging Versie 4- mei 2021.json, Cao Particuliere beveiliging Versie 6 - mei 2022 met zichtbare wijzigingen.json, CAO PB 18 dec 2024- 27 dec 2026 zonder zichtbare wijzigingen.json, cao_2011_definitief.json, Cao Particuliere Beveiliging versie 7 juni 2023 ZONDER zichtbare wijzigingen_1.json, cao_2014_2015_definitief_1.json, Cao Particuliere beveiliging Versie 5- januari 2022.json, Cao Particuliere Beveiliging 2023-2024 versie 2- augustus 2023 ZONDER zichtbare wijzigingen.json, Cao Particuliere Beveiliging versie 7 juni 2023 ZONDER zichtbare wijzigingen.json, cao 1 juli 2018 - 30 juni 2023 definitief.docx _1.json, cao_2012_definitief.json, definitief.json, cao_definitief__september_2017.json, cao_1_juli_2012___30_september_2013_definitief_1.json, cao 1 juli 2018 - 30 juni 2023 definitief versie 2 met aanvullende wijziging voo.json, cao_2014_2015_definitief_part_beveilig.json, cao_definitief_versie_2.json, cao 1 juli 2018 - 30 juni 2023 definitief april 2020.docx.json, cao 1 juli 2018 - 30 juni 2023 definitief.docx .json, cao 1 juli 2018 - 30 juni 2023 definitief versie 2 met wijzigingen voor aanmeldi.json</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
@@ -1738,22 +1594,18 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao_Glastuinbouw_incl_ttw_1_1_2018_integrale_tekst.json, Glastuinbouw aangepast II.json, CAO Glastuinbouw aangepast.json, Integrale tekst cao Glastuinbouw 1 juli 2025 tm 31 maart 2026 (2506-1911).json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022 inclusief derde TTW..json, Glastuinbouw 1 juli 2018 tot en met 31december 2019 incl functiehandboek.docx.json, cao Glastuinbouw 1 juli 2018 tot en met 31december 2019 inclusief 2e TTW en incl.json, Integrale tekst Cao Glastuinbouw 1 januari 2024 tot en met 31 maart 2025 incl. 1e TTW per 1 januari 2024 (2406-1334).json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022 inclusief eerste TTW.json, cao Glastuinbouw 1 juli 2018 tot en met 31december 2019 inclusief functiehandboe.json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022 inclusief tweede TTW.json, cao_Glastuinbouw.json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022.json, Glastuinbouw__TTW_en_functiehandboek.json, cao_Glastuinbouw_2012_2014_registratie_SZW__2.json, Cao Glastuinbouw 1 januari 2023 tot en met 31 december 2023.json, cao_Glastuinbouw_2e_ttw_14_mei_2018_integr.json, Integrale tekst Cao Glastuinbouw 1 april 2025 tm 30 juni 2025 (2506-1846).json, cao_Glastuinbouw_2015____2018.json, Integrale tekst Cao Glastuinbouw 1 januari 2024 tot en met 31 maart 2025 (2404-2053).json</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -1781,19 +1633,11 @@
       <c r="E35" t="n">
         <v>1</v>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F35" t="inlineStr"/>
       <c r="G35" t="n">
         <v>1</v>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H35" t="inlineStr"/>
       <c r="I35" t="n">
         <v>1</v>
       </c>
@@ -1819,19 +1663,15 @@
         <v>17</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
       <c r="G36" t="n">
         <v>1</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO Technische Groothandel 2023-2025_Versie 2024-04-11.json, CAO TG 2023-2025_Tussentijdse AVV-aanpassing_Versie 2025-02-14.json, CAO TG 2023-2025_Tussentijdse aanpassing.json, CAOTechnGroTussentijdseWijz1jan2013Art18lid2.json, CAO TG 2023-2025_Versie 2024-12-11.json, CAO TG 2023-2025_Versie 2025-01-31.json, CAO_2011_2012_Formele_tekst_CAO.json, CAO Technische Groothandel 2019-2022.json, CAOTG20162018Aanpassingen20170807.json, 730 - CAO TG 2019-2022_Tussentijdse wijziging_2022-05-09.json, CAO Technische Groothandel 2023-2025_Versie 2024-04-04.json, CAO Technische Groothandel 2022-2023_Versie 2023-03-27.docx.json, CAO Technische Groothandel 2023-2025_Versie 2024-05-13.json, CAOTechnischeGroothandel20162018.json, CAO Technische Groothandel 2022-2023_Versie 2023-03-07.json, 730 - CAO TG 2019-2022_Tussentijdse wijziging_2022-06-22.json</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -1856,22 +1696,18 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F37" t="inlineStr"/>
       <c r="G37" t="n">
         <v>0</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>GIL_2010_2012_cao_tekst_en_handboek.json, CAOGIL_2015___2016_def_schoon.json, CAOGIL_juni_2016.json, CAOGIL_2012_2013_def_schoon.json</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
@@ -1897,19 +1733,15 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
       <c r="G38" t="n">
         <v>1</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAOVDB_2015_16__tekst_def_geschoond.json, Drogisterijbranche__2010_12_definitieve_tekst.json, CAO_2017_2018_tekst_aangepast_geschoond_def.json, TTW 2025 Cao boekje VDF-tekst geschoond.json, CAO_2017_2018_tekst_def_geschoond_per_april_2018.json, Cao boekje VDF-tekst geschoond.json, CAO_2017_2018_tekst_aangepast_geschoond.json, Cao boekje Drogisterijbranche VDF- schoon.json, Cao boekje VDF-tekst geschoond voor TW.json</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -1937,19 +1769,15 @@
         <v>29</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F39" t="inlineStr"/>
       <c r="G39" t="n">
         <v>1</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao open teelten 4e ttw per 1 juli 2022 - integrale tekst.json, CAO_OT_2017_2020.json, Cao open teelten per 1 maart 2021 tot en met 28 februari 2023 1e TTW integraal.d.json, Cao open teelten per 1 maart 2021 tot en met 28 februari 2023 1e TTW integraal.d_1.json, cao_open_teelten_inc_ttw.json, cao open teelten per 1 juli 2020.docx.json, 1811_2255_2e_tww_cao_open_teelten_per_1_1_2019a.json, Integrale tekst cao Open Teelten 1 maart 2023 tm 30 juni 2024 incl. 2e TTW per 1 juli 2023 (2306-1279).json, Open_Teelten_en_functiehandboek.json, cao_open_teelten_inclusief_ttw_1_dec_2016.json, cao_open_teelten_2016_2017.json, Open Teelten integrale tekst incl ttw.json, Cao Open Teelten 3e TTW per 1 juli 2019 definitief.docx.json, cao_Open_Teelten_ttw_per_1_juli_2018.json, Integrale tekst cao Open Teelten looptijd 1 juli 2024 tm 30 juni 2025 incl. TTW per 1 januari 2025 (2501-0136).json, Cao Open Teelten 4e TTW per 1 januari 2020.docx.json, Integrale tekst cao Open Teelten looptijd 1 juli 2025 tm 30 juni 2027 (2506-2013).json, cao open teelten 3e ttw 1 januari 2022 integraal _.json, 2104-1910 cao Open Teelten 2021-2023.json, Cao open teelten per 1 maart 2021 tot en met 28 februari 2023 2e TTW integraal.d.json, CAO_Open_Teelten__1_juli_2014_tm_30_juni_2015.json, Integrale tekst cao Open Teelten looptijd 1 juli 2024 tm 30 juni 2025 (2410-1079).json, Integrale tekst cao Open Teelten 1 maart 2023 tm 30 juni 2024 - 2303-0178 v0.1.json, Integrale tekst cao Open Teelten 1 maart 2023 tm 30 juni 2024 incl. 3e TTW per 1 januari 2024 (2312-1367).json, cao Open Teelten met 5e ttw integraal per 1 november 2022 - 2210-1226 v0.1.json, cao_Open_Teelten_1_7_2012_tm_30_6_2014.json, Integrale tekst cao Open Teelten 1 maart 2023 tm 30 juni 2024 incl. 1e TTW per 1 maart 2023.json, Cao_Open_Teelten_integrale_tekst_ttw.json</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -1974,22 +1802,18 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F40" t="inlineStr"/>
       <c r="G40" t="n">
         <v>0</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Bijlage 11 _ cao jz 21-23_B11_ Functieboek aanmeld.json, cao_tekst_JZ_2015_2016_def_met_bijlagen_1_tm_10.json, CAO_Jeugdzorg_28_04_11verlengd_schoon.json, cao_JZ_2015__2017_tm_B11.json, cao_tekst_JZ_2017_2019__23_8_17.json, CAO_JZ_2011_14_aanmelding_26_4_2013.json, CAO_JZ_2011_13_aanmelding_7_3_2013.json, Jeugdzorg_Cao_2011_2013_def020712.json, CAO Jeugdzorg versie 101215 versie 4.json, CAO_Jeugdzorg_17_02_12wijz_art12_3_schoon.json, Jeugdzorg_Cao_2011_2013_def.json, cao jeugdzorg aanmeldversie december 2024 compleet jk.json, Aanmeldversie cao Jeugdzorg 19-20.docx.json, cao_tekst_JZ_2017_2019_def_tekst_schoon_5_7_17.json, Cao Jeugdzorg 2024- 2025 aanmeldversie juli 2024 schoon.json, Cao Jeugdzorg 2024- 2025 aanmeldversie.json, cao_jeugdzorg_2014_2016_Aanmeldversie_compleet.json, cao_tekst_JZ_2017_2019_versie_TTW_18_5_2018.json, CAO Jeugdzorg 10-02-11schoon.json, cao_jeugdzorg_2014_2015_def.json</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
@@ -2015,19 +1839,15 @@
         <v>12</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F41" t="inlineStr"/>
       <c r="G41" t="n">
         <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Woondiensten_cao_en_handboek.json, CAO-Woondiensten 2022-2023 versie 01-09-2022.json, Woondiensten_2011_caotekst_en_handboek.json, CAO_Woondiensten_2014_2016_word.json, CAO Woondiensten 2021.json, cao woondiensten en handboek.json, CAO_Woondiensten_2013_tm_juni_definitieve_tekst.json, CAO_Woondiensten_inclusief_Handboek.json, Overzicht renvooi CAO Woondiensten 2019-2020.docx.json, cao tekst woondiensten.json, CAO Woondiensten 2024-2025 def (25 juni 2024).json, CAO_Woondiensten_2017_2018.json</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
@@ -2053,19 +1873,15 @@
         <v>30</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
       <c r="G42" t="n">
         <v>0</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>recreatie_definitief_1.json, cao_definitief_3_0_nav_opmerkingen_szw_avv.json, cao_definitief_1.json, Cao Recreatie, definitief versie 14042025.json, cao_definitief_5_0.json, cao_definitief_2_0_nav_opm_drukproef.json, cao 1 januari 2022 - 31 december 2023 definitief 21042022.json, recreatie_definitief.json, cao 1 januari 2019 - 31 december 2020, definitief aangepast.docx .json, cao_definitief_3_0.json, cao-recreatie 2024 - 2025 herschreven versie opgemaakt definitief 25062024.json, cao 1 januari 2019 - 31 december 2020, definitief aangepast versie augustus 2019.json, cao_definitief.json, Cao Recreatie, definitief versie 29042025.json, cao-recreatie 2024 - 2025 herschreven versie opgemaakt definitief 21052024.json, cao 1 januari 2019 - 31 december 2020, definitief.docx .json, cao_2010_2012_definitieve_versie_april_2012.json, cao_recreatie_2012_2013_definitieve_versie.json, cao_definitief_4_0.json, cao 1 januari 2022 - 31 december 2023 definitief 28122022.json, cao 1 januari 2022 - 31 december 2023 definitief 23012023.json, cao 1 januari 2022 - 31 december 2023 definitief 12052022.json, cao_Recreatie_2013_2014_def__versie.json, cao-recreatie 2024 - 2025 definitief 25062024 - versie 28112024 ivm WML per 1 januari 2025.json, Def_tekst_Ttw_cao_R.json, cao_definitief_2_0.json, cao 1 januari 2022 - 31 december 2023 definitief 01042022.json, cao 1 januari 2021 - 31 december 2021, defintief.json, cao 1 januari 2019 - 31 december 2020, definitief aangepast versie 1 juli.docx.json, handboek_compleet.json</t>
         </is>
       </c>
       <c r="I42" t="inlineStr"/>
@@ -2091,19 +1907,15 @@
         <v>28</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F43" t="inlineStr"/>
       <c r="G43" t="n">
         <v>1</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_tekst_Taxi_cao_nr__679.json, CAO Zorgvervoer en Taxi 2022, definitief incl inhoudsopgave februari 2022.json, CAO Zorgvervoer en Taxi 2023-2024 180424 def. tekst.json, cao tekst Taxivervoer.json, CAO Zorgvervoer en Taxi 2022, definitief incl inhoudsopgave september2022.json, TTW CAO Taxivervoer 2019 2020 v260420 DEF.docx.json, CAO Taxivervoer 2021 NET.docx.json, Taxivervoer_1_juli_2016_tot_en_met_30_juni_2017.json, CAO Zorgvervoer en Taxi 2022, definitief.json, CAO_Taxi_Vervoer_2016.json, CAO Zorgvervoer en Taxi 2024-2025 definitieve tekst 100125.json, TTW CAO Taxivervoer 2019 2020 v050320 DEF NET.docx.json, CAO_Taxivervoer_2019_2020_NET_1.json, Taxivervoer_2009_2013_integrale_cao.json, TTW CAO Taxivervoer 2019 2020 v220620 DEF.docx.json, CAO_Taxivervoer_2017_2018.json, cao_taxivervoer_2016___2017_1.json, TTW_CAO_Taxivervoer_2017_2018.json, CAO_tekst_Taxivervoer_2014_2015_v5_nette_versie.json, TTW_CAO_Taxivervoer_2019_2020.json, cao_taxivervoer_2016___2017.json, CAO Zorgvervoer en Taxi 2024-2025 definitieve tekst 221124.json, CAO Zorgvervoer en Taxi 2023 06012023.json, CAO_tekst_Taxivervoer_2014_2015.json, CAO Zorgvervoer en Taxi 2023-2024 170524 definitieve tekst.json, CAO Taxivervoer 2021 NET v231120.docx.json, CAO_Taxivervoer_2019_2020_NET.json</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -2131,19 +1943,15 @@
         <v>23</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F44" t="inlineStr"/>
       <c r="G44" t="n">
         <v>0</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>verlengde_cao_LEO__inclusief_ttw_1_maart_2016.json, Eindtekst cao Groen, Grond en Infrastructuur 1 januari 2024 - 31 december 2024 incl. 1e ttw per 1 januari 2024.json, LEO_2017_2019.json, cao_leo_2_januari_2012___30_juni_2013_incl_ttw.json, Eindtekst cao Groen, Grond en Infrastructuur 1 januari 2025 - 30 september 2026 incl. 1e ttw per 1 januari 2025.json, 2012-1466 cao GGI incl.ttw def.docx.json, integrale cao LEO 1 juli 2020 tot en met 31 december 2020 incl TTW per 1-11-2020.json, cao GGI 1 januari 2022 tm 31 december 2023 integraal.json, 2212-0813 defintieve tekst cao GGI met ttw per 1 januari 2023.json, cao GGI incl tref woorden def versie 2.docx.json, cao_leo_1_juli_2013_tm_30_juni_2014__20130716N_.json, Eindtekst cao Groen, Grond en Infrastructuur 1 januari 2025 - 30 september 2026.json, Integrale tekst cao Groen, Grond en Infrastructuur 1 januari 2024 - 31 december 2024.json, 2103-1098 cao GGI met 2e TTW.json, cao_LEO_1mei_2016_tot_en_met_30_juni_2017.json, cao_leo_1_juli_2014___31_december_2015tekst_def.json, 2104-0817 integrale cao GGI met 3e ttw.json, 2212-0813b defintieve tekst cao GGI met 1e ttw per 1 januari 2023.json, integrale cao LEO 1 juli 2020 tot en met 31 december 2020 def.docx.json, CAO_LEO__1_april_2010_tot_en_met_1_januari_2012.json, integrale_cao_Leo_2017_2019_a.json, cao_LEO__ttw_per_1_juli_2018.json, cao_leo.json</t>
         </is>
       </c>
       <c r="I44" t="inlineStr"/>
@@ -2171,19 +1979,11 @@
       <c r="E45" t="n">
         <v>0</v>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F45" t="inlineStr"/>
       <c r="G45" t="n">
         <v>0</v>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr">
         <is>
@@ -2207,19 +2007,15 @@
         <v>12</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F46" t="inlineStr"/>
       <c r="G46" t="n">
         <v>1</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao_Apotheken_2012_2013_plat.json, Apotheken cao 2019-2021.docx.json, Apotheken 2019-2021 na ttw.json, Apotheken 50.json, Cao Apotheken 2024-2027 na ttw volledig met bijlagen 07-07-2025.json, 20170222_Def_versie_Cao_Apotheken_2016_2017_schoon.json, 20192401 Concepttekst Cao Apotheken 2017-2019 schoon.docx .json, CAO Apotheken 2021-2024 volledig met bijlagen 02-06-2022 def.json, CAO Apotheken 2021-2024 na ttw volledig met bijlagen 05-07-2022.json, Apotheken_2010_2011_cao_tekst.json, CAO Apotheken 2021-2024 na ttw ivm verhoging.json</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -2247,19 +2043,15 @@
         <v>24</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="n">
         <v>0</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao_2011_2013_ttw4_tijdelijke_maatr_aanmelding.json, cao_Schilders_2013_2014_ttw_1_aanmelding.json, CAO SAVG 2021 2025 (TTW maart 2024) schone versie.json, cao_2011_2013_ttw_1__aanm_.json, CAO SAVG 2021-2025 (jan 2024) (Schilders, Afwerkings-, Vastgoedonderhoud- en Glaszetbedrijf).json, cao_2011_2013_ttw2_functieloon_aanmelding.json, CAO SAG 2016 2021 ttw april 2021.json, CAO SAG 2016 2021 ttw april 2021.2.json, CAO SAG 2016 2021 ttw januari 2021.json, CAO SAG 2016 2021 15 juli 2019.docx.json, CAO SAG 2016 2021 ttw 3 april 2020.json, CAO SAG 2016 2021 ttw 10 oktober 2018.pdf .json, CAO SAVG 2021 2025 TTW 27 oktober 2022.json, CAO_SAG_2016_2019_versie_22_12_2016.json, cao_2011_2013_ttw3_functieloon_aanmelding.json, CAO_SAG_2016_2019__16_september_2016_.json, CAO SAVG 2025.json, CAO SAVG 2021 2025 oktober 2021.json, CAO SAVG 2021 2025 TTW februari 2023.json, cao_Schilders_2013_2014.json, CAO SAVG 2021 2025 december 2021.json, cao_2011_2013.json, CAO_SAG_2016_2019__ttw_29_september_2016_.json, CAO_SAG_2016_2019_ttw_20_november_2017.json</t>
         </is>
       </c>
       <c r="I47" t="inlineStr"/>
@@ -2285,19 +2077,15 @@
         <v>18</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F48" t="inlineStr"/>
       <c r="G48" t="n">
         <v>1</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao_HAZ_2014_2015_zwart_versie_II.json, cao_HAZ_2014_2015_zwart.json, CAO_Huisartsenzorg_2013_W.json, Cao-HZ 2019-2020 na ttw.docx.json, Huisartsenzorg__cao_tekst__cao_721.json, 12_01_25_CAO_tekst_definitief.json, Cao HAZ 2024-2025 met Handleiding FWHZ 3-6-2024.json, wijz_III_cao_HAZ_2015_2017_incl_FWHZ_anmtkst_zwart.json, Huisartsenzorg cao 2019-2020.json, Cao-huisartsenzorg-2022-2023-incl-Handleiding.json, Cao Huisartsenzorg 2021.json, 110919_CAO_Huisartsenzorg_2011_2012_definitief.json, Cao-HZ 2019-2020 na ttw2.docx.json, Cao-huisartsenzorg-2022-2023-incl-Handleiding.avv.json, Cao Huisartsenzorg 2022-2023 na TTW ivm herziening loonsverhoging per 1-1-2023.p.json, huisartsenzorg_2017_2019_TTW.json, Cao_huisartsenzorg_30122015.json</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -2325,19 +2113,15 @@
         <v>18</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F49" t="inlineStr"/>
       <c r="G49" t="n">
         <v>1</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Grafimedia cao 2020-2021 - def 230221.docx.json, Grafimedia cao 2020-2021 juni 2021.json, Grafimedia cao 2022-2024 2 maart 2022.json, Grafimedia def..json, Grafimedia_cao_na_ttw_2015_2018_18122015_def.json, DEF Grafimedia cao 2024-2025 schone versie TCC 29112024.json, Grafimedia_cao.json, Reglement_Garantiefonds_07_12_2011__2_.json, DEF Grafimedia cao 2024-2025 TCC 09122024.json, Cao_2012_2013_wijz_art_169_z_renv_fndsbep_def.json, Grafimedia_cao_2015_2018_def_incl_stat_regl.json, DEF Grafimedia cao 2024-2025 schone versie v23102024.json, Grafimedia cao 2022-2024 15 februari 2022.json, Grafimedia cao 2018-2020 def 12-2-19.pdf .json, Grafimedia cao 2020-2021 6 juli 2021, gewijzigde werkingssfeer.json, Grafimedia cao 2020-2021 gewijzigde werkingssfeer.json, DEF Grafimedia cao 2024-2025 21012025.json</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -2362,22 +2146,18 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F50" t="inlineStr"/>
       <c r="G50" t="n">
         <v>0</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>tekst CAO Kappers 2010-2011.json, Tekst_cao_kappers_compleet.json, CAO Kappers 1 juli 2019 31 januari 2020 25072019.docx.json, CAOKAP~1.json, CAO_Kappers_1_juli_2017_30_juni_2019__3105_.json, CAO Kappers 1 juli 2024 30 juni 2025 (definitief).json, CAOKAP~2.json, CAO Kappers 1 juli 2023 30 juni 2024 geheel def.json, CAO Kappers 1 juli 2019 31 januari 2020 renvooi 07102019.docx.json, CAO_Kappers_1_juli_2017_30_juni_2019_1.json, CAO Kappers 1 juli 2022 30 juni 2023 schoon.json, CAO_Kappers_1_juli_2017_30_juni_2019.json</t>
         </is>
       </c>
       <c r="I50" t="inlineStr"/>
@@ -2403,19 +2183,15 @@
         <v>17</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F51" t="inlineStr"/>
       <c r="G51" t="n">
         <v>0</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao_Slagersbedrijf__versie_1_7_17.json, Cao voor het Slagersbedrijf 2019 - ongerenvooieerd.doc.json, Cao_Slagersbedrijf_1_10_17_tm_31_12_18_na_ttw_1.json, Cao_Slagers_1_4_16_tm_30_9_17.json, Cao_Slagersbedrijf_1_10_17_tm_31_12_18___def.json, Cao_voor_het_Slagersbedrijf_1_4_11_tm_31_3_13.json, Cao_Slagersbedrijf_1_4_15_tm_31_3_16.json, Cao_Slagersbedrijf_1_10_17_tm_31_12_18_na_ttw.json, CAOVOO~1.json, 02 - Cao voor het Slagersbedrijf 1-3-24 tm 31-8-25 - ongerenvooieerd.json, Cao voor het Slagersbedrijf.json, 26-DEF~1.json, Cao_voor_het_Slagersbedrijf_1_4_14_tm_31_3_15_1.json, Cao_voor_het_Slagersbedrijf_1_4_13_tm_31_3_14.json, Cao_voor_het_Slagersbedrijf_1_4_14_tm_31_3_15.json, Cao_voor_het_Slagersbedrijf_1_4_2011_tm_31_3_2013.json, 01-CAO~1.DOC.json</t>
         </is>
       </c>
       <c r="I51" t="inlineStr"/>
@@ -2441,19 +2217,15 @@
         <v>13</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F52" t="inlineStr"/>
       <c r="G52" t="n">
         <v>0</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Dhz-cao 2009-2011 def.json, Cao_DHZ_branche_2015_17_getekend.json, CAO_DHZ_2012_13_def.json, cao DHZ 2022-2023 nieuw geschoond.json, Dhz_cao_2009_2011_def.json, cao DHZ 2024-2026_def_april_2024.json, cao VWDHZ in pdf met handtekeningen.json, CAO-DHZ 2017-2020 wijzigingen geaccepteerd.doc .json, cao DHZ 2024-2026_def_dec_2024.json, CAO-DHZ 2022-2023 geschoond.json, cao DHZ 2024-2026_def_dec_2023.json, cao DHZ 2024-2026_def_mei_2024.json, cao DHZ 2024-2026_def_juni_2025.json</t>
         </is>
       </c>
       <c r="I52" t="inlineStr"/>
@@ -2476,22 +2248,18 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F53" t="inlineStr"/>
       <c r="G53" t="n">
         <v>1</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao_2015_2016_wijziging_SKA_en_SUCON_I.json, cao 1 april 2024 - 31 december 2025 definitief 28062024.json, cao_cc.json, cao_definitief_1.json, cao 1 april 2024 - 31 december 2025.docx.json, cao_2010___2012__versie_juli_2011_.json, Contractcateringbranche__Arbeidsvoorw_cao.json, cao 1 april 2024 - 31 december 2025 18122024 opgeschoonde versie.json, cao 1 april 2022 - 31 maart 2024, definitief 01052023.json, cao 1 april 2022 - 31 maart 2024, definitief 17032023.json, cao arbeidsvoorwaarden, definitief januari 2020.docx.json, cao_avwd_1_april_2013_tot_1_april_2014.json, cao_2014_2015.json, cao arbeidsvoorwaarden 1 april 2019 tot 1 april 2020, definitief.docx.json, cao 1 april 2022 - 31 maart 2024, definitief.json, cao_niet_gerenvooieerd.json, cao arbeidsvoorwaarden, definitief.json, cao 1 april 2022 - 31 maart 2024, definitief 18072023.json, cao_arbeidsvwd_2013_2014_gerenvooieerd.json, cao_1_april_2014_tot_1_juli_2015.json, cao 1 april 2022 - 31 maart 2024, definitief 03072023.json, caotekst_cc.json, cao_definitief_2.json, cao 1 april 2024 - 31 december 2025 definitief 26072024.json, contractcatering cao en handboek.json</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -2519,19 +2287,15 @@
         <v>21</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F54" t="inlineStr"/>
       <c r="G54" t="n">
         <v>0</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_Frugi_Venta_definitief_2012_2014.json, Frugi_Venta_2010-2011__(obv_463120).json, CAO Groothandel in Groenten en Fruit 2019-2020 na ttw art 13 23 40 bijlage III V.json, Groothandel in Groenten en Fruit CAO 2019-2020 na ttw ivm salaristabellen.docx.json, CAO boekje 2020_v5.json, CAO Groothandel in Groenten en Fruit 2019-2020 na ttw2 art 29b en bijlage X.json, CAO_2010-2011_Groothandel_Groenten_Fruit_.json, Frugi_Venta_CAO_2011_2012_.json, CAO Groothandel in Groenten en Fruit 1 jan. 2023 tm 30 juni 2024 versie 26-4-2023 na ttw.json, Groothandel_groenten_en_fruit_2014_2016_difinitief.json, CAO Groothandel in Groenten en Fruit 1 jan. 2023 tm 30 juni 2024 versie 9-3-2023.json, Groothandel_groenten_en_fruit_cao_2017_2018_na_ttw.json, CAO Groothandel in Groenten en Fruit 1 jan. tm 31 dec incl functiehandboek na tt.json, CAO_tekst_Groenten_en_Fruit_met_wijz_.json, Frugi_Venta_2009-2010_Groothandel_AGF.json, GGF_ttw_cao_2017_2018.json, Groothandel_groenten_en_fruit_cao_2017_2018.json, CAO Groothandel in Groenten en Fruit 1 juli 2024 tm 30 juni 2025 .json, Groothandel in Groenten en Fruit 2019-2020 definitief 03112019.json, 2022.08.17 CAO Groothandel in Groenten en Fruit 1 jan. tm 31 dec 2022.json, Groothandel in Groenten en Fruit cao 2021.json</t>
         </is>
       </c>
       <c r="I54" t="inlineStr"/>
@@ -2554,22 +2318,18 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F55" t="inlineStr"/>
       <c r="G55" t="n">
         <v>0</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao Hoveniers 1 juli 2021 - 30 juni 2023 integraal_1.json, Integrale tekst cao voor het Hoveniersbedrijf 1 juli 2023 tm 30 september 2024 incl. TTW per 1 juli.json, CAO Hoveniers 6e ttw per 1 maart 2021.docx.json, Integ_Cao_hov_incl_ttw_2018_2020.json, 20120946N_Cao_hoveniers_2011tm2013_TWW_artikel_9.json, Cao_hov_v3.json, Cao_hoveniers_1_3_2013_tm_31_12_2013_20130472N.json, Integrale tekst cao voor het Hoveniersbedrijf 1 oktober 2024 tm 30 juni 2026 incl. TTW per 1 juli 2025.json, Integrale tekst cao voor het Hoveniersbedrijf 1 juli 2023 tm 30 september 2024 (2402-1326).json, 20120041N_Cao_hoveniers_TTW_2012.json, 20110636N_Cao_hoveniers_01032011_tm_28022013.json, Cao_Hoveniers_integrale_tekst.json, cao Hoveniers incl 4e ttw 1 novemb er 2020 def 2010-0194.docx.json, Integrale_cao_Hov_2018_2020.json, Cao Hoveniers 1 juli 2021 - 30 juni 2023 integraal.json, Cao_hoveniers_tm_29_2_2016_2e_TTW_26_11_2015_def.json, Cao_hoveniers_1_1_2014_tm_29_2_2016_20140383Na.json, Cao Hoveniers 1 juli 2021 - 30 juni 2023 inclusief tussentijdse wijziging per 1.json, Cao_Hov_ttw_27_2_2019.json, TTW_Cao_hov_2_8_16.json, Cao_Hov_ttw_5_12_2018.json, Integrale tekst cao voor het Hoveniersbedrijf 1 oktober 2024 tm 30 juni 2026 (2503-1886).json, Cao Hoveniers 5e ttw per 20 november 2020 - 2011-1582.docx.json, cao_Hoveniersbedrijf_2016_2018_ttw___31_8_2016.json, Cao_hoveniers_tm_29_2_2016_TTW_15_7_2015.json, Cao Hoveniers 1 juli 2021 - 30 juni 2023- ttw 1 januari 2023.json</t>
         </is>
       </c>
       <c r="I55" t="inlineStr"/>
@@ -2595,19 +2355,15 @@
         <v>12</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F56" t="inlineStr"/>
       <c r="G56" t="n">
         <v>0</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO ETD d.d. 15 mei 2023 (naar SZW, TTW).json, tekst_CAO20182020ETD_def.json, tekstCAO_2015_2017_INTEGRAAL.json, CAO-2021-2022 ETD tekst 7 december.docx.json, CAO_2018_2020ETD_maart__def.json, CAO ETD d.d. 23 maart 2023 (naar SZW).json, CAO ETD d.d. 27 februari 2023 (naar SZW).json, Elektro tekstCAO-2010-2011 (januari 2011).json, CAO ETD tekst (d.d. 8 juli 2024).json, CAO ETD platte tekst (d.d. 5 juni 2024).json, CAO-2021-2022 ETD tekst TTW d.d. 20 juni 2023.json, CAO ETD d.d. 17 mei 2023 (naar SZW, Aanmelding TTW).json</t>
         </is>
       </c>
       <c r="I56" t="inlineStr"/>
@@ -2635,19 +2391,11 @@
       <c r="E57" t="n">
         <v>0</v>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F57" t="inlineStr"/>
       <c r="G57" t="n">
         <v>0</v>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr">
         <is>
@@ -2671,19 +2419,15 @@
         <v>17</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F58" t="inlineStr"/>
       <c r="G58" t="n">
         <v>0</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao_Binnendienst_schoon.json, Cao Verzekeringsbedrijf 2022-2023 def versie 24 mei 2022.json, Cao_Binnendienst_2015__2016_addendum.json, Cao voor het Verzekeringsbedrijf 2024.json, CAO Binnendienst 2018-2019.pdf .json, CAO_boekje_Binnendienst_wijzFAR.json, cao_binnendienst_2011_2012.json, Binnendienst_2015___2016_webversie.json, Cao_Binnendienst_2013.json, Cao Verzekeringsbedrijf 2022-2023 TTW februari 2023.json, Cao Verzekeringsbedrijf 2020 - integrale tekst.docx.json, Verzekeringsbedrijf_2016_2017_schoon_1.json, Cao_Verzekeringsbedrijf_2016_2017_schoon_ttw.json, Cao Verzekeringsbedrijf 2021 def versie 20210311.json, Cao_Verzekeringsbedrijf_Binnendienst_2018_2019.json, Cao voor het Verzekeringsbedrijf 2025-2026.json, Cao_binnendienst_2014.json</t>
         </is>
       </c>
       <c r="I58" t="inlineStr"/>
@@ -2709,19 +2453,15 @@
         <v>18</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F59" t="inlineStr"/>
       <c r="G59" t="n">
         <v>0</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_meubelindustrie_2018_2019_Def_1.json, CAO_tekst_2012_2014.json, CAOtekst2017.json, CAO Interieurbouw en Meubelindustrie 2024 clean.json, CAO meubelindustrie 2020-2021 def_1.json, Meubelindustrie__29_juli_2011.json, CAO_meubelindustrie_2018_2019_Def.json, CAO_tekst_2012_2014_1.json, CAO Interieurbouw en Meubelindustrie 2024 clean def.json, meubelindustrie_cao_tekst.json, CAO meubelindustrie 2022-2023.json, CAO meubelindustrie 2020-2021 def.json, CAO meubelindustrie 2018-2019 Def.docx .json, CAO_tekst_2015__2016_aangemeld.json, CAO meubelindustrie 2022-2023 TTW nieuwe cao tekst.json, CAO_tekst_2015__2016_aanmelding_tst_dispensatie.json, CAO meubelindustrie 2020-2021 def P.json, CAO meubelindustrie 2022-2023 TTW.json</t>
         </is>
       </c>
       <c r="I59" t="inlineStr"/>
@@ -2747,19 +2487,15 @@
         <v>8</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F60" t="inlineStr"/>
       <c r="G60" t="n">
         <v>1</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>WFC cao 2025-2027 na ttw 13-2-2025 szw.json, CAO Facilitaire contactcenters 2024 18-12-2023.json, CAO Facilitaire contactcenters 2022-2023 na ttw 23-6-2023_.getekend.json, Cao FACILITAIRE CONTACTCENTERS.pdf .json, CAO Facilitaire contactcenters 2019 - 2021 versie 10.11.2020.json, 2024.12.10 WFC cao 2025-2027 Clean Version Final_ getekend szw.json, CAO Facilitaire contactcenters 2024 na ttw 31-01-2024.json</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -2787,19 +2523,15 @@
         <v>17</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F61" t="inlineStr"/>
       <c r="G61" t="n">
         <v>0</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_CAR_2015_2017.json, HB 5e editie 2024_2.json, CAO_CA_17_19.json, CAO Car 2021 2024b.json, CAO_CAR_2017_2019_TTW_juli_2017.json, HB 5e editie 2024.json, CAO_CAR_2017_2019_TTW_LL_nov_2018.json, carrosserie_aangepast_cao_n_a__v_bed.json, CAO_CAR__TTW_JULI.json, M_T_Totaal_tekst.json, CAO_CAR_2017_2019_TTW_GP_nov_2017.json, M_en_T_Carrosseriebedrijf_cao_en_handboek_doc.json, CAO CARR 2019 2021 SZW TTW Wagweu art 64.docx.json, CAO Car 2021 2024.json, CAO CARR 2019 2021 SZW TTW V2 Wagweu.docx.json, HB 5e editie 2024_1.json, CAO_CAR_arcering___wijz_AOW_LT.json</t>
         </is>
       </c>
       <c r="I61" t="inlineStr"/>
@@ -2822,22 +2554,18 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F62" t="inlineStr"/>
       <c r="G62" t="n">
         <v>0</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Openbaar Vervoer caotekst.json, CAO_OV_tekst_2013_DEFINITIEF_v2.json, CAO_OV_tekst_2014_en_2015_DEFINITIEF.json, CAO_OV_tekst_2016_en_2017_DEFINITIEF.json, CAO OV 01012018 30062020 definitief 160519.pdf .json, CAO_OV_tekst_2014_en_2015_DEFINITIEF_1.json, CAO OV 1 juli 2021 31 december 2022 tekst aanmelding.json, CAO_OV_tekst_2013_DEFINITIEF.json, CAO OV 1 juli 2020 30 juni 2021 tekst aanmelding.json, CAO_OV_tekst_2011_en_2012_def_140512.json, CAO OV 1 januari 2023 31 maart 2025 tekst aanmelding.json</t>
         </is>
       </c>
       <c r="I62" t="inlineStr"/>
@@ -2863,19 +2591,15 @@
         <v>1</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
       <c r="G63" t="n">
         <v>0</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_Tekst___CAO_Vast_2011___2012.json</t>
         </is>
       </c>
       <c r="I63" t="inlineStr"/>
@@ -2901,19 +2625,15 @@
         <v>17</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F64" t="inlineStr"/>
       <c r="G64" t="n">
         <v>1</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao_reisbranche_2016_2018_definitief_einddocument.json, cao Reisbranche 1jul2024-1jul2026 def1.json, 2019 Tekst cao-reisbranche 1 november 2018 - 1 september 2019 - versie 2.0.json, Tekst cao Reisbranche 1jul21-31dec21.json, CAO_2015_2016_aanmelding.json, cao Reisbranche 1jul2024-1jul2026 def.json, CAO_teksten_voor_CAO_2013_2015_wijzigingen_def_R2.json, DEF_Tekst cao Reisbranche 1jan-1jul2022 - avv.docx.json, Tekst_cao_reisbranche_2016_2018_def_tekst.json, cao Reisbranche 1jul2022-1jul2024 - versie 2 sept 2022.json, 2019 Tekst cao-reisbranche 1 november 2018 - 1 september 2019.pdf .json, cao Reisbranche 1jul2022-1jul2024 concept versie.json, AWVN__487825_v1_DefCAO_ANVR_2011_2012.json, cao Reisbranche 1jul2024-1jul2026 def2.json, ANVR_CAO_2012_2013_Gecorrigeerde_tekst_def_R1.json, Tekst cao Reisbranche definitief.docx.json</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -2941,19 +2661,15 @@
         <v>14</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F65" t="inlineStr"/>
       <c r="G65" t="n">
         <v>0</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO NWb 2018-2021-def.json, Cao_NWb_2015_2018_procesafspraken_30_03_2016.json, cao_Netwerkbedrijven_2_0_2011_2013.json, cao NWb 2021-2022.json, cao_NWb_2015_2018.json, cao NWb 2023 ondertekende versie.json, CAO NWb 2018 - 2021 - getekend.pdf .json, cao NWb 2024-2025_getekend.json, WEN25057_cao NWb-2026NL-FINAL zonder handtekening.json, Cao_NWb_2013_2015_met_aanpassing_DI.json, NWb_cao.json, CAO_NWb_2011_def.json, Cao_NWb_2013_1_mei.json, Cao_NWb_2013_2015_met_aanpassing_HNW_schoon.json</t>
         </is>
       </c>
       <c r="I65" t="inlineStr"/>
@@ -2976,22 +2692,18 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>281</v>
+        <v>17</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F66" t="inlineStr"/>
       <c r="G66" t="n">
         <v>0</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_Vleessector_2024-2025 met tussentijdse wijzigingen 3 juni 2024.json, Vleessector_cao_incl__reglement_ongerenvooieerd.json, CAO_Vlees_2011__ongerenvooieerd_.json, CAO_VLEESSECTOR_2014_ongerenvooieerd_1.json, CAO_VLEESSECTOR_2014_ongerenvooieerd.json, CAO_2016_na_opm_artikel_42.json, CAO_VLEESSECTOR_2014_volledige_tekst.json, cao 2021 compleetnav opmerkingen SZW.json, CAO_Vleessector_2024-2025 met wijzigingen geacepteerd voor ministerie.json, cao 2021 definitief voor avv.json, CAO_vleessector_ongerenvooieerde_tekst_2013.json, cao 2019-2020 met wijzigingen geacepteerd definitief.docx_1.json, CAO_2017_2019_tekst_voor_boekje.json, cao vlees 2022-2024 definitief.json, CAO_2016.json, cao 2019-2020 met wijzigingen geacepteerd definitief.docx.json, Tussentijds_gewijzigde_cao.json</t>
         </is>
       </c>
       <c r="I66" t="inlineStr"/>
@@ -3017,19 +2729,15 @@
         <v>7</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F67" t="inlineStr"/>
       <c r="G67" t="n">
         <v>0</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>NHG_cao_1_jan_2014_tot_en_met_31_dec_2018.json, NHG_Cao_tm_31_12_2022.json, wijziging_NHG_CAO__teksten_1_juli_2016_2016.json, NHG-CAO 2019 tm 2022- herziene uitg. conform WAB 1 jan 2020.json, CAO_boekje_NHG_2014_2018_versie_2_mei_2014.json, NHG CAO_herziene uitgave 1 januari 2020 gewijzigd conform de WAB.json, NHG_CAO_05_2014.json</t>
         </is>
       </c>
       <c r="I67" t="inlineStr"/>
@@ -3055,19 +2763,15 @@
         <v>21</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F68" t="inlineStr"/>
       <c r="G68" t="n">
         <v>0</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_Timmer_avv_27_3_2014.json, DEF_ARBVW_2011_2012.json, CAO_Timmer_1_apr___18_t_m__31_mrt__19_2e_vers_.json, CAO_Timmer_aanp_avv_14_4_2014.json, cao_nr__51_aug__18.json, INTEGRALE TEKST cao timmerindustrie 1 aug 2020 - 30 nov 2021.json, Cao Timmer 2024-2025 - incl bijlagen 28-06-2024.json, cao Timmerindustrie 1 dec 21 tt 1 mrt 2024_1.json, cao_Timmerindustrie_TTW_1_1_2015_tm_31_3_2017.json, Int_2__caoTimmer_TTW_1_1_15_tm_31_3_17.json, Cao Timmerindustrie 1 dec 21 tt 1 mrt 2024.json, Cao Timmerindustrie 1 apr 2019 tm 31 juli 2020.json, GEWIJZIGDE_april_DEF_ARBVW_2011_2012.json, Cao_Timmer_apr__2017__apr__2018.json, EINDVERSIE_CAO_TIMMERIND__2015_2017.json, cao Timmer nr 51 INTEGRAAL 1 aug 2020 - 30 nov 21.json, avv_REDACTIETEKST_ARBVW_2013_26sept.json, Minis_Cao_Timmer_apr__2017__apr__2018.json, CAO Timmerindustrie 1 apr 2019 tm 31 juli 2020 wijzigingen sept.19.json, Cao Timmer 2024-2025 - TTW .json, INTEGRALE cao Timmerindustrie 1 dec 21 tt 1 mrt 2024.json</t>
         </is>
       </c>
       <c r="I68" t="inlineStr"/>
@@ -3093,19 +2797,15 @@
         <v>18</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F69" t="inlineStr"/>
       <c r="G69" t="n">
         <v>1</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao Textielverzorging 2024-2025 vs aug24.json, Cao Textielverzorging 2023-2024 doorlopende tekst def.json, Cao Textielverzorging integrale tekst TTW.json, Cao Textielverzorging integrale tekst 2020-2021 TTW2.json, Cao Textielverzorging integrale tekst 2020-2021.json, Cao Textielverzorging 2024-2025.json, Raltex_volledige_tekst_met_alle_bijlagen_NA_TTW.json, Cao Textielverzorging integrale tekst 2020-2021_1.json, Cao Textielverzorging integrale tekst 1-4.json, Raltex_volledige_tekst_met_alle_bijlagen_NA_TTW_1.json, Cao Textielverzorging 2023-2024 TTW doorlopende tekst.json, Cao Textielverzorging integrale tekst.json, Cao Textielverzorging 2025-2026.json, CAO_Aanmelding.json, Tussentijdse_wijziging_AVV_integrale_tekst.json, Raltex_CAO_Textielverzorging_doorlopende_tekst.json, digitaleintegraletekstraltex.json</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -3133,19 +2833,15 @@
         <v>2</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F70" t="inlineStr"/>
       <c r="G70" t="n">
         <v>0</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>140408_CAO_2012_2014_eindtekst_3_juli_2013_hvb.json, CAO_tekst_Tuincentra.json</t>
         </is>
       </c>
       <c r="I70" t="inlineStr"/>
@@ -3171,19 +2867,15 @@
         <v>11</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F71" t="inlineStr"/>
       <c r="G71" t="n">
         <v>1</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Groothandel_in_Bloemen_en_Planten_2009-2012.json, VGB cao 2024 - 2026.json, VGB TTW 2021-2023.json, VGB cao tekst.json, CAO tekst juli 2019 tm juni 2021.json, CAO_GBP_2017_2019_Definitieve_versie_1.json, Definitieve cao VGB 2021-2023.json, CAO_GBP_2014_2016_definitieve_versie.json, CAO_GBP_2017_2019_Definitieve_versie.json, Groothandel_in_Bloemen_en_Planten____CAO_2012_2014.json</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -3208,22 +2900,18 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F72" t="inlineStr"/>
       <c r="G72" t="n">
         <v>0</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>VBZ_cao_2017_def.json, Cao Zoetwarenindustrie 2023-2024.json, Cao na ttw Zoetwaren looptijd 1 januari 2023 tm 30 september 2024 (6 november 2023).json, VBZ_CAO_2012_2013__na_ttw_ivm_avv.json, VBZ_cao_2015_2016.json, Cao Zoetwarenindustrie 2021-2022 def.json, Zoetwarenindustrie_cao_2018.json, Cao Zoetwaren 2024-2026 na ttw (12 juni 2025).json, Herschreven cao Zoetwaren_finale versie (2 december 2024)_incl. IKB en akkoord cao-partijen (25 april 2025).json, VBZ_CAO_2012_2013__def.json, VBZ_cao_2014.json, Zoetwaren_arbvoorw_CAO_2011_2012_.json, zoetwarindustrie cao 2019-2020 FINAAL.docx .json, Zoetwarenindustrie 2019-2020 na ttw ivm artikel 14 en 25 lid 3.pdf .json, Cao Zoetwarenindustrie 2021-2022 na correctie art 31.json</t>
         </is>
       </c>
       <c r="I72" t="inlineStr"/>
@@ -3249,19 +2937,15 @@
         <v>21</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F73" t="inlineStr"/>
       <c r="G73" t="n">
         <v>0</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao MITT 2024-2025 versie 18 06112024 (003).json, SZW_CAOMITT2016_19_meld_2e_tussent__wijz__sch.json, CAO_MITT_2012_2014_schoon_dd__18_10_2012.json, CAOMITT_2014_2016_tussent_wijz_dec__2015_sch2.json, CAO MITT 2020 na ttw2 art. 1.3 en 6.3.json, SZW_CAO_MITT_2010_2012__wijziging_dec_2011_schoon.json, CAO MITT 2022-2023 definitief.json, SZW_CAO_MITT_2010_2012__wijziging_jan_2012_schoon.json, CAO MITT 2020 _1.json, SZW_CAOMITT2016_19_meld_3e_tussent__wijz__sch_.json, MITT cao 2019-2020.json, SZW_CAO_MITT_2012_2014_schoon_dd_6_9_2012.json, CAO MITT 2010-2012 -melding sept 2010-schoon.json, CAO_MITT_2014_2016_tussent__wijz__sch_szw.json, CAO MITT 2020 .json, CAO_MITT_2014_2016___schoon___niet_geel_gearceerd.json, CAO MITT 2021-2022.json, CAOMITT2014_16_tussent_wijz__juli_2017_sch_szw.json, CAO MITT 2023 versie 06072023.json, SZW_CAOMITT2016_19_melding__tussent__wijz__sch.json, SZW_CAOMITT2016_19_melding_schn_geen_wijz__zichtb_.json</t>
         </is>
       </c>
       <c r="I73" t="inlineStr"/>
@@ -3287,19 +2971,15 @@
         <v>13</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F74" t="inlineStr"/>
       <c r="G74" t="n">
         <v>0</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Tekst CAO Boek en Kantoor 24 25 ongemark def.json, CAO_Kantoor_18_19_def_aanm.json, CAO_Kantoor_en_Boek_16_17_def.json, CAO_Kantoor_en_Boek_17_18_def.json, Boekhandel Kantoorvakhandel 2010-2012.json, Cao_Boekhandel_en_Kantoorvakhandel_2014_2016.json, Cao_Boekhandel_en_Kantoorvakhandel_2012_2014.json, Tekst CAO Boek en Kantoor 21 23 def.json, Cao_Boekh_en_Kantoorvakh_2012_2014_def.json, 070224_Tekst CAO Boek en Kantoor 23 24 ongemark def.json, Tekst CAO Boek en Kantoor 19 20 31-10-2019 ongemark def aanm.docx.json, CAO_Kantoor_en_Boek_17_18_nw_def.json, CAO_Kantoor_en_Boek_17_18_nw_sept.json</t>
         </is>
       </c>
       <c r="I74" t="inlineStr"/>
@@ -3325,19 +3005,15 @@
         <v>9</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F75" t="inlineStr"/>
       <c r="G75" t="n">
         <v>0</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_voor_de_Zorgverzekeraars_2013_2015.json, CAO_Zorgverzekeraars_2018_2019.json, CAO Zorgverzekeraars 2019-2020.json, CAO voor de Zorgverzekeraars 2022-2024.json, Cao_zorgverzekeraars_2015_2016_definitief.json, CAO voor de Zorgverzekeraars 2010-2011.json, Cao_voor_de_Zorgverzekeraars_2016_2018.json, Cao voor de Zorgverzekeraars 2021-2022.json, CAO_voor_de_Zorgverzekeraars_2011_2012.json</t>
         </is>
       </c>
       <c r="I75" t="inlineStr"/>
@@ -3363,19 +3039,15 @@
         <v>18</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F76" t="inlineStr"/>
       <c r="G76" t="n">
         <v>1</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao_tekst_Tank_Was_2017_2019_v1.json, cao_tekst_Tank_Was_2017_2019_def.json, cao tekst Tank Was 2022-2023, definitief.json, cao tekst Tank Was 2020 2021 versie 20 juli 2020.doc.json, CAO_tekst_2013_2015.json, cao tekst Tank Was 2024 - 2025, definitief 21032024.json, cao_tekst_Tank_Was_def_3_juni_2016_1.json, cao_tekst_Tank_Was_2017_2019_def_1.json, cao tekst Tank Was 2024 - 2025, definitief 25012024.json, CAO_tekst_2013_2015_def.json, CAO_tekst_2011_2013.json, cao tekst Tank Was 2020 2021 versie 22 juni.doc.json, Ingediend bij SZW - Eindtekst cao Tankstations en Wasbedrijven 1 april 2025 - 31 december 2026.json, cao_tekst_Tank_Was_def_3_juni_2016.json, CAO_tekst_2011_2013__2_.json, cao tekst Tank Was 2022-2023, definitief 28032022.json, cao tekst Tank Was 2020 2021 versie 22 juli 2020.doc.json</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -3403,19 +3075,15 @@
         <v>20</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F77" t="inlineStr"/>
       <c r="G77" t="n">
         <v>0</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO-tekst 2021_2022_geschoond3.json, CAO-tekst 2020_def.docx.json, CAO_tekst_2015_2016_geschoond.json, handel__in_bouwmaterialen_cao_integraal.json, CAO-tekst 2023_2024_geschoond_02.json, CAO-tekst 2019_vs4_def.docx .json, CAO_tekst_2017_2018_geschoond.json, CAO-tekst 2019.docx .json, CAO-tekst 2023_2024_geschoond_04.json, CAO-tekst 2019_vs3.docx .json, CAO-tekst 2024-2025 versie 1.0.json, CAO_tekst_2010_2012_per01042013.json, CAO-tekst 2021_2022_geschoond.json, integrale CAO-tekst 2010-2012.json, hibin_CAO_tekst_2017_2018.json, CAO-tekst 2019_vs2.docx .json, CAO-tekst 2024-2025 versie 2.0.json, CAO-tekst 2023-2024 versie 1.0 zonder wijzigingen.json, cao tekst.json, CAO-tekst 2021_2022_defV2_geschoond.json</t>
         </is>
       </c>
       <c r="I77" t="inlineStr"/>
@@ -3441,19 +3109,15 @@
         <v>18</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F78" t="inlineStr"/>
       <c r="G78" t="n">
         <v>0</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023 inclusief T.json, Cao_productiegerichte_dierhouderij_2014_2017.json, Eindtekst_cao_Dierhouderij_2012_2013_incl__ttw.json, cao_tekst_integraal.json, cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023.json, cao productiegerichte dierhouderij 2021 versie 30 januari 2021.docx.json, CAO_Dierhouderij_2010__2012.json, cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023_1.json, Eindtekst cao Productiegerichte Dierhouderij 1 januari 2024 - 31 december 2025.json, Eindtekst cao Productiegerichte Dierhouderij 1 januari 2024 - 31 december 2025 incl. 2e ttw per 1 januari 2025.json, Eindtekst cao Productiegerichte Dierhouderij 1 januari 2024 - 31 december 2025 incl. 1e ttw per 1 januari 2024.json, cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023 inclusief T_1.json, cao_Pg_Dierhouderij.json, Integrale tekst cao Productiegerichte Dierhouderij 2022 - 2023 (TTW per 1 juli 2023).json, cao_tekst_Pg_Dierhouderij.json, 20120967N_Eindtekst_cao_Dierhouderij_2012_2013.json, cao productiegerichte dierhouderij 2021 ttw 17 maart 2021.json, cao PGD integraal def.docx.json</t>
         </is>
       </c>
       <c r="I78" t="inlineStr"/>
@@ -3479,19 +3143,15 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F79" t="inlineStr"/>
       <c r="G79" t="n">
         <v>0</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_PLb_2013_caotekst.json, Sector-cao PLb 2025-2026 definitief.json, Cao PLb versie 5 juli 2021-signed.json, Productie__en_Leveringsbedrijven_cao_2011_2013.json, CAO tekst CAO PLb 2023-2024 ondertekend door cao-partijen.json, CAO_PLb_2013_def___ondertekend.json, CaoPLb_herstel_foute_verwijz_en_redac_wijz_tbvAVV.json, CAO PLb 2022-2023 definitief ondertekend.json, CAO PLb 2018 - 2020 ondertekend.pdf .json, CAO_PLb_2015___2018_definitief__30_juni_2016_.json</t>
         </is>
       </c>
       <c r="I79" t="inlineStr"/>
@@ -3517,19 +3177,15 @@
         <v>3</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F80" t="inlineStr"/>
       <c r="G80" t="n">
         <v>1</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_BTU_2014.json, CAO_BTU_2012_2013_v1_21_Geschoond.json</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -3557,19 +3213,15 @@
         <v>14</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F81" t="inlineStr"/>
       <c r="G81" t="n">
         <v>0</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao_Bloemenspeciaalzaken_16_8_2018.json, 1. 20250117 Def. cao Gesp. detailhandel bloemen en planten 2025-2026.json, cao_2011__2012_definitief.json, CAO_Gespec_Detailh_Bloemen_en_Planten_2018___2019.json, 2__Cao_Gesp___Detailh__in_Bloemen_en_Planten.json, Gewijzigde tekst 14 mei 2020 2.1.c Cao Gespecialiseerde detailhandel in bloemen.json, def. cao tekst Gespecialiseerde detailhandel in bloemen en planten 2023.json, 2024-02-15 Def. tekst tussentijds gewijzigde cao met wijzigingen bijgehouden cao Gespecialiseerde detailhandel in bloemen en planten 2024.json, def. cao tekst Gespecialiseerde detailhandel in bloemen en planten 2023_1.json, Cao_tekst_1.json, c. 20240403 (Schoon) Tekst tussentijds gewijzigde cao Gespecialiseerde detailhandel bloemen en planten.json, 2024-01-19 Def. tekst schoon cao Gespecialiseerde detailhandel in bloemen en planten 2024.json, Cao_tekst.json, 2.1.c Cao Gespecialiseerde detailhandel in bloemen en planten 2020 - 2022.docx.json</t>
         </is>
       </c>
       <c r="I81" t="inlineStr"/>
@@ -3595,19 +3247,15 @@
         <v>13</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
       <c r="G82" t="n">
         <v>1</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO Waterbouw 2023-2024 schoon.json, CAO Waterbouw 2019-2020 definitief.docx .json, CAO Waterbouw 2021-2022 Integraal 03.12.2021.json, CAO_Waterbouw VERSIE 110329.json, CAO_VVW12.json, CAO Waterbouw 2022-2023_1.json, CAO Waterbouw 2024-2025 schoon.json, CAO Waterbouw 2022-2023.json, CAO_Waterbouw_2013_2014_def.json, CAO_Waterbouw__def_23_mei_2014_AVV.json, CAO_Waterbouw_2018_2019_definitief.json, CAO_Waterbouw_2015_2018_def__8_juli_2015.json</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -3635,19 +3283,15 @@
         <v>14</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F83" t="inlineStr"/>
       <c r="G83" t="n">
         <v>0</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Textielgroothandel_cao_2014_2016.json, Textielgroothandel_cao_ttw.json, Textielgroothandel_cao_2017_2018.json, Cao 2021-2023 na ttw.json, Textielgroothandel_CAO_2011_2012.json, Textielgroothandel_cao_2018_2020.json, cao_2016_2017_Textielgroothandel.json, Cao Textielgroothandel 2024-2026 versie 21-1-2025.json, Textielgroothandel_2012_2013.json, Cao Textielgroothandel 2023-2024 versie 19-7-2023.json, Cao Textielgroothandel 2023-2024 versie 21-8-2023.json, Textielgroothandel_CAO_2013_2014.json, cao 2021-2023.json, Textielgr__NVW_ttw_ivm_fkb_2012_2013_obv_1538864.json</t>
         </is>
       </c>
       <c r="I83" t="inlineStr"/>
@@ -3673,19 +3317,15 @@
         <v>13</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
       <c r="G84" t="n">
         <v>0</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_Sport_2016_2018_DEF.json, def__cao_WOS_01_01_2012_totmet_31_12_2012.json, WOS_cao_2013_definitief.json, CAO DEFINITIEF WOS.pdf .json, CAO_Sport_2015.json, Definitieve cao Sport 2022 - 2023.json, Sport cao 2024-2025.json, Sport-CAO 2019-2020 ttw.json, Sport 2021 definitief.json, CAO Sport 2022-2023 2.json, Sport_WOS_cao_2014.json, CAO 2009_2012_definitief.json, CAO_Sport_2016_2018_DEF_1.json</t>
         </is>
       </c>
       <c r="I84" t="inlineStr"/>
@@ -3708,22 +3348,18 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F85" t="inlineStr"/>
       <c r="G85" t="n">
         <v>0</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao 2022-2023 6 januari 2022 aanmelding.json, cao 2022-2023 ttw februari 2023 integraal.json, cao_afbouw_2011_12__integrale_cao.json, CAO_2015_2017_TTW_integrale_tekst.json, cao 2020-2021 integraal2.docx.json, 20241203 cao 2024-2025 ttw januari 2025 integraal.json, CAO_2013_2014_definitief_2.json, CAO_2018_2019_integraal_versie_8.json, CAO 2018-2019 integraal.docx .json, cao 2022-2023 ttw 10 maart 2023 integraal.json, CAO_2015_2017_integrale_tekst2.json, cao afbouw 2022-2023 6 januari 2022 aanmelding 2.docx.json, cao 2020-2021 integraal.docx.json, CAO_2015_2017_TTW_integrale_tekst_1.json, cao 2024-2025, ttw augustus 2024, integraal.json, CAO_2015_2017_integrale_tekst.json, CAO_2013_2014_definitief.json, cao 2020-2021 ttw integraal.docx.json, CAO_2018_2019_integraal.json, cao 2024-2025, 18 april 2024 integraal.json, cao 2024-2025, 30 januari 2024 integraal.json</t>
         </is>
       </c>
       <c r="I85" t="inlineStr"/>
@@ -3746,22 +3382,18 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F86" t="inlineStr"/>
       <c r="G86" t="n">
         <v>0</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>15_00080a_NvW_Cao_OB_2015_2019_wijz_geaccepteerd.json, 2024-08-09 Cao OB gehele tekst met juiste opmaak_inhoudsopgave.json, Cao OB 1.7.2020 31.12.2022 ondertekend TUSSENTIJDSE TEKSTUELE WIJZIGINGEN GEAC.json, Cao_OB_2015_2019_salaristabel_1_juli_2017.json, Cao OB 2024 2026_incl gewijz Ontheffingsregeling.json, Cao_OB_2015_2019_invulling_loonruimte_2017.json, Cao OB_1.7.2019-1.7.2020.docx.json, Cao_OB_2015_2019_invulling_loonruimte_2016.json, 13_00052_Cao_OB_2014.json, 241129 Cao OB 2024 2026 tussentijdse wijzigingen.json, Cao_OB_verlenging_1_januari_2015_tot_15_juni_2015.json, CAO_2012_2013_def_incl_aanpassing_vakantiewet.json, Cao_OB_2015_2019_invulling_loonruimte_2019.json, Cao_OB_2015_2019_invulling_loonruimte_2018.json, Cao OB 1.7.2020 31.12.2022 ondertekend TUSSENTIJDSE WIJZIGING SALARISGARANTIE_GE.json, CAO 2010-2011.json, Cao_OB_2015_2019_WML_2018.json, 231122_wijz geaccepteerd_tussentijdse wijziging ivm avv_230428 cao OB 1.1.2023_31.3.2024_DEF.json, 230428 cao OB 1.1.2023_31.3.2024_DEF.json, Cao OB 1.7.2020 31.12.2022 ondertekend.json, Openbare_Bibliotheken_2012_2013.json</t>
         </is>
       </c>
       <c r="I86" t="inlineStr"/>
@@ -3787,19 +3419,15 @@
         <v>20</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F87" t="inlineStr"/>
       <c r="G87" t="n">
         <v>0</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Architecten_met_salaristabel.json, Cao_2013_2015.json, Cao Architectenbureaus 2021 2023 incl functiehandboek schoon.json, 43 Cao 25-26 excl wijzigingen_ (002).json, cao 2019-2021 incl functiehandboek met gewenste wijzigingen - aangemeld.docx.json, CAO_2013_2015__2_.json, 43 Cao voor architectenbureaus_ 1 jan tm 31 dec 2024_schone tekst.json, CAO_nw_2011_2013_boekje.json, 43 Cao voor architectenbureaus_ 1 jan tm 31 dec 2024_schone tekst - Kopie.json, Cao Architectenbureaus 2021 2023 incl functiehandboek_TTW artikel 22 lid 5_schoon.json, cao_architectenbureaus_2017_2019_2.json, 43 Cao voor architectenbureaus_ 1 jan tm 31 dec 2024_schone tekst - Kopie_1.json, cao_2015_2017_opmaak_A4.json, cao_architectenbureaus_2017_2019.json, cao tekst 2020, incl. functiehandboek TTW.docx.json, cao_architectenbureaus_2017_2019_per1_7_2018_def.json, CAO_2015_2017_1.json, cao 2019-2021 incl functiehandboek - aangemeld.docx .json, 43 Cao voor architectenbureaus_schoon_1 mrt tm 31 dec 2023.json, CAO_2015_2017.json</t>
         </is>
       </c>
       <c r="I87" t="inlineStr"/>
@@ -3827,19 +3455,11 @@
       <c r="E88" t="n">
         <v>0</v>
       </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F88" t="inlineStr"/>
       <c r="G88" t="n">
         <v>0</v>
       </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr">
         <is>
@@ -3863,19 +3483,15 @@
         <v>14</v>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F89" t="inlineStr"/>
       <c r="G89" t="n">
         <v>0</v>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao Betonproductenindustrie 2025-2026 versie 17-2-2025.json, Integrale_Cao_tekst_2017_2019_vs3.json, Cao Betonproductenindustrie 2023 versie 13-3-2023.json, Integrale_Cao_tekst_2017_2019_vs2.json, Cao Betonproductenindustrie 2021-2022 definitief.json, Cao Betonproductenindustrie 2019-2021 versie 08-04-2021.json, cao voor de betonproductenindustrie.json, CAO_2017_2019.json, Cao Betonproductenindustrie 2019-2021 na ttw versie 25-05-2021.json, Cao Betonproductenindustrie 2021-2022 na ttw definitief.json, CAO_voor_de_betonproductenindustrie_2011_2013.json, Cao_BPI_2014_2017_nieuwe_tekst.json, Cao Betonproductenindustrie 2024 versie 8-5-2024.json, cao_voor_de_betonproductenindustrie_2013__2014.json</t>
         </is>
       </c>
       <c r="I89" t="inlineStr"/>
@@ -3903,19 +3519,11 @@
       <c r="E90" t="n">
         <v>0</v>
       </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F90" t="inlineStr"/>
       <c r="G90" t="n">
         <v>0</v>
       </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H90" t="inlineStr"/>
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr">
         <is>
@@ -3939,19 +3547,15 @@
         <v>14</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F91" t="inlineStr"/>
       <c r="G91" t="n">
         <v>0</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cao Railinfrastructuur -staand DEFINITIEF periode 8-2025 voor AVV.json, Def tekst Cao 2021 versie 0.7_01062021.json, Rallinfra_CAO_2011_2012__definitief.json, Railinfra_CAO_2014_def_26042016.json, PDF Werkdocument Cao 2023 vers.02 01032023 (002).json, versie 2 def Cao Railinfrastructuur - DEFINITIEF juni 2024 - versie voor AVV - kopie.json, Cao Railinfrastructuur - 9 juli 2024.json, Rallinfra caotekst.json, railinfra_addendum_en_cao.json, Railinfra_CAO_2017_def_280917_1.json, Tekst Cao 2018.2019 def d.d. 22-05-2019 .pdf .json, Railinfra_CAO_2013__DEF_02_08_13.json, Railinfra_CAO_2017_def_280917.json, Cao Railinfrastructuur - DEFINITIEF 21 maart 2024 (002).json</t>
         </is>
       </c>
       <c r="I91" t="inlineStr"/>
@@ -3974,22 +3578,18 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F92" t="inlineStr"/>
       <c r="G92" t="n">
         <v>0</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao_arbeidsvoorwaarden_2018_2020_getekend.json, Cao_graan_be_en_verwerkende_bedrijven_2015___2017.json, cao tekst 2010 - 2012 per 1-4-2011.json, Cao Graanbe- en verwerkende bedrijven 2020 - 2022.json, x DEF Cao-teksten graanbe- en verwerkende bedrijven 2025.json, Cao_boekje_2012_2013.json, Cao Graanbe- en verwerkende Bedrijven 2024.pdf.json, CAO_boekje_2014___2015.json, cao_tekst_2013___2014.json, Tekst_cao_graan_2017__2018_def_MET_handtekening.json, cao_boekje_2015_2017.json, cao_arbeidsvoorwaarden_2018_2020_getekend_1.json, cao_tekst_2015___2017.json, Cao Graanbe- en verwerkende Bedrijven 2023 DEF.json, cao_tekst_2013___2014_DEF_Z_HT.json</t>
         </is>
       </c>
       <c r="I92" t="inlineStr"/>
@@ -4015,19 +3615,15 @@
         <v>13</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F93" t="inlineStr"/>
       <c r="G93" t="n">
         <v>1</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Nieuwe CAO 2018-2020 volledig.docx.json, AGF_detailhandel_in_Nieuwe_CAO_2018_2020.json, CAO_Aardapp__en_loont_.json, CAO_2016_2018_AGF_Detailhandel.json, CAO_2016_2018_AGF_Detailhandel_1.json, CAO_2014_2016_AGF_Detailhandel_zonder_bijlagen.json, Definitieve tekst CAO AGF Detailhandel 2024-2025_1.json, CAO AGF Detailhandel 2021-2024 def_.json, CAO AGF Detailhandel 2021-2024 aanmelding.json, CAO AGF Detailhandel 2020-2021 volledig.docx.json, CAO AGF Detailhandel 2020-2021 volledig def.docx.json, cao 2010-2012 volledig.json</t>
         </is>
       </c>
       <c r="I93" t="n">
@@ -4055,19 +3651,15 @@
         <v>12</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F94" t="inlineStr"/>
       <c r="G94" t="n">
         <v>0</v>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>sociale afspraken 2020 - 2023 geschoond.json, CAO Banden- en Wielenbranche 2023 na ttw 17-7-2023.json, sociale afspraken 2019 - 2020 geschoond.docx.json, CAO Banden- en Wielenbranche 2023 12-6-2023.json, sociale afspraken 2020 - 2023 geschoond_1.json, CAO Banden- en Wielenbranche 2024-2025 versie 9-4-2024 (2).json, cao_2016_2017_geschoond_26_07_16.json, sociale_afspraken_2018___2019_geschoond.json, CAO_2016___2017_geschoond.json, CAO_2010___2012_geschoond.json, CAO Banden- en Wielenbranche 2024-2025 na ttw2 versie 26-6-2024.json, CAO na ttw Banden- en Wielenbranche 2024-2025 versie 30-4-2024.json</t>
         </is>
       </c>
       <c r="I94" t="inlineStr"/>
@@ -4090,22 +3682,18 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F95" t="inlineStr"/>
       <c r="G95" t="n">
         <v>0</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Zuivel cao I 2022 tussentijdse wijziging dec 2021.json, Zuivel I 2018-2020.pdf .json, Cao I zuivel 2022na ttw def.json, AWVN__534089_v1_Zuivel_CAO_I_2012_2014.json, Zuivel_cao_I_2016_2018.json, Zuivel I 2020.json, Zuivel cao I 2022.json, Zuivel_CAO_I_na_ttw2.json, Zuivel cao I 2021.json, Zuivel_2016_2018_cao_I.json, DEF cao I zuivel 1 april 2024 tot 1 april 2025.json, Zuivel I 2018-2020.docx .json, Zuivel_CAO_I_na_ttw_2012_2014_obv__1499987v0_2.json, Zuivelindustrie_tekst_nieuw_2014_2016.json, Cao I zuivel na ttw 1 januari 2023 tot en met 31 maart 2024.json, Zuivel cao I 1 januari 2023 tot en met 31 maart 2024.json, Zuivel_ttw_ivm_Arla_obv_481097.json</t>
         </is>
       </c>
       <c r="I95" t="inlineStr"/>
@@ -4131,19 +3719,15 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F96" t="inlineStr"/>
       <c r="G96" t="n">
         <v>0</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>tekst_CAO_01112010__01012012.json, CAO_Banken_2022.DefNL.json, NVB_CAO-boekje_2025_digitaal__redacted.json, NVB_CAO-boekje_2023_addendum.20240502.json, CAO__01012014_tot_01072014__CAO_tekst_14_jan_2014.json, NVB CAO-boekje 2021_14-04.json, NVB CAO-boekje 2023_digitaal-NL.json, CAO_Banken.json, OD18976_NVB CAO-boekje 2019_digitaal.pdf - CAO Banken_PDF digitaal NL versie.pdf .json, CAO_2017.json</t>
         </is>
       </c>
       <c r="I96" t="inlineStr"/>
@@ -4169,19 +3753,15 @@
         <v>17</v>
       </c>
       <c r="E97" t="n">
-        <v>0</v>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F97" t="inlineStr"/>
       <c r="G97" t="n">
         <v>0</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>ICK cao 2024-2025.json, ICK CAO 2022 v2.json, ICK-cao 2023.json, ICK CAO 2021_1.json, CAO 2019.json, ICK_CAO_2017.json, ICK-CAO 2018.pdf .json, ICK CAO 2021.json, ICK cao 2025-2026.json, Digitale_versie_ICK_CAO_2012.json, ICK_CAO_2016_definitief.json, Tekst_ICK_CAO_2011.json, ICK_CAO_2015___definitief.json, Definitieve_Tekst_ICK_CAO_2013_18_februari_2013_MV.json, Definitieve_tekst_ICK_CAO_2014_6_maart_2014.json, Cdef_ ICK CAO 2022.json, ICK CAO 2020_def.docx.json</t>
         </is>
       </c>
       <c r="I97" t="inlineStr"/>
@@ -4209,19 +3789,11 @@
       <c r="E98" t="n">
         <v>0</v>
       </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F98" t="inlineStr"/>
       <c r="G98" t="n">
         <v>0</v>
       </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr">
         <is>
@@ -4245,19 +3817,15 @@
         <v>18</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F99" t="inlineStr"/>
       <c r="G99" t="n">
         <v>0</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_pluimvee_per_1_januari_2017.json, Cao pluimvee - cao 2021-2023 versie 7-9-2021.json, Cao pluimvee - 2019 na ttw2 ivm wijziging art 28.pdf .json, CAO_pluimvee_per_1_januari_2017_per_13_2_2017.json, Pluimvee cao 2019.pdf .json, Cao pluimvee - 2019 na ttw3 ivm wijziging art 25.docx .json, CAO_pluimvee_per_1_januari_2017_per_9_2_2017.json, CAO_pluimvee_per_1_januari_2017_per_23_3_2018.json, Cao pluimvee - cao 2020-2021 na ttw2 art 77 .json, Cao pluimvee - cao 2020-2021 na ttw art 31 52 77 78 79 bijlage 3 .json, pluimvee - 2019 na ttw ivm wijziging art 55.pdf .json, Cao pluimvee - cao 2023-2025 def.json, CAO_pluimvee_per_1_januari_2017_per_19_4_2018.json, Cao pluimvee - cao 2020-2021 .json, Cao pluimvee na ttw - cao 2023-2025.json, CAO_pluimvee_per_1_mei_2012.json, CAO_pluimvee_per_1_mei_2013.json, Cao pluimvee 2023-2025 na ttw 9-4-2024 (incl. gewijzigd functiehandboek).json</t>
         </is>
       </c>
       <c r="I99" t="inlineStr"/>
@@ -4283,19 +3851,15 @@
         <v>12</v>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F100" t="inlineStr"/>
       <c r="G100" t="n">
         <v>0</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO Grondstoffen Energie en Omgeving Services 2022-2023-2024 - signed.json, Cao_GEO_PROCES_2018_2019.json, cao_GEO_vernieuwd_definitief.json, GEO_Cao.json, CAO GEO PROCES en SERVICES 2020.json, cao_afval_en_milieu_proces_2013_2014_met_handtek.json, cao_Afval_en_Milieu_Proces_2014_2015.json, Energiebedrijf_1471.json, Cao GEO SERVICES 2024-2026.json, Cao_Afval_en_Milieu_Proces_2016_2017.json, Cao 2022-2024 Proces - ondertekening.json, CAO Grondstoffen Energie en Omgeving PROCES 2021 20210503 ondertekend.json</t>
         </is>
       </c>
       <c r="I100" t="inlineStr"/>
@@ -4318,22 +3882,18 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F101" t="inlineStr"/>
       <c r="G101" t="n">
         <v>0</v>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Tuinzaadbedrijven 1 januari 2023 - 31 december 2023 definitief.json, Cao_Tuinzaadbedrijven_20180101___20191231.json, Afspraken cao Tuinzaadbedrijven 2020 versie definitief.json, Tekst CAO Tuinzaadbedrijven 1 januari 2024 - 31 december 2025 def.json, Plantum___CAO_2011____2014.json, Tuinzaadbedrijven 2021 - 2022 TTW augustus 2022.json, CAO_Tuinzaadbedrijven_1_jan_2018_tm_31_dec_2019.json, Plantum___definitieve_CAO_2011___2014.json, defintieve tekst CAO Tuinzaadbedrijven 2021 - 2022.json, Tuinzaadbedrijven 2021 - 2022 TTW2.json, CAO_Tuinzaden_2016_2017.json, Tuinzaden_cao_2014_2016.json, 2e__gem_t_t_w__1_10_2011___01_01_2014.json, Plantum_ttw_CAO_2011_2014.json</t>
         </is>
       </c>
       <c r="I101" t="inlineStr"/>
@@ -4356,22 +3916,18 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>294</v>
+        <v>2</v>
       </c>
       <c r="E102" t="n">
-        <v>1</v>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F102" t="inlineStr"/>
       <c r="G102" t="n">
         <v>1</v>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Goederenvervoer_Nederland_2012_2013.json, CAO_KNV_1_januari_2014__1_januari_2017.json</t>
         </is>
       </c>
       <c r="I102" t="n">
@@ -4399,19 +3955,15 @@
         <v>2</v>
       </c>
       <c r="E103" t="n">
-        <v>0</v>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F103" t="inlineStr"/>
       <c r="G103" t="n">
         <v>0</v>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Integrale CAO tekst.json, Tekst_Bioscoopbedrijf___aanmelding.json</t>
         </is>
       </c>
       <c r="I103" t="inlineStr"/>
@@ -4434,22 +3986,18 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E104" t="n">
-        <v>0</v>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F104" t="inlineStr"/>
       <c r="G104" t="n">
         <v>0</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>2024_31okt_tekstcaotbvavvschoon_MvD.json, 2022jun30_HWi_CAOtekst_1apr2022-31mrt2023_Cao-Aanmelden_exclCaoFondsOOA.json, 2024Mrt25_schonetekstcao.json, CAOtekst_2014_PvL_6mei2014.json, CAOtekst_1apr2019-31dec2019_PvL_6mei2019.pdf .json, CAOtekst_1apr2017_31mrt2019_PvL_30mei2018.json, 2021nov12_HWi_CAOtekst_1apr2020-31mrt2022.json, CAOtekst_2012_2013_PvL_5jun2012.json, 2024jan30_CAOHH2023-2024.json, CAOtekst_1apr2017_31mrt2019.json, 2020jan8_PvL_CAOtekst_1apr2019-31mrt2020.json, CAOtekst_2012_2013_PvL_26jul2012.json, 2020feb3_PvL_CAOtekst_1apr2019-31mrt2020.json, 2024_17dec_schone_tekstcaotbvavv_MvD4.json, 2025_14jan_schone_tekstcaotbvavv_MvD.json, 2021dec17_HWi_CAOtekst-tbv-Cao-aanmelden_1apr2020-31mrt2022_exclCaoFondsOOA_v2.d.json, CAOtekst_2015_31mrt2017_PvL_11sep2015.json</t>
         </is>
       </c>
       <c r="I104" t="inlineStr"/>
@@ -4472,22 +4020,18 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E105" t="n">
-        <v>0</v>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F105" t="inlineStr"/>
       <c r="G105" t="n">
         <v>0</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>20240725 CAO Particulier Kaaspakhuis 01-01-2024- 1-05-2025 wijzigingen bijgehouden.json, 20072021 CAO-boekje 2021-2022.json, CAO Particulier Kaaspakhuis 01-01-2024 definitief.json, CAO-tekst definitief.docx_1.json, CAO_tekst_integraal.json, CAO_tekst_definitief.json, CAO 2010-2012 tekst.json, CAO-tekst definitief.docx.json, CAO Particulier Kaaspakhuis 2023 versie 17-7-2023.json, CAO Particulier Kaaspakhuis 2023 na ttw versie 1-8-2023.json, CAOtekst_AVV__integraal_.json, CAOtekst_AVV__integraal__verlenging.json, CAO_tekst_integraal1.json, CAO-tekst 2021-2022 OKT schoon.json</t>
         </is>
       </c>
       <c r="I105" t="inlineStr"/>
@@ -4513,19 +4057,15 @@
         <v>13</v>
       </c>
       <c r="E106" t="n">
-        <v>0</v>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F106" t="inlineStr"/>
       <c r="G106" t="n">
         <v>0</v>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO visdetailhandel 2019-2020 definitieve versie aangeboden aan ministerie.docx .json, cao_tkst_AVV_na_gesprek_ministerie_1.json, Integrale cao-tekst visdetailhandel 2025 geschoond.json, CAO visdetailhandel 2021-2023 def voor ministerie na controle wg.json, Integrale cao-tekst visdetailhandel 2024 .json, Cao visdetailhandel 2025 tussentijdse wijzigingen juni 2025.json, Integrale cao-tekst visdetailhandel 2021-2023.json, Integrale cao-tekst visdetailhandel 2024 (definitieve versie 21 februari 2024).json, VNV_cao_boekje_A5_2015_408280_C.json, CAO_visdetailhandel_per_1__1__2015_org__getekend.json, cao_tkst_AVV_na_gesprek_ministerie.json, visdetailhandel cao en bijlagen.json, Cao_Visdetailhandel_2017_2018.json</t>
         </is>
       </c>
       <c r="I106" t="inlineStr"/>
@@ -4548,22 +4088,18 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E107" t="n">
-        <v>0</v>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F107" t="inlineStr"/>
       <c r="G107" t="n">
         <v>0</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>cao bb 2025-2026 def. 250617 zonder namen en handtekeningen.json, CAO_2015_2016_definitieve_tekst.json, Def. nieuwe tekst cao bb 2020 2021.docx.json, Integrale_tekst_CAO_BB_TTW.json, CAO_tekst_brochure_BB_1_1__2012_19_03__20122.json, CAO 1-1-2019 tm 31-12-2019 def tekst.docx .json, cao bb 2023-2024 integrale tekst definitief 230106.json, Tekst_CAO_BB_1_april_2013_tm_31_decb_2014.json, tekst_CAO_BB_2012_2013__versie_szw.json, FSO cao 2020 nieuwe tekst.doc.json, CAO_20_11_2016_tm_31_12_2018_correctie.json, Tekst_CAO_BB_1_4_13_tm_31_13.json</t>
         </is>
       </c>
       <c r="I107" t="inlineStr"/>
@@ -4589,19 +4125,15 @@
         <v>2</v>
       </c>
       <c r="E108" t="n">
-        <v>0</v>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F108" t="inlineStr"/>
       <c r="G108" t="n">
         <v>0</v>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>CAO_Slijterijen_2011_2013_integrale_tekst_def.json, Slijterijen 2010-2011 integrale tekst definitief.json</t>
         </is>
       </c>
       <c r="I108" t="inlineStr"/>
@@ -4627,19 +4159,15 @@
         <v>18</v>
       </c>
       <c r="E109" t="n">
-        <v>1</v>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F109" t="inlineStr"/>
       <c r="G109" t="n">
         <v>1</v>
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>HB 5e editie 2024_2.json, m_en_t_islollatiebedrijf_kvo.json, CAO_ISO_2017_2019__TTW.json, CAO ISO 2019 2021 SZW TTW V2 wagweu.docx.json, CAO_ISO_arcering___wijz_AOW_LT.json, CAO_ISO_17_19.json, CAO ISO 2021 2024_1.json, CAO ISO 2021 2024.json, HB 5e editie 2024.json, CAO_ISO_2017_2019__TTW_GP_nov_2017.json, CAO ISO 2021 2024b.json, M_T_Isolatie_Cao___Handboek.json, CAO_ISO_2017_2019__TTW_LL_nov_2018.json, CAO_ISO.json, CAO ISO 2019 2021 SZW TTW wagweu art 64.docx.json, Isolatie_cao_en_handboek.json, HB 5e editie 2024_1.json</t>
         </is>
       </c>
       <c r="I109" t="n">

</xml_diff>

<commit_message>
Refactor progress tracking and update script imports
- Removed unused scripts
- Adjusted the total row count in the extracted data analysis report to reflect the latest data.
</commit_message>
<xml_diff>
--- a/inputExcel/CAO_Frequencies_2014.xlsx
+++ b/inputExcel/CAO_Frequencies_2014.xlsx
@@ -503,15 +503,27 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -531,15 +543,27 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -559,17 +583,25 @@
       <c r="E4" t="n">
         <v>39</v>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G4" t="n">
         <v>39</v>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>ABU CAO voor Uitzendkrachten 2021 integraal.json, ABU-LBV CAO voor Uitzendkrachten 2021 integraal 7-22.json, Cao_integraal_1_7_2017.json, Cao_integraal_5_11_2017.json, Cao_integraal.json, ABU CAO voor Uitzendkrachten 2023 integraal 9-03-23.json, CAO_integrale_tekst.json, CAO_voor_uzk_14_10_2015_integraal.json, CAO_mei_2011_integraal.json, Cao_integraal_1_1_2019_integraal.json, CAO_1_november_integraal.json, ABU CAO voor Uitzendkrachten 2022 integraal.json, ABU CAO voor Uitzendkrachten 30-12-2019.json, ABU CAO voor Uitzendkrachten 2021 - 2023 versie juli 2022 integraal.json, CAO UZK januari 2011 integraal.json, ABU CAO voor Uitzendkrachten 2021 - 2023 versie januari 2023 met integraal.json, Cao_integraal_5_11_2017_1.json, ABU CAO voor Uitzendkrachten 2023 integraal_1.json, CAO_voor_uzk_16_9_2015_integraal.json, ABU CAO voor Uitzendkrachten 30-12-2019 integraal mei.json, ABU CAO voor Uitzendkrachten 2023 integraal.json, CAO_voor_Uitzendkrachten_dec__2012_integraal.json, CAO_voor_Uitzendkrachten_5_11_2012_integraal.json, ABU CAO voor Uitzendkrachten 30-12-2019 integraal 2020.doc.json, CAO_voor_Uitzendkrachten_juli_2013_integraal.json, CAO_voor_Uitzendkrachten_maart_2013_integraal.json, CAO_voor_Uitzendkrachten_1_4__2012_integraal.json, Cao voor Uitzendkrachten 2026-2028.json, CAO UZK april 2011 integraal.json, Uitzendkrachten_tekst.json, ABU CAO voor Uitzendkrachten 30-12-2019 integraal dec.json, Cao 1-7-2019 integraal.json, CAO_voor_Uitzendkrachten_integraal_1.json, CAO_voor_uzk_29_6_2015_integraal.json, ABU CAO voor Uitzendkrachten 1-1-2021 wijz. bijhouden.doc.json, CAO_voor_Uitzendkrachten_integraal.json, CAO_voor_uzk_29_12_14_integraal.json, Cao_integraal_1_7_2018.json, ABU CAO voor Uitzendkrachten 2024.json</t>
+          <t>ABU-LBV CAO voor Uitzendkrachten 2021 integraal 7-22.json, Cao_integraal_1_7_2017.json, Cao_integraal_5_11_2017.json, ABU CAO voor Uitzendkrachten 2023 integraal 9-03-23.json, CAO_integrale_tekst.json, CAO_voor_uzk_14_10_2015_integraal.json, CAO_mei_2011_integraal.json, Cao_integraal_1_1_2019_integraal.json, CAO_1_november_integraal.json, ABU CAO voor Uitzendkrachten 2022 integraal.json, ABU CAO voor Uitzendkrachten 30-12-2019.json, ABU CAO voor Uitzendkrachten 2021 - 2023 versie januari 2023 met integraal.json, Cao_integraal_5_11_2017_1.json, ABU CAO voor Uitzendkrachten 2023 integraal_1.json, ABU CAO voor Uitzendkrachten 2023 integraal.json, CAO_voor_Uitzendkrachten_dec__2012_integraal.json, CAO_voor_Uitzendkrachten_5_11_2012_integraal.json, ABU CAO voor Uitzendkrachten 30-12-2019 integraal 2020.doc.json, CAO_voor_Uitzendkrachten_juli_2013_integraal.json, CAO_voor_Uitzendkrachten_maart_2013_integraal.json, CAO_voor_Uitzendkrachten_1_4__2012_integraal.json, Cao voor Uitzendkrachten 2026-2028.json, CAO UZK april 2011 integraal.json, Uitzendkrachten_tekst.json, ABU CAO voor Uitzendkrachten 30-12-2019 integraal dec.json, Cao 1-7-2019 integraal.json, CAO_voor_Uitzendkrachten_integraal_1.json, CAO_voor_uzk_29_6_2015_integraal.json, CAO_voor_Uitzendkrachten_integraal.json, CAO_voor_uzk_29_12_14_integraal.json, Cao_integraal_1_7_2018.json, ABU CAO voor Uitzendkrachten 2024.json</t>
         </is>
       </c>
     </row>
@@ -591,17 +623,25 @@
       <c r="E5" t="n">
         <v>14</v>
       </c>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G5" t="n">
         <v>14</v>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>KHN_cao_2018_2019.json, 20200310 cao_horeca_2020_wijziging_op_kvo.docx.json, 20221124 cao_horeca_2022-2023 na 2020_wijziging bijlage loontabellen schoon.json, 202404~2.json, Horeca_CAO_.json, Horeca_cao__2018_2019_na_ttw.json, 20240103 cao_horeca_2024 - tussentijdse wijziging - schone versie.json, Cao Horeca 2025-2026 incl handboek.json, cao_horeca_2018_2019_na_ttw2.json, 20200101 cao_horeca_2020_wijziging_op_ttw2_schone versie.docx.json, 20220524 cao_horeca_2022-2023 na 2020_wijziging bijlage loontabellen schoon.json, 20220101 cao_horeca_2022-2023 na 2020_wijziging_op_kvo_avv versie bronbestand.do.json, 20131221 cao_horeca_2024 - schone versie.json, 20220520 cao_horeca_2022-2023 na 2020_wijziging mei-avv.json</t>
+          <t>KHN_cao_2018_2019.json, 20200310 cao_horeca_2020_wijziging_op_kvo.docx.json, Horeca_CAO_.json, Horeca_cao__2018_2019_na_ttw.json, 20240103 cao_horeca_2024 - tussentijdse wijziging - schone versie.json, Cao Horeca 2025-2026 incl handboek.json, cao_horeca_2018_2019_na_ttw2.json, 20200101 cao_horeca_2020_wijziging_op_ttw2_schone versie.docx.json, 20220524 cao_horeca_2022-2023 na 2020_wijziging bijlage loontabellen schoon.json, 20220101 cao_horeca_2022-2023 na 2020_wijziging_op_kvo_avv versie bronbestand.do.json, 20131221 cao_horeca_2024 - schone versie.json, 20220520 cao_horeca_2022-2023 na 2020_wijziging mei-avv.json</t>
         </is>
       </c>
     </row>
@@ -623,17 +663,25 @@
       <c r="E6" t="n">
         <v>7</v>
       </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G6" t="n">
         <v>7</v>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>CAO VGL 2024 tot en met 2026 .json, CAO VGL 2017-2019 v4 schoon 300418 incl loonschalen def. 090518.docx .json, VGL_Cao_2013___2017_getekend.json, VGL_cao_2011_2013_doorlopende_tekst_200212.json, CAO VGL 2019-2020 definitief schoon 010420.docx.json, 211229 CAO VGL 2020 tot en met 2023 met aangepaste loonschalen - 23-12-2021 V.json, 240105 VGL-cao 2023 tot en met 2024 met aangepaste loonschalen - DEF. (schoon).json</t>
+          <t>CAO VGL 2024 tot en met 2026 .json, CAO VGL 2017-2019 v4 schoon 300418 incl loonschalen def. 090518.docx .json, VGL_Cao_2013___2017_getekend.json, VGL_cao_2011_2013_doorlopende_tekst_200212.json, 211229 CAO VGL 2020 tot en met 2023 met aangepaste loonschalen - 23-12-2021 V.json, 240105 VGL-cao 2023 tot en met 2024 met aangepaste loonschalen - DEF. (schoon).json</t>
         </is>
       </c>
     </row>
@@ -655,15 +703,27 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -683,17 +743,25 @@
       <c r="E8" t="n">
         <v>9</v>
       </c>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G8" t="n">
         <v>9</v>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>CAO_ziekenhuizen_2017_2019_FINALDEF.json, NVZ CAO 2021 2023 schone versie.json, Cao Ziekenhuizen 2023-2025.json, NLVRZH067_CAO_Ziekenhuizen_14PM.json, CAO_Ziekenhuizen_totaal.json, NVZ CAO 2021 2023 schone versie compleet.json, Tekst_Cao_Ziekenhuizen_2011_2014_definitief.json, Ziekenhuizen_2011_2014_zonder_renvooi.json, CAO_ziekenhuizen_2017_2019_DEF.json</t>
+          <t>CAO_ziekenhuizen_2017_2019_FINALDEF.json, NVZ CAO 2021 2023 schone versie.json, Cao Ziekenhuizen 2023-2025.json, NLVRZH067_CAO_Ziekenhuizen_14PM.json, CAO_Ziekenhuizen_totaal.json, NVZ CAO 2021 2023 schone versie compleet.json, Ziekenhuizen_2011_2014_zonder_renvooi.json</t>
         </is>
       </c>
     </row>
@@ -715,17 +783,25 @@
       <c r="E9" t="n">
         <v>13</v>
       </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G9" t="n">
         <v>13</v>
       </c>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>CAO LMB 2019 - 2020 V 210220 def .docx.json, CAO LMB 2020 2023 schone versie feb 22.json, CAO_LMB_2013_2017_SZW_schoon_V3_20160530.json, CAO LMB incl fuwa 2020 2023 schone versie feb 22.json, CAO_LMB_2013_2017_SZW_schoon.json, CAO LMB incl fuwa 2023 - schoon getekend.json, Vakcentrum CAO 2024-2026 .json, CAO LMB 2020 2023 schone versie.json, levensmiddelensbedrijf_definitief.json, CAO LMB incl fuwa 2023 - schoon v 20231808 ongetekend.json, CAO_LMB_2013_2017_SZW_V4_schoon.json, CAO_LMB_2017____2019_def_01_02_2018_schone_versie.json, CAO LMB 2019 - 2020 V 210220 def.docx.json</t>
+          <t>CAO LMB 2019 - 2020 V 210220 def .docx.json, CAO_LMB_2013_2017_SZW_schoon_V3_20160530.json, CAO LMB incl fuwa 2020 2023 schone versie feb 22.json, CAO_LMB_2013_2017_SZW_schoon.json, CAO LMB incl fuwa 2023 - schoon getekend.json, Vakcentrum CAO 2024-2026 .json, CAO LMB 2020 2023 schone versie.json, levensmiddelensbedrijf_definitief.json, CAO LMB incl fuwa 2023 - schoon v 20231808 ongetekend.json, CAO_LMB_2017____2019_def_01_02_2018_schone_versie.json, CAO LMB 2019 - 2020 V 210220 def.docx.json</t>
         </is>
       </c>
     </row>
@@ -747,19 +823,23 @@
       <c r="E10" t="n">
         <v>28</v>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G10" t="n">
         <v>28</v>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>CAO 2021 definitief.json, CAO 2019-2021 definitief.docx.json, CAO 2022-2024 defintief_2.json, CAO 2022-2024 (met wijzigingen 6-7-2023).json, CAO 2024 (1-1-2024 tm 30-6-2024)_1.json, CAO_2017_2018_definitief.json, RAS_caotekst_2010_2011_aanmelding_20072011.json, CAO 2019 tot 2021 definitief.docx.json, CAO_2014_2016_2.json, CAO 2022-2024 defintief.json, CAO 2019 2021 definitief.docx.json, CAO_2017_2019_definitief.json, CAO 2021 definitief_1.json, CAO 2024 (1-1-2024 tm 30-6-2024).json, CAO_2017_2019_definitief___met_renvooi___20_7_2018.json, CAO_2014_2016.json, CAO_2017_2019_definitief_1.json, CAO 2024-2026 definitief met alle bijlagen cao.json, CAO.json, CAO 2019-2021 nota van wijziging 8-7-2019.docx.json, Schoonmaak__en_Glazenwassers_cao_stat__en_regl_.json, CAO 2024-2026 definitief met bijlagen.json, CAO 2024 (1-1-2024 tm 30-6-2024)_2.json, CAO_2014_2016_1.json, CAO 2022-2024 defintief_1.json, CAO 2019-2021 -definitief.docx .json, CAO 2022-2024 definitief 1 10 2022.json, schoonmaak_en_glazenwassersbedrijf.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -779,17 +859,25 @@
       <c r="E11" t="n">
         <v>18</v>
       </c>
-      <c r="F11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G11" t="n">
         <v>18</v>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Versie 20250114 Teksten CAO PO 2024-2025.json, Def CAO-PO 2023-2024 23012024.json, cao_po_2013_verlengd_2014_140107_handtek.json, 20180719_cao_po_2018_2019_def_getekend.json, 20160711_cao_po_2016_2017_versie_iia.json, 201600701_cao_po_2016_2017_DEFINITIEF_1_juli_2017.json, Def cao po 2021 schoon 6dec2021.json, 20190222_CAO_PO_2018_2019_gewijzigd_feb_2019.json, cao_po_2013_def_versie.json, 20141217_cao_po_2014_2015_tekenversie_REE_EvB_copy.json, 20170427_cao_po_opnieuw_gewijzigd_tbv_AVV_.json, CAO_Appo_en_GOVak_2018_2023.json, cao_po_2013_verlengd_2014_140107_handtek_1.json, CAO-PO 2023-2024.json, 20161230_cao_po_gewijzigd_per_1_jan_2017.json, Def cao 2019-2020 nav aanvullende afspraken .json, caopo2013_verlngd_handtek_april2014.json, Def cao primair onderwijs 2019-2020.json</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -811,15 +899,27 @@
       <c r="E12" t="n">
         <v>32</v>
       </c>
-      <c r="F12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G12" t="n">
         <v>32</v>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I12" t="n">
-        <v>416</v>
-      </c>
-      <c r="J12" t="inlineStr"/>
+        <v>400</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>TTW_CAO_2014_aanmelding_juli_2014.json, Bouw CAO 2011 aanmelding TTW 1-2011.json</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -839,19 +939,23 @@
       <c r="E13" t="n">
         <v>14</v>
       </c>
-      <c r="F13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G13" t="n">
         <v>14</v>
       </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Def_tekst_CAO_GHZ_2014_2015_vs20140709.json, CAO2021-2024_Augustus2023def_0_0.json, Tekst CAO GHZ 2021-2024_DEFGEW.json, gehandicaptenzorg integrale tekst.json, Tekst CAO GHZ 2021-2024 schone versie V2.json, CAO GHZ 2019-2021 versie oktober 2020 zonder wijzigingen bijhouden.docx.json, Tekst CAO Gehandicaptenzorg 2025-2026 (ID 161822).json, Tekst CAO GHZ 2021-2024.json, CAO GHZ 2019-2021 definitief zonder wijzigingen 20200107.docx.json, CAO_Gehandicaptenzorg_2017_2019_def.json, CAO Gehandicaptenzorg 2021-2024 tweede ronde.json, CAO_GHZ_2016_def_29_2_2016.json, CAO_Gehandicaptenzorg_2011_2014.json, Definitieve_tekst_CAO_GHZ_2014_2015.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -871,17 +975,25 @@
       <c r="E14" t="n">
         <v>18</v>
       </c>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G14" t="n">
         <v>18</v>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I14" t="n">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>CAO_MB_arcering___wijz_AOW_LT.json, CAO MB 2021 2024_1.json, HB 5e editie 2024_2.json, CAO_MB_17_19.json, CAO_MB_2017_2019_TTW_GP_nov_2017.json, MenT_Metaalbewerkingsbedr__CAO_tot_.json, HB 5e editie 2024.json, CAO_MB_2017_2019_TTW_juli_2017.json, CAO MB 2021 2024b.json, MT_Metaalbew__CAO___handb_.json, CAO_MB_2017_2019_TTW_LL_nov_2018.json, cao_mb_aangepast_n_a_v_bed.json, CAO_MB.json, CAO MB 2019 2021SZW TTW V2 Wagweu.docx.json, CAO MB 2021 2024.json, CAO_MB_TTW_juli.json, HB 5e editie 2024_1.json</t>
+          <t>CAO_MB_arcering___wijz_AOW_LT.json, CAO MB 2021 2024_1.json, HB 5e editie 2024_2.json, CAO_MB_17_19.json, CAO_MB_2017_2019_TTW_GP_nov_2017.json, MenT_Metaalbewerkingsbedr__CAO_tot_.json, HB 5e editie 2024.json, CAO_MB_2017_2019_TTW_juli_2017.json, CAO MB 2021 2024b.json, MT_Metaalbew__CAO___handb_.json, cao_mb_aangepast_n_a_v_bed.json, CAO MB 2019 2021SZW TTW V2 Wagweu.docx.json, CAO MB 2021 2024.json, HB 5e editie 2024_1.json</t>
         </is>
       </c>
     </row>
@@ -903,15 +1015,27 @@
       <c r="E15" t="n">
         <v>14</v>
       </c>
-      <c r="F15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G15" t="n">
         <v>14</v>
       </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I15" t="n">
         <v>263</v>
       </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -931,19 +1055,23 @@
       <c r="E16" t="n">
         <v>37</v>
       </c>
-      <c r="F16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G16" t="n">
         <v>37</v>
       </c>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>cao_2014_2016_aanmelding.json, CAO VVT 2022-2024 verlengde cao ttw2.json, CAO_VVT_2016_2018_def.json, CAO VVT 2022-2023 ttwnov22b.json, CAO VVT 2022-2023 ttwnov22c.json, cao_VVT_tot_1_januari_2015.json, CAO VVT 2025-2026_versie april 2025.json, CAO VVT 2022-2023 ttwnov22.json, cao_2018.json, CAO_VVT_2010_2012_2_.json, gewijzigde_cao_2016_2018.json, CAO VVT 2022-2024 verlengde cao def.json, CAO_VVT_2010_2012_nieuwe_aanmelding_okt_.json, cao 2019-2021 .docx.json, cao_VVT_2018_2019.json, CAO VVT 2022-2024 verlengde cao ttw.json, CAO 2021 aanmelding_1.json, CAO VVT 2022-2023 tussentijdse wijziging.json, cao 2019-2021 tussentijdse wijziging .docx.json, CAO VVT 2022-2023 ttw april23.json, gewijzigde_cao_2016_2018_artikel_1_1_.json, cao 2019-2021 tussentijdse wijziging versie 18 febr.docx.json, CAO VVT 2022-2023 ttwnov.json, CAO 2021 aanmelding.json, gewijzigde_cao_VVT.json, cao 2019-2021 tussentijdse wijziging.docx.json, cao_teksten_2013_2014_aanmelding.json, CAO VVT 2025-2026_TTW 1.json, cao_t_b_v__avv2.json, wijziging_art_1_1__cao_aanmelding.json, cao_VVT.json, CAO_VVT_2012_2013_docx.json, Tekst_aanmelding_CAO_VVT_2013_2014.json, CAO VVT 2022-2023 aanmelding.json, CAO VVT 2022-2023 ttwnov22a.json, gewijzigde_cao_2016_2018_artikel_12_2.json, CAO VVT 2022-2024 verlengde cao ttw_1.json</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -963,17 +1091,25 @@
       <c r="E17" t="n">
         <v>16</v>
       </c>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G17" t="n">
         <v>16</v>
       </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>CAO_Metalektro_2013_2015_Basis.json, Cao Basis 2022-2024 dd 25-1.json, Basis_CAO_Metalektro_versie_voor_website.json, Basis_CAO_Metalektro_2011_2013_1.json, Basis_CAO_ME_2011_2013__versie_121008.json, Basis_CAO_Metalektro_2011_2013.json, Basis-cao Metalektro aanmelding ttw 21-8-19.docx.json, Cao Basis def. versie 15-7-24 markeringen en statuten.json, Basis 20-22 aanmelding 18-1-22.json, Cao Basis schone versie 9-9-2024 en statuten.json, Cao Basis schone versie 09-12-2024 en statuten.json, Cao Basis def. versie 29-11-22 met statuten ROM en SSF.json, CAO_Metalektro_Basis__met_statuten_.json, Basis-cao Metalektro hertaald - def. versie schoon 23-7-19OB.docx.json, Def. versie aanmelding 15-11 Basis-cao Metalektro 20-22.json, Basis_CAO_Metalektro_met_statutenfondsen.json</t>
+          <t>CAO_Metalektro_2013_2015_Basis.json, Cao Basis 2022-2024 dd 25-1.json, Basis_CAO_Metalektro_versie_voor_website.json, Basis_CAO_Metalektro_2011_2013_1.json, Basis_CAO_ME_2011_2013__versie_121008.json, Basis_CAO_Metalektro_2011_2013.json, Basis-cao Metalektro aanmelding ttw 21-8-19.docx.json, Cao Basis def. versie 15-7-24 markeringen en statuten.json, Basis 20-22 aanmelding 18-1-22.json, Cao Basis schone versie 9-9-2024 en statuten.json, Cao Basis def. versie 29-11-22 met statuten ROM en SSF.json, CAO_Metalektro_Basis__met_statuten_.json, Basis-cao Metalektro hertaald - def. versie schoon 23-7-19OB.docx.json, Def. versie aanmelding 15-11 Basis-cao Metalektro 20-22.json, Basis_CAO_Metalektro_met_statutenfondsen.json</t>
         </is>
       </c>
     </row>
@@ -995,21 +1131,25 @@
       <c r="E18" t="n">
         <v>25</v>
       </c>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G18" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>NBBU-cao voor uitzendkrachten per 1 juni 2021 def ondertekend.json</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>definitieve_cao_tekst.json, NBBU cao voor uitzendkrachten - 30122019 - DEFINITIEF.doc.json, Cao_uzk_1_7_2016.json, NBBU_CAO_Uitzendkrachten-NL 2023 def..json, NBBU_CAO_uitzendkrachten_2017.json, NBBU_CAO_Uitzendkrachten-NL 2024.def.json, NBBU cao tussentijdse wijzigingen januari 2023.json, NBBU cao per 1-1-2022 defintief wijziging accept.json, NBBU_Uitzendkrachten_1060.json, NBBU Cao UK 2009-2013 SZW niet gemarkeerd.json, NBBU_CAO_Uitzendkrachten_2016_V3.json, 2180679_NBBU_CAO_Uitzendkrachten_2018_OTFp.json, NBBU_CAO_Uitzendkrachten_2015_per_1_juli_DEF.json, NBBU_CAO_Uitzendkrachten_2015-2019_versie 2019 NL OTF.pdf .json, NBBUCAO_wijzigingen_geaccepteerd_SZW.json, Cao uitzendkrachten LBV onwerkbaar weer dec 2021 wijzigingen geaccpteerd.json, c1032_f9599_fp2852_2011654_NBBU_Uitzend_versie_2.json, NBBU_CAO_Uitzendkrachten 2015-2019_versie 2019 NL OTF.docx.json, NBBU cao tussentijdse wijzigingen def.json, NBBU_CAO_Uitzendkrachten-NL_2021.json, NBBU_CAO_Uitzendkrachten_2015.json, NBBU_CAO_Uitzendkrachten-NL_JUN 2023_v1.json, NBBU_CAO_Uitzendkrachten_2018.json, NBBU_CAO_Uitzendkrachten_2015_2019_def_.json</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -1031,15 +1171,27 @@
       <c r="E19" t="n">
         <v>0</v>
       </c>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I19" t="n">
         <v>0</v>
       </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1059,17 +1211,25 @@
       <c r="E20" t="n">
         <v>9</v>
       </c>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G20" t="n">
         <v>9</v>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>CAO PDF DEF.json, CAO VO 2023-2024 (def 14.12.23).json, CAO VO 2022 2023 spreads def voor aanmelding SZW (nov 22).json, CAO_VO_2014__2015.json, CAO VO 2024 2025 zonder handtekeningen en namen (tbv aanmelding) PDF.json, CAO_VO_2018_2019_voor_aanmelding_SZW.json, CAO_VO_2016_2017_ondertekend_DEFPDF.json, VOR_CAO_web_2020_03 beveiligd.json, CAO_VO_2011_2012_def.json</t>
+          <t>CAO VO 2023-2024 (def 14.12.23).json, CAO VO 2022 2023 spreads def voor aanmelding SZW (nov 22).json, CAO_VO_2014__2015.json, CAO VO 2024 2025 zonder handtekeningen en namen (tbv aanmelding) PDF.json, CAO_VO_2018_2019_voor_aanmelding_SZW.json, CAO_VO_2016_2017_ondertekend_DEFPDF.json, VOR_CAO_web_2020_03 beveiligd.json</t>
         </is>
       </c>
     </row>
@@ -1091,17 +1251,25 @@
       <c r="E21" t="n">
         <v>11</v>
       </c>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G21" t="n">
         <v>11</v>
       </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>cao ggz tekst 05-02-2024.json, GGZ cao met wijziging salarisschaal.json, Word_werkbestand_CAO_GGZ_2017_2019.json, Tekst_CAO_GGZ_2011_2013_juli_2012.json, GGZ_CAOgids_gewijzigd3dec2015.json, CAO_GGZ_2015_2017.json, tekst CAO GGZ 2021-2024.json, cao 2019-2021 min SZW.json, Werkversie_CAO_GGZ_2011.json, GGZ1504_01_binnenwerkCAOgids.json, Wijzigingen CAO GGZ 2019-2021 excl bijlage VI - 31 december 2020 definitief.docx.json</t>
+          <t>cao ggz tekst 05-02-2024.json, GGZ cao met wijziging salarisschaal.json, Word_werkbestand_CAO_GGZ_2017_2019.json, Tekst_CAO_GGZ_2011_2013_juli_2012.json, GGZ_CAOgids_gewijzigd3dec2015.json, CAO_GGZ_2015_2017.json, tekst CAO GGZ 2021-2024.json, cao 2019-2021 min SZW.json, Werkversie_CAO_GGZ_2011.json, GGZ1504_01_binnenwerkCAOgids.json</t>
         </is>
       </c>
     </row>
@@ -1123,13 +1291,17 @@
       <c r="E22" t="n">
         <v>7</v>
       </c>
-      <c r="F22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G22" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Web-versie-SW-CAO-boekje-2021-2025.json</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -1137,7 +1309,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>130214_gehelecao1_versienatosw_4_AP.json, Tekst Cao SW 2020.json, 20191208_Cao tekst 2019.docx.json, 20211015__Tekst Cao SW 2021-2025_def.json, cao sociale werkvoorziening.json</t>
+          <t>130214_gehelecao1_versienatosw_4_AP.json, Tekst Cao SW 2020.json, Web-versie-SW-CAO-boekje-2021-2025.json, 20191208_Cao tekst 2019.docx.json, 20211015__Tekst Cao SW 2021-2025_def.json, cao sociale werkvoorziening.json</t>
         </is>
       </c>
     </row>
@@ -1159,17 +1331,25 @@
       <c r="E23" t="n">
         <v>18</v>
       </c>
-      <c r="F23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G23" t="n">
         <v>18</v>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>HB 5e editie 2024_2.json, CAO_TI_arcering___wijz_AOW_LT.json, CAO_TI_deel.json, CAO TI 2019 2021 TTW V2 Wagweu.docx.json, CAO TI 2021 2024.json, M_en_T_Technisch_Installatiebedrijf_cao_en_handb_.json, CAO_TI_2017_2019_TTW_LL_nov_2018.json, CAO TI 2021 2024_1.json, CAO_TI_2017_2019_TTW_juli_2017.json, HB 5e editie 2024.json, CAO_TI_2011_2013_incl_wijz_4c_aangepast_n_a_v_bed.json, MenT_Technisch_Install_tot_cao_2297.json, c2255_f14208_fp3241_CAO_TI_17_19_arcering.json, CAO TI 2019 2021 TTW Wagweu en art 64 .docx.json, CAO TI 2021 2024b.json, CAO_TI_2017_2019_TTW_GP_nov_2017.json, CAO_TI_TTW_juli.json, HB 5e editie 2024_1.json</t>
+          <t>HB 5e editie 2024_2.json, CAO_TI_arcering___wijz_AOW_LT.json, CAO_TI_deel.json, CAO TI 2019 2021 TTW V2 Wagweu.docx.json, CAO TI 2021 2024.json, M_en_T_Technisch_Installatiebedrijf_cao_en_handb_.json, CAO_TI_2017_2019_TTW_LL_nov_2018.json, CAO TI 2021 2024_1.json, CAO_TI_2017_2019_TTW_juli_2017.json, HB 5e editie 2024.json, CAO_TI_2011_2013_incl_wijz_4c_aangepast_n_a_v_bed.json, MenT_Technisch_Install_tot_cao_2297.json, CAO TI 2019 2021 TTW Wagweu en art 64 .docx.json, CAO TI 2021 2024b.json, CAO_TI_TTW_juli.json, HB 5e editie 2024_1.json</t>
         </is>
       </c>
     </row>
@@ -1191,17 +1371,25 @@
       <c r="E24" t="n">
         <v>36</v>
       </c>
-      <c r="F24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G24" t="n">
         <v>36</v>
       </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cao_Fashion_en_Sport_Inretail.json, 230418 cao Retail Non-Food def.json, 171115_Cao_F_S__L_2016_2018_definitief_hvb_2.json, 170118_Cao_F_S__L_2016_2018_hvb.json, cao_Mode__Sport_1_7_2010_tot_1_7_2012.json, 220629 cao Retail Non-Food def.json, 220208 cao Retail Non-Food schone versie.json, 221214 cao Retail Non-Food schone versie.json, 230630 cao Retail Non-Food def.json, 150824_Cao_Fashion__Sport_en_Lifestyle.json, 211130 Cao Retail Non-Food 1-1-2022 def..json, 210805 Cao Retail Non-Food 1-7-21 def.json, Cao_Fashion_en_Sport_Inretail_21_8_2013.json, cao_Mode__Sport_1_7_2010_tot_1_7_2012_22_8_2011.json, 190730 cao Retail Non-Food per 1 juli 2019 definitief.docx.json, 241218 Cao Retail Non-Food jan 2025 definitief.json, 190730 cao Retail Non-Food per 1 juli 2019.docx.json, 250617 Cao Retail Non-Food juli 2025 def.json, 150824_Cao_Fashion__Sport___Lifestyle_hvb.json, 240206 cao Retail Non-Food def..json, 170313_Cao_F_S__L_2016_2018_incl_Wonen_def_hvb.json, 201207 Cao Retail Non-Food 1-1-21 definitief.docx.json, 180921_cao_Retail_Non_Food_definitief_hvb.json, 191227 cao Retail Non-Food per 1 januari 2020 definitief.docx.json, 170214_Cao_F_S__L_2016_2018_hvb.json, 210811 Cao Retail Non-Food 1-7-21 def.json, 240508 Cao Retail Non-Food definitief.json, 151020_Cao_Fashion__Sport___Lifestyle_hvb.json, 170630_Cao_F_S__L_2016_2018_definitief_hvb.json, 210128 Cao Retail Non-Food 1-1-21 definitief.docx.json, 190128_cao_Retail_Non_Food_definitief_hvb_bg.json, 240625 Cao Retail Non-Food definitief.json, 171115_Cao_F_S__L_2016_2018_definitief_hvb_1.json, 160715_Cao_F__S___L_2016_2018_gewijzigd_hvb.json, 171115_Cao_F_S__L_2016_2018_definitief_hvb.json, 161031_Cao_F_S__L_2016_2018_hvb.json</t>
+          <t>Cao_Fashion_en_Sport_Inretail.json, 230418 cao Retail Non-Food def.json, 171115_Cao_F_S__L_2016_2018_definitief_hvb_2.json, 170118_Cao_F_S__L_2016_2018_hvb.json, cao_Mode__Sport_1_7_2010_tot_1_7_2012.json, 220208 cao Retail Non-Food schone versie.json, 221214 cao Retail Non-Food schone versie.json, 211130 Cao Retail Non-Food 1-1-2022 def..json, 210805 Cao Retail Non-Food 1-7-21 def.json, cao_Mode__Sport_1_7_2010_tot_1_7_2012_22_8_2011.json, 190730 cao Retail Non-Food per 1 juli 2019 definitief.docx.json, 241218 Cao Retail Non-Food jan 2025 definitief.json, 190730 cao Retail Non-Food per 1 juli 2019.docx.json, 250617 Cao Retail Non-Food juli 2025 def.json, 150824_Cao_Fashion__Sport___Lifestyle_hvb.json, 240206 cao Retail Non-Food def..json, 180921_cao_Retail_Non_Food_definitief_hvb.json, 191227 cao Retail Non-Food per 1 januari 2020 definitief.docx.json, 170214_Cao_F_S__L_2016_2018_hvb.json, 210811 Cao Retail Non-Food 1-7-21 def.json, 240508 Cao Retail Non-Food definitief.json, 151020_Cao_Fashion__Sport___Lifestyle_hvb.json, 170630_Cao_F_S__L_2016_2018_definitief_hvb.json, 210128 Cao Retail Non-Food 1-1-21 definitief.docx.json, 190128_cao_Retail_Non_Food_definitief_hvb_bg.json, 240625 Cao Retail Non-Food definitief.json, 160715_Cao_F__S___L_2016_2018_gewijzigd_hvb.json, 171115_Cao_F_S__L_2016_2018_definitief_hvb.json, 161031_Cao_F_S__L_2016_2018_hvb.json</t>
         </is>
       </c>
     </row>
@@ -1223,17 +1411,25 @@
       <c r="E25" t="n">
         <v>16</v>
       </c>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G25" t="n">
         <v>16</v>
       </c>
-      <c r="H25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2025-07-01 CAO MVT 2025 - 2027 - incl HFI DEF.json, Concept cao MVT - incl HFI DEF.json, CAO MvT 2020-2021 DEFversie 19 januari 2021.docx.json, CAO_MvT_2014_2018_11_september.json, CAO_tekst_2011_2012_compleet_versie_2_augustus.json, Cao MVT - incl HFI 8 juni 2022.json, CAO_tekst_2011_2012_compleet_versie_19_juli.json, Cao MVT - incl HFI 31 januari 2024.json, CAO MvT 2020-2021 versie 23 dec 2020.docx.json, CAO MvT 2018-2020 DEF 2 oktober 2019.docx.json, Cao MVT - zonder HFI DEF 6 feb 2023.json, 2024-04 Cao MVT 2023 - 2025 - incl HFI vs 2.json, CAO MvT 2018-2020 DEF 29 mei19.docx .json, CAO_tekst_2012_2014_definitief.json, CAO_tekst_2011_2012_compleet_versie_28_juli.json, CAO_MvT_2014_2018_29_november_2016.json</t>
+          <t>2025-07-01 CAO MVT 2025 - 2027 - incl HFI DEF.json, Concept cao MVT - incl HFI DEF.json, CAO MvT 2020-2021 DEFversie 19 januari 2021.docx.json, CAO_tekst_2011_2012_compleet_versie_2_augustus.json, Cao MVT - incl HFI 8 juni 2022.json, Cao MVT - incl HFI 31 januari 2024.json, CAO MvT 2020-2021 versie 23 dec 2020.docx.json, Cao MVT - zonder HFI DEF 6 feb 2023.json, 2024-04 Cao MVT 2023 - 2025 - incl HFI vs 2.json, CAO MvT 2018-2020 DEF 29 mei19.docx .json, CAO_MvT_2014_2018_29_november_2016.json</t>
         </is>
       </c>
     </row>
@@ -1255,19 +1451,23 @@
       <c r="E26" t="n">
         <v>10</v>
       </c>
-      <c r="F26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G26" t="n">
         <v>10</v>
       </c>
-      <c r="H26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Cao_umc_2013___2015_officiele_tekst.json, Officiele_versie_NL_Cao_UMC_2011_2013.json, SZW_15_14272_Cao_umc_2015_2017.json, Cao umc 2018-2020 def versie maart 2019.pdf .json, 19.9945 Umcs Cao umc 2018-2020 per 1-1-2020.json, 15_11628_Cao_umc_2015_2017_DEF.json, Cao_umc_2015_2017_versie_8_2017.json, Cao UMC wijzigingen per januari 2023.json, Cao umc 2022 2023 pdf.json, NFU-24.01131 CAO NL v08 def.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1287,17 +1487,25 @@
       <c r="E27" t="n">
         <v>21</v>
       </c>
-      <c r="F27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G27" t="n">
         <v>21</v>
       </c>
-      <c r="H27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Integrale Cao Kinderopvang 2021-2022.json, CAO_Kinderopvang_difi.json, CAOKINDEROPVANG 1011 (ttw160311).json, Integrale cao Kinderopvang 2020 - 2021 - gewijzigd.json, Integrale Cao Kinderopvang 2025-2026.json, CAO_Kinderopvang_2012_2014_basistekst060214.json, CAO_Kinderopvang.json, Integrale Cao Kinderopvang 2021-2022 - 280721.json, CAO_Kinderopvang_2012_2014_aanmeld150813.json, Integrale Cao Kinderopvang 2024.json, CAO_Kinderopvang_2012_2014_basistekst101114.json, CAO_Kinderopvang_2012_2014_def.json, CAO_Kinderopvang_2018_2019.json, CAO_Kinderopvang_2016_2017.json, Integrale Cao Kinderopvang 2024 16-07-2024.json, Integrale gewijzigde Cao Kinderopvang 2023-2024.json, Integrale Cao Kinderopvang 2023-2024.json, Integrale gewijzigde cao Kinderopvang 2020-2021 (schone versie).docx.json, Integrale Cao Kinderopvang 2023-2024 (21-12-2023).json, Integrale cao Kinderopvang 2020 - 2021.json, Integrale Cao Kinderopvang 2024 20-12-2024.json</t>
+          <t>Integrale Cao Kinderopvang 2021-2022.json, CAO_Kinderopvang_difi.json, CAOKINDEROPVANG 1011 (ttw160311).json, Integrale Cao Kinderopvang 2025-2026.json, CAO_Kinderopvang_2012_2014_basistekst060214.json, Integrale Cao Kinderopvang 2021-2022 - 280721.json, CAO_Kinderopvang_2012_2014_aanmeld150813.json, CAO_Kinderopvang_2018_2019.json, CAO_Kinderopvang_2016_2017.json, Integrale Cao Kinderopvang 2024 16-07-2024.json, Integrale gewijzigde Cao Kinderopvang 2023-2024.json, Integrale Cao Kinderopvang 2023-2024.json, Integrale Cao Kinderopvang 2023-2024 (21-12-2023).json</t>
         </is>
       </c>
     </row>
@@ -1319,17 +1527,25 @@
       <c r="E28" t="n">
         <v>26</v>
       </c>
-      <c r="F28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G28" t="n">
         <v>26</v>
       </c>
-      <c r="H28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cao Sociaal Werk 2021-2023_definitief231122.json, Cao Sociaal Werk 2021 2023_280422definitief.json, CAO W&amp;MD 2008-2012 compleet 10_3.json, caosociaalwerk20172019_def191017_inclfuboek.json, welzijn_en_maatschappelijke__tekst.json, CAO_W_MD_2008_2012_AVV_zichtb_renv_17_05_2011.json, CAOWMD20082011aanmelding2012.json, CAOWMD1213__270213__definitief.json, CAOWMD20142016_definitief_301214_.json, Cao Sociaal Werk 2023-2025(ttw031224opttw010724)definitief.json, CAOSOCIAALWERK1921definitief_030120.json, CAOWMD20142016_ttw220615_definitiefgewijzigd.json, CAO_WMD_2008_2011_aanmeldversie.json, Cao Sociaal Werk 2023-2025(gewijzigdper091023).json, Cao Sociaal Werk 2023-2025(gewijzigdper091023)def.json, CAOSOCIAALWERK1921gewijzigdivmpsz_290720_def.json, CAOWMD_VERLENGING_2012_ttw_ivm_avv.json, CAOWMD_2012_TTW_ivm_AOW_datum.json, Cao Sociaal Werk 2023-2025(metcorrectie150224).json, CAOWMD_aanmelding_VERLENGING_2012_ttw_ivm_avv.json, Cao Sociaal Werk 2023-2025(definitief_tussentijdsgewijzigdper010724).json, Cao Sociaal Werk 2023-2025(definitief240723)def.json, welzijn_maatschappelijk_dienstverlenning.json, CAOSOCIAALWERK1719_070218__ttw_corr_avv_def.json, CAOSOCIAALWERK1719_completetekst_def_030419schoon.docx .json, ttwnov15_CAOWMD1416_def_exb2b15_wijzws_151215_def.json</t>
+          <t>Cao Sociaal Werk 2021-2023_definitief231122.json, CAO W&amp;MD 2008-2012 compleet 10_3.json, caosociaalwerk20172019_def191017_inclfuboek.json, welzijn_en_maatschappelijke__tekst.json, CAO_W_MD_2008_2012_AVV_zichtb_renv_17_05_2011.json, CAOWMD20142016_ttw220615_definitiefgewijzigd.json, CAO_WMD_2008_2011_aanmeldversie.json, Cao Sociaal Werk 2023-2025(gewijzigdper091023).json, Cao Sociaal Werk 2023-2025(gewijzigdper091023)def.json, CAOSOCIAALWERK1921gewijzigdivmpsz_290720_def.json, CAOWMD_VERLENGING_2012_ttw_ivm_avv.json, CAOWMD_2012_TTW_ivm_AOW_datum.json, Cao Sociaal Werk 2023-2025(metcorrectie150224).json, Cao Sociaal Werk 2023-2025(definitief_tussentijdsgewijzigdper010724).json, welzijn_maatschappelijk_dienstverlenning.json, CAOSOCIAALWERK1719_070218__ttw_corr_avv_def.json, CAOSOCIAALWERK1719_completetekst_def_030419schoon.docx .json, ttwnov15_CAOWMD1416_def_exb2b15_wijzws_151215_def.json</t>
         </is>
       </c>
     </row>
@@ -1351,17 +1567,25 @@
       <c r="E29" t="n">
         <v>13</v>
       </c>
-      <c r="F29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G29" t="n">
         <v>13</v>
       </c>
-      <c r="H29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>CAO_2011_2014_def.json, CAO Nederlandse Universiteiten 31 december 2019 tm 31 december 2020.json, Cao Nederlandse Universiteiten 1 juli 2017 - 31 december 2019.pdf .json, CAO NU 1 juli 2024 - 30 juni 2025 eerste webversie.json, Collectieve Arbeids Overeenkomst 1 januari - 31 december 2020 webversie CAO NU.p.json, 16066-12 VSNU-CAO Nederlandse Universiteiten 2020.json, CAO NU 20222-2023 definitieve tekst schoon.json, VSNU-CAO Nederlandse Universiteiten 2021-2022-NL definitieve versie 10-11-21.json, Ned_Universiteiten_1536.json, CAONU_1_januari_2015___1_juli_2016.json, CAONU_1_januari_2015___1_juli_2016_1.json, CAO_NU_2_juli_2016___30_juni_2017.json, CAO NU 2023-2024 definitief.json</t>
+          <t>CAO_2011_2014_def.json, CAO Nederlandse Universiteiten 31 december 2019 tm 31 december 2020.json, Cao Nederlandse Universiteiten 1 juli 2017 - 31 december 2019.pdf .json, CAO NU 1 juli 2024 - 30 juni 2025 eerste webversie.json, Collectieve Arbeids Overeenkomst 1 januari - 31 december 2020 webversie CAO NU.p.json, CAO NU 20222-2023 definitieve tekst schoon.json, VSNU-CAO Nederlandse Universiteiten 2021-2022-NL definitieve versie 10-11-21.json, Ned_Universiteiten_1536.json, CAONU_1_januari_2015___1_juli_2016.json, CAONU_1_januari_2015___1_juli_2016_1.json, CAO_NU_2_juli_2016___30_juni_2017.json, CAO NU 2023-2024 definitief.json</t>
         </is>
       </c>
     </row>
@@ -1383,17 +1607,25 @@
       <c r="E30" t="n">
         <v>15</v>
       </c>
-      <c r="F30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G30" t="n">
         <v>15</v>
       </c>
-      <c r="H30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>CAO MBO 2022-2023.json, CAO MBO 2022-2023 in Word - addendum schone versie 22022023.json, CAO_MBO_2016_2017____Nieuwe_versie_25042018.json, CAO_MBO_2018_2020_in_Word.json, CAO MBO 2023-2024.json, Beroepsonderwijs_en_Volwasseneneducatie_BVE_1022.json, CAO_MBO_2016_2017_definitief.json, cao_mbo_2014_singlepage_def.json, CAO MBO 2021-2022 - wijzigingen doorgevoerd 17122021.json, CAO MBO 2021 - wijzigingen geaccepteerd 09072021.json, CAO_MBO_2016_2017___Nieuwe_versie.json, CAO MBO 2024.json, CAO MBO 2020-2021 - wijzigingen geaccepteerd 29062020 def.json, CAO MBO 2018-2020 - wijzigingen geaccepteerd 712020.json, CAO_MBO_2014_2015_in_Word___nieuwe_versie.json</t>
+          <t>CAO MBO 2022-2023.json, CAO MBO 2022-2023 in Word - addendum schone versie 22022023.json, CAO_MBO_2016_2017____Nieuwe_versie_25042018.json, CAO_MBO_2018_2020_in_Word.json, CAO MBO 2023-2024.json, Beroepsonderwijs_en_Volwasseneneducatie_BVE_1022.json, CAO_MBO_2016_2017_definitief.json, cao_mbo_2014_singlepage_def.json, CAO MBO 2021-2022 - wijzigingen doorgevoerd 17122021.json, CAO MBO 2021 - wijzigingen geaccepteerd 09072021.json, CAO_MBO_2016_2017___Nieuwe_versie.json, CAO MBO 2024.json, CAO_MBO_2014_2015_in_Word___nieuwe_versie.json</t>
         </is>
       </c>
     </row>
@@ -1415,21 +1647,25 @@
       <c r="E31" t="n">
         <v>27</v>
       </c>
-      <c r="F31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G31" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>cao tekst .json</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>235</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>BAKKERSBEDRIJF_cao.json, 01_CAO_BAKKERSBEDRIJF_1_MAART_2012.json, cao Bakkersbedrijf, definitief versie 03062024 (5).docx.json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016.json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016_1.json, 01_CAO_BAKKERSBEDRIJF_1_AUGUSTUS_2011_1.json, Cao Bakkersbedrijf 1 juni 2021 - 1 juni 2023 definitief 08072022.json, 01 CAO BAKKERSBEDRIJF 1 APRIL 2019.docx .json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2014.json, Cao Bakkersbedrijf 1 juni 2021 - 1 juni 2023 definitief 12082022.json, cao Bakkersbedrijf definitief versie 15082024.json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2015.json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2015_1.json, CAO BAKKERSBEDRIJF 1 AUGUSTUS 2020 incl Bijlagen.docx.json, Cao Bakkersbedrijf 1 juni 2021 - 1 juni 2023 definitief 25072022.json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016_2.json, BAKKERSBEDRIJF_1_AUGUSTUS_2011_incl_bijlagen.json, 01_CAO_BAKKERSBEDRIJF_1_AUGUSTUS_2011.json, CAO BAKKERSBEDRIJF 1 AUGUSTUS 2020 incl Bijlagen_1.json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016___def_.json, 01_CAO_BAKKERSBEDRIJF_1_MAART_2012___definitief.json, BAKKERSBEDRIJF_cao_tekst_en_bijlagen.json, CAO BAKKERSBEDRIJF 1 AUGUSTUS 2020 incl Bijlagen.json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2014_1.json, CAO tekst.json, cao Bakkersbedrijf, definitief versie 26072024.json</t>
+          <t>01_CAO_BAKKERSBEDRIJF_1_MAART_2012.json, cao Bakkersbedrijf, definitief versie 03062024 (5).docx.json, cao tekst .json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016.json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016_1.json, 01_CAO_BAKKERSBEDRIJF_1_AUGUSTUS_2011_1.json, Cao Bakkersbedrijf 1 juni 2021 - 1 juni 2023 definitief 08072022.json, 01 CAO BAKKERSBEDRIJF 1 APRIL 2019.docx .json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2014.json, Cao Bakkersbedrijf 1 juni 2021 - 1 juni 2023 definitief 12082022.json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2015.json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2015_1.json, Cao Bakkersbedrijf 1 juni 2021 - 1 juni 2023 definitief 25072022.json, CAO BAKKERSBEDRIJF 1 AUGUSTUS 2020 incl Bijlagen_1.json, 01_CAO_BAKKERSBEDRIJF_1_OKTOBER_2016___def_.json, BAKKERSBEDRIJF_cao_tekst_en_bijlagen.json, CAO BAKKERSBEDRIJF 1 AUGUSTUS 2020 incl Bijlagen.json, 01_CAO_BAKKERSBEDRIJF_1_APRIL_2014_1.json, cao Bakkersbedrijf, definitief versie 26072024.json</t>
         </is>
       </c>
     </row>
@@ -1451,17 +1687,25 @@
       <c r="E32" t="n">
         <v>11</v>
       </c>
-      <c r="F32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G32" t="n">
         <v>11</v>
       </c>
-      <c r="H32" t="inlineStr"/>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I32" t="n">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>cao_hbo_2014_2016.json, 085_021_CAO_2018_2020_PAGINA_S.json, 085_021_CAO_2020_DEFDEF.json, CAO_2024_2025def.json, CAO_DEF_2017_2018___.json, caohbo_2012_2013_definitief.json, CAO_2021-2022_DEF.json, cao_hbo_2014_2016_1.json, 085_021_CAO_2022_2023DEF.json, CAOHBO_2023_2024.json</t>
+          <t>085_021_CAO_2018_2020_PAGINA_S.json, 085_021_CAO_2020_DEFDEF.json, CAO_2024_2025def.json, CAO_DEF_2017_2018___.json, caohbo_2012_2013_definitief.json, cao_hbo_2014_2016_1.json, CAOHBO_2023_2024.json</t>
         </is>
       </c>
     </row>
@@ -1483,17 +1727,25 @@
       <c r="E33" t="n">
         <v>25</v>
       </c>
-      <c r="F33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G33" t="n">
         <v>25</v>
       </c>
-      <c r="H33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>cao 1 juli 2018 - 30 juni 2023 definitief mei 2020.docx.json, cao_1_juli_2012___30_september_2013_definitief.json, Cao Particuliere beveiliging Versie 3- april 2021.json, CAO PB 18 dec 2024- 27 dec 2026.json, cao_2014_2015_definitief.json, Cao Particuliere beveiliging Versie 4- mei 2021.json, Cao Particuliere beveiliging Versie 6 - mei 2022 met zichtbare wijzigingen.json, CAO PB 18 dec 2024- 27 dec 2026 zonder zichtbare wijzigingen.json, cao_2011_definitief.json, Cao Particuliere Beveiliging versie 7 juni 2023 ZONDER zichtbare wijzigingen_1.json, cao_2014_2015_definitief_1.json, Cao Particuliere beveiliging Versie 5- januari 2022.json, Cao Particuliere Beveiliging 2023-2024 versie 2- augustus 2023 ZONDER zichtbare wijzigingen.json, Cao Particuliere Beveiliging versie 7 juni 2023 ZONDER zichtbare wijzigingen.json, cao 1 juli 2018 - 30 juni 2023 definitief.docx _1.json, cao_2012_definitief.json, definitief.json, cao_definitief__september_2017.json, cao_1_juli_2012___30_september_2013_definitief_1.json, cao 1 juli 2018 - 30 juni 2023 definitief versie 2 met aanvullende wijziging voo.json, cao_2014_2015_definitief_part_beveilig.json, cao_definitief_versie_2.json, cao 1 juli 2018 - 30 juni 2023 definitief april 2020.docx.json, cao 1 juli 2018 - 30 juni 2023 definitief.docx .json, cao 1 juli 2018 - 30 juni 2023 definitief versie 2 met wijzigingen voor aanmeldi.json</t>
+          <t>cao 1 juli 2018 - 30 juni 2023 definitief mei 2020.docx.json, cao_1_juli_2012___30_september_2013_definitief.json, Cao Particuliere beveiliging Versie 3- april 2021.json, CAO PB 18 dec 2024- 27 dec 2026.json, cao_2014_2015_definitief.json, Cao Particuliere beveiliging Versie 4- mei 2021.json, Cao Particuliere beveiliging Versie 6 - mei 2022 met zichtbare wijzigingen.json, Cao Particuliere Beveiliging versie 7 juni 2023 ZONDER zichtbare wijzigingen_1.json, Cao Particuliere beveiliging Versie 5- januari 2022.json, cao 1 juli 2018 - 30 juni 2023 definitief.docx _1.json, cao_2012_definitief.json, definitief.json, cao_definitief__september_2017.json, cao_1_juli_2012___30_september_2013_definitief_1.json, cao_2014_2015_definitief_part_beveilig.json, cao_definitief_versie_2.json, cao 1 juli 2018 - 30 juni 2023 definitief april 2020.docx.json, cao 1 juli 2018 - 30 juni 2023 definitief versie 2 met wijzigingen voor aanmeldi.json</t>
         </is>
       </c>
     </row>
@@ -1515,17 +1767,25 @@
       <c r="E34" t="n">
         <v>20</v>
       </c>
-      <c r="F34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G34" t="n">
         <v>20</v>
       </c>
-      <c r="H34" t="inlineStr"/>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>cao_Glastuinbouw_incl_ttw_1_1_2018_integrale_tekst.json, Glastuinbouw aangepast II.json, CAO Glastuinbouw aangepast.json, Integrale tekst cao Glastuinbouw 1 juli 2025 tm 31 maart 2026 (2506-1911).json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022 inclusief derde TTW..json, Glastuinbouw 1 juli 2018 tot en met 31december 2019 incl functiehandboek.docx.json, cao Glastuinbouw 1 juli 2018 tot en met 31december 2019 inclusief 2e TTW en incl.json, Integrale tekst Cao Glastuinbouw 1 januari 2024 tot en met 31 maart 2025 incl. 1e TTW per 1 januari 2024 (2406-1334).json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022 inclusief eerste TTW.json, cao Glastuinbouw 1 juli 2018 tot en met 31december 2019 inclusief functiehandboe.json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022 inclusief tweede TTW.json, cao_Glastuinbouw.json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022.json, Glastuinbouw__TTW_en_functiehandboek.json, cao_Glastuinbouw_2012_2014_registratie_SZW__2.json, Cao Glastuinbouw 1 januari 2023 tot en met 31 december 2023.json, cao_Glastuinbouw_2e_ttw_14_mei_2018_integr.json, Integrale tekst Cao Glastuinbouw 1 april 2025 tm 30 juni 2025 (2506-1846).json, cao_Glastuinbouw_2015____2018.json, Integrale tekst Cao Glastuinbouw 1 januari 2024 tot en met 31 maart 2025 (2404-2053).json</t>
+          <t>Glastuinbouw aangepast II.json, CAO Glastuinbouw aangepast.json, Integrale tekst cao Glastuinbouw 1 juli 2025 tm 31 maart 2026 (2506-1911).json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022 inclusief derde TTW..json, Glastuinbouw 1 juli 2018 tot en met 31december 2019 incl functiehandboek.docx.json, cao Glastuinbouw 1 juli 2018 tot en met 31december 2019 inclusief 2e TTW en incl.json, Integrale tekst Cao Glastuinbouw 1 januari 2024 tot en met 31 maart 2025 incl. 1e TTW per 1 januari 2024 (2406-1334).json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022 inclusief eerste TTW.json, cao Glastuinbouw 1 juli 2018 tot en met 31december 2019 inclusief functiehandboe.json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022 inclusief tweede TTW.json, cao_Glastuinbouw.json, Cao Glastuinbouw 1 januari 2020 tot en met 31 december 2022.json, Glastuinbouw__TTW_en_functiehandboek.json, cao_Glastuinbouw_2012_2014_registratie_SZW__2.json, Cao Glastuinbouw 1 januari 2023 tot en met 31 december 2023.json, cao_Glastuinbouw_2e_ttw_14_mei_2018_integr.json, Integrale tekst Cao Glastuinbouw 1 april 2025 tm 30 juni 2025 (2506-1846).json, cao_Glastuinbouw_2015____2018.json, Integrale tekst Cao Glastuinbouw 1 januari 2024 tot en met 31 maart 2025 (2404-2053).json</t>
         </is>
       </c>
     </row>
@@ -1547,11 +1807,19 @@
       <c r="E35" t="n">
         <v>1</v>
       </c>
-      <c r="F35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G35" t="n">
         <v>1</v>
       </c>
-      <c r="H35" t="inlineStr"/>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I35" t="n">
         <v>0</v>
       </c>
@@ -1579,19 +1847,23 @@
       <c r="E36" t="n">
         <v>17</v>
       </c>
-      <c r="F36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G36" t="n">
         <v>17</v>
       </c>
-      <c r="H36" t="inlineStr"/>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I36" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>CAO Technische Groothandel 2023-2025_Versie 2024-04-11.json, CAO TG 2023-2025_Tussentijdse AVV-aanpassing_Versie 2025-02-14.json, CAO TG 2023-2025_Tussentijdse aanpassing.json, CAOTechnGroTussentijdseWijz1jan2013Art18lid2.json, CAO TG 2023-2025_Versie 2024-12-11.json, CAO TG 2023-2025_Versie 2025-01-31.json, CAO_2011_2012_Formele_tekst_CAO.json, CAO_Technische_Groothandel_2014_2016_Formele_tekst.json, CAO Technische Groothandel 2019-2022.json, CAOTG20162018Aanpassingen20170807.json, 730 - CAO TG 2019-2022_Tussentijdse wijziging_2022-05-09.json, CAO Technische Groothandel 2023-2025_Versie 2024-04-04.json, CAO Technische Groothandel 2022-2023_Versie 2023-03-27.docx.json, CAO Technische Groothandel 2023-2025_Versie 2024-05-13.json, CAOTechnischeGroothandel20162018.json, CAO Technische Groothandel 2022-2023_Versie 2023-03-07.json, 730 - CAO TG 2019-2022_Tussentijdse wijziging_2022-06-22.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1611,11 +1883,19 @@
       <c r="E37" t="n">
         <v>4</v>
       </c>
-      <c r="F37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G37" t="n">
         <v>4</v>
       </c>
-      <c r="H37" t="inlineStr"/>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I37" t="n">
         <v>0</v>
       </c>
@@ -1643,19 +1923,23 @@
       <c r="E38" t="n">
         <v>10</v>
       </c>
-      <c r="F38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G38" t="n">
         <v>10</v>
       </c>
-      <c r="H38" t="inlineStr"/>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I38" t="n">
-        <v>24</v>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>CAOVDB_2015_16__tekst_def_geschoond.json, Drogisterijbranche__2010_12_definitieve_tekst.json, CAO_2017_2018_tekst_aangepast_geschoond_def.json, TTW 2025 Cao boekje VDF-tekst geschoond.json, CAO_2017_2018_tekst_def_geschoond_per_april_2018.json, CAO_2017_2018_tekst_aangepast_geschoond.json, Cao boekje Drogisterijbranche VDF- schoon.json, Cao boekje VDF-tekst geschoond voor TW.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1675,19 +1959,23 @@
       <c r="E39" t="n">
         <v>29</v>
       </c>
-      <c r="F39" t="inlineStr"/>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G39" t="n">
         <v>29</v>
       </c>
-      <c r="H39" t="inlineStr"/>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I39" t="n">
-        <v>7</v>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>cao open teelten 4e ttw per 1 juli 2022 - integrale tekst.json, CAO_OT_2017_2020.json, Cao open teelten per 1 maart 2021 tot en met 28 februari 2023 1e TTW integraal.d.json, Cao open teelten per 1 maart 2021 tot en met 28 februari 2023 1e TTW integraal.d_1.json, cao_open_teelten_inc_ttw.json, cao open teelten per 1 juli 2020.docx.json, 1811_2255_2e_tww_cao_open_teelten_per_1_1_2019a.json, Integrale tekst cao Open Teelten 1 maart 2023 tm 30 juni 2024 incl. 2e TTW per 1 juli 2023 (2306-1279).json, Integrale tekst cao Open Teelten incl. 6e TTW per 1 januari 2023 - 2302-0811 v0..json, Open_Teelten_en_functiehandboek.json, cao_open_teelten_inclusief_ttw_1_dec_2016.json, cao_open_teelten_2016_2017.json, Open Teelten integrale tekst incl ttw.json, Cao Open Teelten 3e TTW per 1 juli 2019 definitief.docx.json, cao_Open_Teelten_ttw_per_1_juli_2018.json, Integrale tekst cao Open Teelten looptijd 1 juli 2024 tm 30 juni 2025 incl. TTW per 1 januari 2025 (2501-0136).json, Cao Open Teelten 4e TTW per 1 januari 2020.docx.json, Integrale tekst cao Open Teelten looptijd 1 juli 2025 tm 30 juni 2027 (2506-2013).json, cao open teelten 3e ttw 1 januari 2022 integraal _.json, 2104-1910 cao Open Teelten 2021-2023.json, Cao open teelten per 1 maart 2021 tot en met 28 februari 2023 2e TTW integraal.d.json, CAO_Open_Teelten__1_juli_2014_tm_30_juni_2015.json, Integrale tekst cao Open Teelten looptijd 1 juli 2024 tm 30 juni 2025 (2410-1079).json, Integrale tekst cao Open Teelten 1 maart 2023 tm 30 juni 2024 incl. 3e TTW per 1 januari 2024 (2312-1367).json, cao Open Teelten met 5e ttw integraal per 1 november 2022 - 2210-1226 v0.1.json, cao_Open_Teelten_1_7_2012_tm_30_6_2014.json, Integrale tekst cao Open Teelten 1 maart 2023 tm 30 juni 2024 incl. 1e TTW per 1 maart 2023.json, Cao_Open_Teelten_integrale_tekst_ttw.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1707,17 +1995,25 @@
       <c r="E40" t="n">
         <v>20</v>
       </c>
-      <c r="F40" t="inlineStr"/>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G40" t="n">
         <v>20</v>
       </c>
-      <c r="H40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Bijlage 11 _ cao jz 21-23_B11_ Functieboek aanmeld.json, cao_tekst_JZ_2015_2016_def_met_bijlagen_1_tm_10.json, CAO_Jeugdzorg_28_04_11verlengd_schoon.json, cao_JZ_2015__2017_tm_B11.json, cao_tekst_JZ_2017_2019__23_8_17.json, CAO_JZ_2011_14_aanmelding_26_4_2013.json, CAO_JZ_2011_13_aanmelding_7_3_2013.json, Jeugdzorg_Cao_2011_2013_def020712.json, CAO Jeugdzorg versie 101215 versie 4.json, CAO_Jeugdzorg_17_02_12wijz_art12_3_schoon.json, Jeugdzorg_Cao_2011_2013_def.json, cao jeugdzorg aanmeldversie december 2024 compleet jk.json, Aanmeldversie cao Jeugdzorg 19-20.docx.json, cao_tekst_JZ_2017_2019_def_tekst_schoon_5_7_17.json, Cao Jeugdzorg 2024- 2025 aanmeldversie juli 2024 schoon.json, Cao Jeugdzorg 2024- 2025 aanmeldversie.json, cao_jeugdzorg_2014_2016_Aanmeldversie_compleet.json, cao_tekst_JZ_2017_2019_versie_TTW_18_5_2018.json, CAO Jeugdzorg 10-02-11schoon.json, cao_jeugdzorg_2014_2015_def.json</t>
+          <t>Bijlage 11 _ cao jz 21-23_B11_ Functieboek aanmeld.json, cao_JZ_2015__2017_tm_B11.json, cao_tekst_JZ_2017_2019__23_8_17.json, CAO_JZ_2011_14_aanmelding_26_4_2013.json, CAO_JZ_2011_13_aanmelding_7_3_2013.json, Jeugdzorg_Cao_2011_2013_def020712.json, CAO Jeugdzorg versie 101215 versie 4.json, CAO_Jeugdzorg_17_02_12wijz_art12_3_schoon.json, Jeugdzorg_Cao_2011_2013_def.json, cao jeugdzorg aanmeldversie december 2024 compleet jk.json, Aanmeldversie cao Jeugdzorg 19-20.docx.json, cao_tekst_JZ_2017_2019_def_tekst_schoon_5_7_17.json, Cao Jeugdzorg 2024- 2025 aanmeldversie.json, cao_jeugdzorg_2014_2016_Aanmeldversie_compleet.json, cao_tekst_JZ_2017_2019_versie_TTW_18_5_2018.json, CAO Jeugdzorg 10-02-11schoon.json, cao_jeugdzorg_2014_2015_def.json</t>
         </is>
       </c>
     </row>
@@ -1739,17 +2035,25 @@
       <c r="E41" t="n">
         <v>12</v>
       </c>
-      <c r="F41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G41" t="n">
         <v>12</v>
       </c>
-      <c r="H41" t="inlineStr"/>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Woondiensten_cao_en_handboek.json, CAO-Woondiensten 2022-2023 versie 01-09-2022.json, Woondiensten_2011_caotekst_en_handboek.json, CAO_Woondiensten_2014_2016_word.json, CAO Woondiensten 2021.json, cao woondiensten en handboek.json, CAO_Woondiensten_2013_tm_juni_definitieve_tekst.json, CAO_Woondiensten_inclusief_Handboek.json, Overzicht renvooi CAO Woondiensten 2019-2020.docx.json, cao tekst woondiensten.json, CAO Woondiensten 2024-2025 def (25 juni 2024).json, CAO_Woondiensten_2017_2018.json</t>
+          <t>Woondiensten_cao_en_handboek.json, Woondiensten_2011_caotekst_en_handboek.json, CAO_Woondiensten_2014_2016_word.json, CAO Woondiensten 2021.json, cao woondiensten en handboek.json, CAO_Woondiensten_2013_tm_juni_definitieve_tekst.json, CAO_Woondiensten_inclusief_Handboek.json, Overzicht renvooi CAO Woondiensten 2019-2020.docx.json, cao tekst woondiensten.json, CAO Woondiensten 2024-2025 def (25 juni 2024).json</t>
         </is>
       </c>
     </row>
@@ -1771,17 +2075,25 @@
       <c r="E42" t="n">
         <v>30</v>
       </c>
-      <c r="F42" t="inlineStr"/>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G42" t="n">
         <v>30</v>
       </c>
-      <c r="H42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>recreatie_definitief_1.json, cao_definitief_3_0_nav_opmerkingen_szw_avv.json, cao_definitief_1.json, Cao Recreatie, definitief versie 14042025.json, cao_definitief_5_0.json, cao_definitief_2_0_nav_opm_drukproef.json, cao 1 januari 2022 - 31 december 2023 definitief 21042022.json, recreatie_definitief.json, cao 1 januari 2019 - 31 december 2020, definitief aangepast.docx .json, cao_definitief_3_0.json, cao-recreatie 2024 - 2025 herschreven versie opgemaakt definitief 25062024.json, cao 1 januari 2019 - 31 december 2020, definitief aangepast versie augustus 2019.json, cao_definitief.json, Cao Recreatie, definitief versie 29042025.json, cao-recreatie 2024 - 2025 herschreven versie opgemaakt definitief 21052024.json, cao 1 januari 2019 - 31 december 2020, definitief.docx .json, cao_2010_2012_definitieve_versie_april_2012.json, cao_recreatie_2012_2013_definitieve_versie.json, cao_definitief_4_0.json, cao 1 januari 2022 - 31 december 2023 definitief 28122022.json, cao 1 januari 2022 - 31 december 2023 definitief 23012023.json, cao 1 januari 2022 - 31 december 2023 definitief 12052022.json, cao_Recreatie_2013_2014_def__versie.json, cao-recreatie 2024 - 2025 definitief 25062024 - versie 28112024 ivm WML per 1 januari 2025.json, Def_tekst_Ttw_cao_R.json, cao_definitief_2_0.json, cao 1 januari 2022 - 31 december 2023 definitief 01042022.json, cao 1 januari 2021 - 31 december 2021, defintief.json, cao 1 januari 2019 - 31 december 2020, definitief aangepast versie 1 juli.docx.json, handboek_compleet.json</t>
+          <t>recreatie_definitief_1.json, cao_definitief_1.json, Cao Recreatie, definitief versie 14042025.json, cao_definitief_5_0.json, cao_definitief_2_0_nav_opm_drukproef.json, cao 1 januari 2022 - 31 december 2023 definitief 21042022.json, recreatie_definitief.json, cao 1 januari 2019 - 31 december 2020, definitief aangepast.docx .json, cao_definitief_3_0.json, cao-recreatie 2024 - 2025 herschreven versie opgemaakt definitief 25062024.json, cao 1 januari 2019 - 31 december 2020, definitief aangepast versie augustus 2019.json, cao_definitief.json, Cao Recreatie, definitief versie 29042025.json, cao-recreatie 2024 - 2025 herschreven versie opgemaakt definitief 21052024.json, cao 1 januari 2019 - 31 december 2020, definitief.docx .json, cao_2010_2012_definitieve_versie_april_2012.json, cao_definitief_4_0.json, cao 1 januari 2022 - 31 december 2023 definitief 28122022.json, cao_Recreatie_2013_2014_def__versie.json, cao-recreatie 2024 - 2025 definitief 25062024 - versie 28112024 ivm WML per 1 januari 2025.json, Def_tekst_Ttw_cao_R.json, cao_definitief_2_0.json, cao 1 januari 2022 - 31 december 2023 definitief 01042022.json, cao 1 januari 2021 - 31 december 2021, defintief.json, handboek_compleet.json</t>
         </is>
       </c>
     </row>
@@ -1803,21 +2115,25 @@
       <c r="E43" t="n">
         <v>28</v>
       </c>
-      <c r="F43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G43" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>CAO Taxivervoer 2021 NET v231120.docx.json</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>CAO_tekst_Taxi_cao_nr__679.json, CAO Zorgvervoer en Taxi 2022, definitief incl inhoudsopgave februari 2022.json, CAO Zorgvervoer en Taxi 2023-2024 180424 def. tekst.json, cao tekst Taxivervoer.json, CAO Zorgvervoer en Taxi 2022, definitief incl inhoudsopgave september2022.json, TTW CAO Taxivervoer 2019 2020 v260420 DEF.docx.json, CAO Taxivervoer 2021 NET.docx.json, Taxivervoer_1_juli_2016_tot_en_met_30_juni_2017.json, CAO Zorgvervoer en Taxi 2022, definitief.json, Taxivervoer_CAO_aann__CAO_627.json, CAO_Taxi_Vervoer_2016.json, CAO Zorgvervoer en Taxi 2024-2025 definitieve tekst 100125.json, TTW CAO Taxivervoer 2019 2020 v050320 DEF NET.docx.json, CAO_Taxivervoer_2019_2020_NET_1.json, Taxivervoer_2009_2013_integrale_cao.json, TTW CAO Taxivervoer 2019 2020 v220620 DEF.docx.json, CAO_Taxivervoer_2017_2018.json, cao_taxivervoer_2016___2017_1.json, TTW_CAO_Taxivervoer_2017_2018.json, CAO_tekst_Taxivervoer_2014_2015_v5_nette_versie.json, TTW_CAO_Taxivervoer_2019_2020.json, cao_taxivervoer_2016___2017.json, CAO Zorgvervoer en Taxi 2024-2025 definitieve tekst 221124.json, CAO Zorgvervoer en Taxi 2023 06012023.json, CAO_tekst_Taxivervoer_2014_2015.json, CAO Zorgvervoer en Taxi 2023-2024 170524 definitieve tekst.json, CAO_Taxivervoer_2019_2020_NET.json</t>
+          <t>CAO_tekst_Taxi_cao_nr__679.json, CAO Zorgvervoer en Taxi 2022, definitief incl inhoudsopgave februari 2022.json, CAO Zorgvervoer en Taxi 2023-2024 180424 def. tekst.json, CAO Zorgvervoer en Taxi 2022, definitief incl inhoudsopgave september2022.json, TTW CAO Taxivervoer 2019 2020 v260420 DEF.docx.json, CAO Taxivervoer 2021 NET.docx.json, Taxivervoer_1_juli_2016_tot_en_met_30_juni_2017.json, CAO Zorgvervoer en Taxi 2022, definitief.json, CAO_Taxi_Vervoer_2016.json, TTW CAO Taxivervoer 2019 2020 v050320 DEF NET.docx.json, CAO_Taxivervoer_2019_2020_NET_1.json, Taxivervoer_2009_2013_integrale_cao.json, TTW CAO Taxivervoer 2019 2020 v220620 DEF.docx.json, CAO_Taxivervoer_2017_2018.json, cao_taxivervoer_2016___2017_1.json, TTW_CAO_Taxivervoer_2017_2018.json, CAO_tekst_Taxivervoer_2014_2015_v5_nette_versie.json, TTW_CAO_Taxivervoer_2019_2020.json, cao_taxivervoer_2016___2017.json, CAO Zorgvervoer en Taxi 2024-2025 definitieve tekst 221124.json, CAO Zorgvervoer en Taxi 2023 06012023.json, CAO Zorgvervoer en Taxi 2023-2024 170524 definitieve tekst.json, CAO Taxivervoer 2021 NET v231120.docx.json, CAO_Taxivervoer_2019_2020_NET.json</t>
         </is>
       </c>
     </row>
@@ -1839,17 +2155,25 @@
       <c r="E44" t="n">
         <v>23</v>
       </c>
-      <c r="F44" t="inlineStr"/>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G44" t="n">
         <v>23</v>
       </c>
-      <c r="H44" t="inlineStr"/>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I44" t="n">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>verlengde_cao_LEO__inclusief_ttw_1_maart_2016.json, Eindtekst cao Groen, Grond en Infrastructuur 1 januari 2024 - 31 december 2024 incl. 1e ttw per 1 januari 2024.json, LEO_2017_2019.json, cao_leo_2_januari_2012___30_juni_2013_incl_ttw.json, 2012-1466 cao GGI incl.ttw def.docx.json, integrale cao LEO 1 juli 2020 tot en met 31 december 2020 incl TTW per 1-11-2020.json, cao GGI 1 januari 2022 tm 31 december 2023 integraal.json, 2212-0813 defintieve tekst cao GGI met ttw per 1 januari 2023.json, cao GGI incl tref woorden def versie 2.docx.json, cao_leo_1_juli_2013_tm_30_juni_2014__20130716N_.json, Eindtekst cao Groen, Grond en Infrastructuur 1 januari 2025 - 30 september 2026.json, Integrale tekst cao Groen, Grond en Infrastructuur 1 januari 2024 - 31 december 2024.json, 2103-1098 cao GGI met 2e TTW.json, cao_LEO_1mei_2016_tot_en_met_30_juni_2017.json, cao_leo_1_juli_2014___31_december_2015tekst_def.json, 2104-0817 integrale cao GGI met 3e ttw.json, 2212-0813b defintieve tekst cao GGI met 1e ttw per 1 januari 2023.json, integrale cao LEO 1 juli 2020 tot en met 31 december 2020 def.docx.json, CAO_LEO__1_april_2010_tot_en_met_1_januari_2012.json, integrale_cao_Leo_2017_2019_a.json, cao_LEO__ttw_per_1_juli_2018.json, cao_leo.json</t>
+          <t>LEO_2017_2019.json, cao_leo_2_januari_2012___30_juni_2013_incl_ttw.json, 2012-1466 cao GGI incl.ttw def.docx.json, integrale cao LEO 1 juli 2020 tot en met 31 december 2020 incl TTW per 1-11-2020.json, cao GGI 1 januari 2022 tm 31 december 2023 integraal.json, 2212-0813 defintieve tekst cao GGI met ttw per 1 januari 2023.json, Eindtekst cao Groen, Grond en Infrastructuur 1 januari 2025 - 30 september 2026.json, Integrale tekst cao Groen, Grond en Infrastructuur 1 januari 2024 - 31 december 2024.json, 2103-1098 cao GGI met 2e TTW.json, cao_LEO_1mei_2016_tot_en_met_30_juni_2017.json, cao_leo_1_juli_2014___31_december_2015tekst_def.json, 2104-0817 integrale cao GGI met 3e ttw.json, integrale cao LEO 1 juli 2020 tot en met 31 december 2020 def.docx.json, CAO_LEO__1_april_2010_tot_en_met_1_januari_2012.json, integrale_cao_Leo_2017_2019_a.json, cao_LEO__ttw_per_1_juli_2018.json, cao_leo.json</t>
         </is>
       </c>
     </row>
@@ -1871,15 +2195,27 @@
       <c r="E45" t="n">
         <v>0</v>
       </c>
-      <c r="F45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G45" t="n">
         <v>0</v>
       </c>
-      <c r="H45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I45" t="n">
         <v>0</v>
       </c>
-      <c r="J45" t="inlineStr"/>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1899,17 +2235,25 @@
       <c r="E46" t="n">
         <v>12</v>
       </c>
-      <c r="F46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G46" t="n">
         <v>12</v>
       </c>
-      <c r="H46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I46" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cao_Apotheken_2012_2013_plat.json, Cao Apotheken 2024-2027 na ttw volledig met bijlagen 07-07-2025.json, CAO Apotheken 2021-2024 volledig met bijlagen 02-06-2022 def.json, CAO Apotheken 2021-2024 na ttw volledig met bijlagen 05-07-2022.json, Cao_Apotheken_2014_plat.json, CAO Apotheken 2021-2024 na ttw ivm verhoging.json</t>
+          <t>CAO Apotheken 2021-2024 volledig met bijlagen 02-06-2022 def.json, CAO Apotheken 2021-2024 na ttw volledig met bijlagen 05-07-2022.json, Cao_Apotheken_2014_plat.json, CAO Apotheken 2021-2024 na ttw ivm verhoging.json</t>
         </is>
       </c>
     </row>
@@ -1931,17 +2275,25 @@
       <c r="E47" t="n">
         <v>24</v>
       </c>
-      <c r="F47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G47" t="n">
         <v>24</v>
       </c>
-      <c r="H47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I47" t="n">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>cao_2011_2013_ttw4_tijdelijke_maatr_aanmelding.json, cao_Schilders_2013_2014_ttw_1_aanmelding.json, CAO SAVG 2021 2025 (TTW maart 2024) schone versie.json, cao_2011_2013_ttw_1__aanm_.json, CAO SAVG 2021-2025 (jan 2024) (Schilders, Afwerkings-, Vastgoedonderhoud- en Glaszetbedrijf).json, cao_2011_2013_ttw2_functieloon_aanmelding.json, CAO SAG 2016 2021 ttw april 2021.json, CAO SAG 2016 2021 ttw april 2021.2.json, CAO SAG 2016 2021 ttw januari 2021.json, CAO SAG 2016 2021 15 juli 2019.docx.json, CAO SAG 2016 2021 ttw 3 april 2020.json, CAO SAG 2016 2021 ttw 10 oktober 2018.pdf .json, CAO_SAG_2016_2019_versie_22_12_2016.json, cao_2011_2013_ttw3_functieloon_aanmelding.json, CAO_SAG_2016_2019__16_september_2016_.json, CAO SAVG 2025.json, CAO SAVG 2021 2025 oktober 2021.json, CAO SAVG 2021 2025 TTW februari 2023.json, cao_Schilders_2013_2014.json, CAO SAVG 2021 2025 december 2021.json, cao_2011_2013.json, CAO_SAG_2016_2019__ttw_29_september_2016_.json, CAO_SAG_2016_2019_ttw_20_november_2017.json</t>
+          <t>cao_Schilders_2013_2014_ttw_1_aanmelding.json, CAO SAVG 2021 2025 (TTW maart 2024) schone versie.json, cao_2011_2013_ttw_1__aanm_.json, CAO SAVG 2021-2025 (jan 2024) (Schilders, Afwerkings-, Vastgoedonderhoud- en Glaszetbedrijf).json, CAO SAG 2016 2021 ttw april 2021.json, CAO SAG 2016 2021 ttw april 2021.2.json, CAO SAG 2016 2021 ttw januari 2021.json, CAO SAG 2016 2021 15 juli 2019.docx.json, CAO SAG 2016 2021 ttw 10 oktober 2018.pdf .json, CAO_SAG_2016_2019_versie_22_12_2016.json, cao_2011_2013_ttw3_functieloon_aanmelding.json, CAO_SAG_2016_2019__16_september_2016_.json, CAO SAVG 2021 2025 oktober 2021.json, cao_Schilders_2013_2014.json, CAO SAVG 2021 2025 december 2021.json, cao_2011_2013.json, CAO_SAG_2016_2019__ttw_29_september_2016_.json, CAO_SAG_2016_2019_ttw_20_november_2017.json</t>
         </is>
       </c>
     </row>
@@ -1963,19 +2315,23 @@
       <c r="E48" t="n">
         <v>18</v>
       </c>
-      <c r="F48" t="inlineStr"/>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G48" t="n">
         <v>18</v>
       </c>
-      <c r="H48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I48" t="n">
-        <v>9</v>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>cao_HAZ_2014_2015_zwart_versie_II.json, cao_HAZ_2014_2015_zwart.json, CAO_Huisartsenzorg_2013_W.json, Cao-HZ 2019-2020 na ttw.docx.json, Huisartsenzorg__cao_tekst__cao_721.json, 12_01_25_CAO_tekst_definitief.json, CAO_Huisartsenzorg_2013_W_versie_2.json, Cao HAZ 2024-2025 met Handleiding FWHZ 3-6-2024.json, wijz_III_cao_HAZ_2015_2017_incl_FWHZ_anmtkst_zwart.json, Huisartsenzorg cao 2019-2020.json, Cao-huisartsenzorg-2022-2023-incl-Handleiding.json, Cao Huisartsenzorg 2021.json, 110919_CAO_Huisartsenzorg_2011_2012_definitief.json, Cao-HZ 2019-2020 na ttw2.docx.json, Cao Huisartsenzorg 2022-2023 na TTW ivm herziening loonsverhoging per 1-1-2023.p.json, huisartsenzorg_2017_2019_TTW.json, Cao_huisartsenzorg_30122015.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1995,17 +2351,25 @@
       <c r="E49" t="n">
         <v>18</v>
       </c>
-      <c r="F49" t="inlineStr"/>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G49" t="n">
         <v>18</v>
       </c>
-      <c r="H49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Grafimedia cao 2020-2021 - def 230221.docx.json, Grafimedia cao 2020-2021 juni 2021.json, Grafimedia cao 2022-2024 2 maart 2022.json, Grafimedia def..json, Grafimedia_cao_na_ttw_2015_2018_18122015_def.json, DEF Grafimedia cao 2024-2025 schone versie TCC 29112024.json, Grafimedia_cao.json, Reglement_Garantiefonds_07_12_2011__2_.json, DEF Grafimedia cao 2024-2025 TCC 09122024.json, Cao_2012_2013_wijz_art_169_z_renv_fndsbep_def.json, Grafimedia_cao_2015_2018_def_incl_stat_regl.json, DEF Grafimedia cao 2024-2025 schone versie v23102024.json, Grafimedia cao 2022-2024 15 februari 2022.json, Grafimedia cao 2018-2020 def 12-2-19.pdf .json, Grafimedia cao 2020-2021 6 juli 2021, gewijzigde werkingssfeer.json, Grafimedia cao 2022-2024 1 april 2022.json, Grafimedia cao 2020-2021 gewijzigde werkingssfeer.json, DEF Grafimedia cao 2024-2025 21012025.json</t>
+          <t>Grafimedia cao 2020-2021 - def 230221.docx.json, Grafimedia cao 2020-2021 juni 2021.json, Grafimedia cao 2022-2024 2 maart 2022.json, Grafimedia def..json, Grafimedia_cao_na_ttw_2015_2018_18122015_def.json, DEF Grafimedia cao 2024-2025 schone versie TCC 29112024.json, Grafimedia_cao.json, DEF Grafimedia cao 2024-2025 TCC 09122024.json, Cao_2012_2013_wijz_art_169_z_renv_fndsbep_def.json, Grafimedia_cao_2015_2018_def_incl_stat_regl.json, DEF Grafimedia cao 2024-2025 schone versie v23102024.json, Grafimedia cao 2018-2020 def 12-2-19.pdf .json, Grafimedia cao 2020-2021 6 juli 2021, gewijzigde werkingssfeer.json, Grafimedia cao 2022-2024 1 april 2022.json, Grafimedia cao 2020-2021 gewijzigde werkingssfeer.json, DEF Grafimedia cao 2024-2025 21012025.json</t>
         </is>
       </c>
     </row>
@@ -2027,17 +2391,25 @@
       <c r="E50" t="n">
         <v>12</v>
       </c>
-      <c r="F50" t="inlineStr"/>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G50" t="n">
         <v>12</v>
       </c>
-      <c r="H50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>tekst CAO Kappers 2010-2011.json, Tekst_cao_kappers_compleet.json, CAO Kappers 1 juli 2019 31 januari 2020 25072019.docx.json, CAOKAP~1.json, CAO_Kappers_1_juli_2017_30_juni_2019__3105_.json, CAO Kappers 1 juli 2024 30 juni 2025 (definitief).json, CAOKAP~2.json, CAO Kappers 1 juli 2023 30 juni 2024 geheel def.json, CAO Kappers 1 juli 2019 31 januari 2020 renvooi 07102019.docx.json, CAO_Kappers_1_juli_2017_30_juni_2019_1.json, CAO Kappers 1 juli 2022 30 juni 2023 schoon.json, CAO_Kappers_1_juli_2017_30_juni_2019.json</t>
+          <t>tekst CAO Kappers 2010-2011.json, Tekst_cao_kappers_compleet.json, CAO Kappers 1 juli 2019 31 januari 2020 25072019.docx.json, CAOKAP~1.json, CAO_Kappers_1_juli_2017_30_juni_2019__3105_.json, CAO Kappers 1 juli 2024 30 juni 2025 (definitief).json, CAOKAP~2.json, CAO Kappers 1 juli 2023 30 juni 2024 geheel def.json, CAO Kappers 1 juli 2019 31 januari 2020 renvooi 07102019.docx.json, CAO Kappers 1 juli 2022 30 juni 2023 schoon.json, CAO_Kappers_1_juli_2017_30_juni_2019.json</t>
         </is>
       </c>
     </row>
@@ -2059,17 +2431,25 @@
       <c r="E51" t="n">
         <v>17</v>
       </c>
-      <c r="F51" t="inlineStr"/>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G51" t="n">
         <v>17</v>
       </c>
-      <c r="H51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cao_Slagersbedrijf__versie_1_7_17.json, Cao voor het Slagersbedrijf 2019 - ongerenvooieerd.doc.json, Cao_Slagersbedrijf_1_10_17_tm_31_12_18_na_ttw_1.json, Cao_Slagers_1_4_16_tm_30_9_17.json, Cao_Slagersbedrijf_1_10_17_tm_31_12_18___def.json, Cao_voor_het_Slagersbedrijf_1_4_11_tm_31_3_13.json, Cao_Slagersbedrijf_1_4_15_tm_31_3_16.json, Cao_Slagersbedrijf_1_10_17_tm_31_12_18_na_ttw.json, CAOVOO~1.json, 02 - Cao voor het Slagersbedrijf 1-3-24 tm 31-8-25 - ongerenvooieerd.json, Cao voor het Slagersbedrijf.json, 26-DEF~1.json, Cao_voor_het_Slagersbedrijf_1_4_14_tm_31_3_15_1.json, Cao_voor_het_Slagersbedrijf_1_4_13_tm_31_3_14.json, Cao_voor_het_Slagersbedrijf_1_4_14_tm_31_3_15.json, Cao_voor_het_Slagersbedrijf_1_4_2011_tm_31_3_2013.json, 01-CAO~1.DOC.json</t>
+          <t>Cao_Slagersbedrijf__versie_1_7_17.json, Cao voor het Slagersbedrijf 2019 - ongerenvooieerd.doc.json, Cao_Slagersbedrijf_1_10_17_tm_31_12_18_na_ttw_1.json, Cao_Slagers_1_4_16_tm_30_9_17.json, Cao_Slagersbedrijf_1_10_17_tm_31_12_18___def.json, Cao_voor_het_Slagersbedrijf_1_4_11_tm_31_3_13.json, Cao_Slagersbedrijf_1_4_15_tm_31_3_16.json, Cao_Slagersbedrijf_1_10_17_tm_31_12_18_na_ttw.json, CAOVOO~1.json, 02 - Cao voor het Slagersbedrijf 1-3-24 tm 31-8-25 - ongerenvooieerd.json, Cao voor het Slagersbedrijf.json, 26-DEF~1.json, Cao_voor_het_Slagersbedrijf_1_4_14_tm_31_3_15_1.json, Cao_voor_het_Slagersbedrijf_1_4_14_tm_31_3_15.json, Cao_voor_het_Slagersbedrijf_1_4_2011_tm_31_3_2013.json</t>
         </is>
       </c>
     </row>
@@ -2091,17 +2471,25 @@
       <c r="E52" t="n">
         <v>13</v>
       </c>
-      <c r="F52" t="inlineStr"/>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G52" t="n">
         <v>13</v>
       </c>
-      <c r="H52" t="inlineStr"/>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Dhz-cao 2009-2011 def.json, Cao_DHZ_branche_2015_17_getekend.json, CAO_DHZ_2012_13_def.json, cao DHZ 2022-2023 nieuw geschoond.json, Dhz_cao_2009_2011_def.json, cao DHZ 2024-2026_def_april_2024.json, cao VWDHZ in pdf met handtekeningen.json, CAO-DHZ 2017-2020 wijzigingen geaccepteerd.doc .json, cao DHZ 2024-2026_def_dec_2024.json, CAO-DHZ 2022-2023 geschoond.json, cao DHZ 2024-2026_def_dec_2023.json, cao DHZ 2024-2026_def_mei_2024.json, cao DHZ 2024-2026_def_juni_2025.json</t>
+          <t>CAO_DHZ_2012_13_def.json, cao DHZ 2022-2023 nieuw geschoond.json, cao DHZ 2024-2026_def_april_2024.json, cao DHZ 2024-2026_def_dec_2024.json, CAO-DHZ 2022-2023 geschoond.json, cao DHZ 2024-2026_def_dec_2023.json, cao DHZ 2024-2026_def_mei_2024.json, cao DHZ 2024-2026_def_juni_2025.json</t>
         </is>
       </c>
     </row>
@@ -2123,19 +2511,23 @@
       <c r="E53" t="n">
         <v>26</v>
       </c>
-      <c r="F53" t="inlineStr"/>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G53" t="n">
         <v>26</v>
       </c>
-      <c r="H53" t="inlineStr"/>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>cao_2015_2016_wijziging_SKA_en_SUCON_I.json, cao 1 april 2024 - 31 december 2025 definitief 28062024.json, cao_cc.json, cao_definitief_1.json, cao 1 april 2024 - 31 december 2025.docx.json, cao_2010___2012__versie_juli_2011_.json, Contractcateringbranche__Arbeidsvoorw_cao.json, cao 1 april 2024 - 31 december 2025 18122024 opgeschoonde versie.json, cao 1 april 2022 - 31 maart 2024, definitief 01052023.json, cao 1 april 2022 - 31 maart 2024, definitief 17032023.json, cao arbeidsvoorwaarden, definitief januari 2020.docx.json, cao_avwd_1_april_2013_tot_1_april_2014.json, cao_definitief.json, cao_2014_2015.json, cao arbeidsvoorwaarden 1 april 2019 tot 1 april 2020, definitief.docx.json, cao 1 april 2022 - 31 maart 2024, definitief.json, cao_niet_gerenvooieerd.json, cao arbeidsvoorwaarden, definitief.json, cao 1 april 2022 - 31 maart 2024, definitief 18072023.json, cao_arbeidsvwd_2013_2014_gerenvooieerd.json, cao_1_april_2014_tot_1_juli_2015.json, cao 1 april 2022 - 31 maart 2024, definitief 03072023.json, caotekst_cc.json, cao_definitief_2.json, cao 1 april 2024 - 31 december 2025 definitief 26072024.json, contractcatering cao en handboek.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -2155,21 +2547,25 @@
       <c r="E54" t="n">
         <v>21</v>
       </c>
-      <c r="F54" t="inlineStr"/>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G54" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>CAO Groothandel in Groenten en Fruit 1 jan. tm 31 dec incl functiehandboek na tt.json</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>CAO_Frugi_Venta_definitief_2012_2014.json, Frugi_Venta_2010-2011__(obv_463120).json, CAO Groothandel in Groenten en Fruit 2019-2020 na ttw art 13 23 40 bijlage III V.json, Groothandel in Groenten en Fruit CAO 2019-2020 na ttw ivm salaristabellen.docx.json, CAO boekje 2020_v5.json, CAO Groothandel in Groenten en Fruit 2019-2020 na ttw2 art 29b en bijlage X.json, CAO_2010-2011_Groothandel_Groenten_Fruit_.json, Frugi_Venta_CAO_2011_2012_.json, CAO Groothandel in Groenten en Fruit 1 jan. 2023 tm 30 juni 2024 versie 26-4-2023 na ttw.json, Groothandel_groenten_en_fruit_2014_2016_difinitief.json, CAO Groothandel in Groenten en Fruit 1 jan. 2023 tm 30 juni 2024 versie 9-3-2023.json, Groothandel_groenten_en_fruit_cao_2017_2018_na_ttw.json, CAO_tekst_Groenten_en_Fruit_met_wijz_.json, Frugi_Venta_2009-2010_Groothandel_AGF.json, GGF_ttw_cao_2017_2018.json, Groothandel_groenten_en_fruit_cao_2017_2018.json, CAO Groothandel in Groenten en Fruit 1 juli 2024 tm 30 juni 2025 .json, Groothandel in Groenten en Fruit 2019-2020 definitief 03112019.json, Groothandel in Groenten en Fruit cao 2021.json</t>
+          <t>Frugi_Venta_2010-2011__(obv_463120).json, CAO Groothandel in Groenten en Fruit 2019-2020 na ttw art 13 23 40 bijlage III V.json, Groothandel in Groenten en Fruit CAO 2019-2020 na ttw ivm salaristabellen.docx.json, CAO boekje 2020_v5.json, CAO_2010-2011_Groothandel_Groenten_Fruit_.json, Frugi_Venta_CAO_2011_2012_.json, CAO Groothandel in Groenten en Fruit 1 jan. 2023 tm 30 juni 2024 versie 26-4-2023 na ttw.json, Groothandel_groenten_en_fruit_2014_2016_difinitief.json, CAO Groothandel in Groenten en Fruit 1 jan. 2023 tm 30 juni 2024 versie 9-3-2023.json, Groothandel_groenten_en_fruit_cao_2017_2018_na_ttw.json, CAO Groothandel in Groenten en Fruit 1 jan. tm 31 dec incl functiehandboek na tt.json, GGF_ttw_cao_2017_2018.json, Groothandel_groenten_en_fruit_cao_2017_2018.json, CAO Groothandel in Groenten en Fruit 1 juli 2024 tm 30 juni 2025 .json, Groothandel in Groenten en Fruit cao 2021.json</t>
         </is>
       </c>
     </row>
@@ -2191,19 +2587,23 @@
       <c r="E55" t="n">
         <v>26</v>
       </c>
-      <c r="F55" t="inlineStr"/>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G55" t="n">
         <v>26</v>
       </c>
-      <c r="H55" t="inlineStr"/>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>Cao Hoveniers 1 juli 2021 - 30 juni 2023 integraal_1.json, Integrale tekst cao voor het Hoveniersbedrijf 1 juli 2023 tm 30 september 2024 incl. TTW per 1 juli.json, CAO Hoveniers 6e ttw per 1 maart 2021.docx.json, Integ_Cao_hov_incl_ttw_2018_2020.json, 20120946N_Cao_hoveniers_2011tm2013_TWW_artikel_9.json, Cao_hov_v3.json, Cao_hoveniers_1_3_2013_tm_31_12_2013_20130472N.json, Integrale tekst cao voor het Hoveniersbedrijf 1 oktober 2024 tm 30 juni 2026 incl. TTW per 1 juli 2025.json, Integrale tekst cao voor het Hoveniersbedrijf 1 juli 2023 tm 30 september 2024 (2402-1326).json, 20120041N_Cao_hoveniers_TTW_2012.json, 20110636N_Cao_hoveniers_01032011_tm_28022013.json, Cao_Hoveniers_integrale_tekst.json, cao Hoveniers incl 4e ttw 1 novemb er 2020 def 2010-0194.docx.json, Integrale_cao_Hov_2018_2020.json, Cao Hoveniers 1 juli 2021 - 30 juni 2023 integraal.json, Cao_hoveniers_tm_29_2_2016_2e_TTW_26_11_2015_def.json, Cao_hoveniers_1_1_2014_tm_29_2_2016_20140383Na.json, Cao Hoveniers 1 juli 2021 - 30 juni 2023 inclusief tussentijdse wijziging per 1.json, Cao_Hov_ttw_27_2_2019.json, TTW_Cao_hov_2_8_16.json, Cao_Hov_ttw_5_12_2018.json, Integrale tekst cao voor het Hoveniersbedrijf 1 oktober 2024 tm 30 juni 2026 (2503-1886).json, Cao Hoveniers 5e ttw per 20 november 2020 - 2011-1582.docx.json, cao_Hoveniersbedrijf_2016_2018_ttw___31_8_2016.json, Cao_hoveniers_tm_29_2_2016_TTW_15_7_2015.json, Cao Hoveniers 1 juli 2021 - 30 juni 2023- ttw 1 januari 2023.json</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2223,19 +2623,23 @@
       <c r="E56" t="n">
         <v>12</v>
       </c>
-      <c r="F56" t="inlineStr"/>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G56" t="n">
         <v>12</v>
       </c>
-      <c r="H56" t="inlineStr"/>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I56" t="n">
-        <v>0</v>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>CAO ETD d.d. 15 mei 2023 (naar SZW, TTW).json, tekst_CAO20182020ETD_def.json, tekstCAO_2015_2017_INTEGRAAL.json, CAO-2021-2022 ETD tekst 7 december.docx.json, CAO_2018_2020ETD_maart__def.json, CAO ETD d.d. 23 maart 2023 (naar SZW).json, CAO ETD d.d. 27 februari 2023 (naar SZW).json, Elektro tekstCAO-2010-2011 (januari 2011).json, CAO ETD tekst (d.d. 8 juli 2024).json, CAO ETD platte tekst (d.d. 5 juni 2024).json, CAO-2021-2022 ETD tekst TTW d.d. 20 juni 2023.json, CAO ETD d.d. 17 mei 2023 (naar SZW, Aanmelding TTW).json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -2255,15 +2659,27 @@
       <c r="E57" t="n">
         <v>0</v>
       </c>
-      <c r="F57" t="inlineStr"/>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G57" t="n">
         <v>0</v>
       </c>
-      <c r="H57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I57" t="n">
         <v>0</v>
       </c>
-      <c r="J57" t="inlineStr"/>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -2283,17 +2699,25 @@
       <c r="E58" t="n">
         <v>17</v>
       </c>
-      <c r="F58" t="inlineStr"/>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G58" t="n">
         <v>17</v>
       </c>
-      <c r="H58" t="inlineStr"/>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I58" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cao_Binnendienst_schoon.json, Cao Verzekeringsbedrijf 2022-2023 def versie 24 mei 2022.json, Cao_Binnendienst_2015__2016_addendum.json, Cao voor het Verzekeringsbedrijf 2024.json, CAO Binnendienst 2018-2019.pdf .json, CAO_boekje_Binnendienst_wijzFAR.json, cao_binnendienst_2011_2012.json, Binnendienst_2015___2016_webversie.json, Cao_Binnendienst_2013.json, Cao Verzekeringsbedrijf 2022-2023 TTW februari 2023.json, Cao Verzekeringsbedrijf 2020 - integrale tekst.docx.json, Verzekeringsbedrijf_2016_2017_schoon_1.json, Cao_Verzekeringsbedrijf_2016_2017_schoon_ttw.json, Cao Verzekeringsbedrijf 2021 def versie 20210311.json, Cao_Verzekeringsbedrijf_Binnendienst_2018_2019.json, Cao voor het Verzekeringsbedrijf 2025-2026.json, Cao_binnendienst_2014.json</t>
+          <t>Cao Verzekeringsbedrijf 2022-2023 def versie 24 mei 2022.json, Cao_Binnendienst_2015__2016_addendum.json, Cao voor het Verzekeringsbedrijf 2024.json, CAO Binnendienst 2018-2019.pdf .json, CAO_boekje_Binnendienst_wijzFAR.json, cao_binnendienst_2011_2012.json, Binnendienst_2015___2016_webversie.json, Cao Verzekeringsbedrijf 2022-2023 TTW februari 2023.json, Cao Verzekeringsbedrijf 2020 - integrale tekst.docx.json, Verzekeringsbedrijf_2016_2017_schoon_1.json, Cao Verzekeringsbedrijf 2021 def versie 20210311.json, Cao_Verzekeringsbedrijf_Binnendienst_2018_2019.json, Cao voor het Verzekeringsbedrijf 2025-2026.json, Cao_binnendienst_2014.json</t>
         </is>
       </c>
     </row>
@@ -2315,19 +2739,23 @@
       <c r="E59" t="n">
         <v>18</v>
       </c>
-      <c r="F59" t="inlineStr"/>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G59" t="n">
         <v>18</v>
       </c>
-      <c r="H59" t="inlineStr"/>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I59" t="n">
-        <v>12</v>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>CAO_meubelindustrie_2018_2019_Def_1.json, CAO_tekst_2012_2014.json, CAOtekst2017.json, CAO Interieurbouw en Meubelindustrie 2024 clean.json, CAO meubelindustrie 2020-2021 def_1.json, Meubelindustrie__29_juli_2011.json, CAO_meubelindustrie_2018_2019_Def.json, CAO_tekst_2012_2014_1.json, CAO Interieurbouw en Meubelindustrie 2024 clean def.json, meubelindustrie_cao_tekst.json, CAO meubelindustrie 2022-2023.json, CAO meubelindustrie 2020-2021 def.json, CAO meubelindustrie 2018-2019 Def.docx .json, CAO_tekst_2015__2016_aangemeld.json, CAO meubelindustrie 2022-2023 TTW nieuwe cao tekst.json, CAO meubelindustrie 2020-2021 def P.json, CAO meubelindustrie 2022-2023 TTW.json</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2347,17 +2775,25 @@
       <c r="E60" t="n">
         <v>8</v>
       </c>
-      <c r="F60" t="inlineStr"/>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G60" t="n">
         <v>8</v>
       </c>
-      <c r="H60" t="inlineStr"/>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I60" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>WFC cao 2025-2027 na ttw 13-2-2025 szw.json, CAO Facilitaire contactcenters 2024 18-12-2023.json, CAO Facilitaire contactcenters 2022-2023 na ttw 23-6-2023_.getekend.json, CAO Facilitaire contactcenters 2022-2023 SIGNED.json, Cao FACILITAIRE CONTACTCENTERS.pdf .json, 2024.12.10 WFC cao 2025-2027 Clean Version Final_ getekend szw.json, CAO Facilitaire contactcenters 2024 na ttw 31-01-2024.json</t>
+          <t>WFC cao 2025-2027 na ttw 13-2-2025 szw.json, CAO Facilitaire contactcenters 2024 18-12-2023.json, CAO Facilitaire contactcenters 2022-2023 na ttw 23-6-2023_.getekend.json, CAO Facilitaire contactcenters 2022-2023 SIGNED.json, Cao FACILITAIRE CONTACTCENTERS.pdf .json, CAO Facilitaire contactcenters 2024 na ttw 31-01-2024.json</t>
         </is>
       </c>
     </row>
@@ -2379,17 +2815,25 @@
       <c r="E61" t="n">
         <v>17</v>
       </c>
-      <c r="F61" t="inlineStr"/>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G61" t="n">
         <v>17</v>
       </c>
-      <c r="H61" t="inlineStr"/>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>CAO_CAR_2015_2017.json, HB 5e editie 2024_2.json, CAO_CA_17_19.json, CAO Car 2021 2024b.json, CAO_CAR_2017_2019_TTW_juli_2017.json, HB 5e editie 2024.json, CAO_CAR_2017_2019_TTW_LL_nov_2018.json, carrosserie_aangepast_cao_n_a__v_bed.json, CAO_CAR__TTW_JULI.json, M_T_Totaal_tekst.json, CAO_CAR_2017_2019_TTW_GP_nov_2017.json, M_en_T_Carrosseriebedrijf_cao_en_handboek_doc.json, CAO CARR 2019 2021 SZW TTW Wagweu art 64.docx.json, CAO Car 2021 2024.json, CAO CARR 2019 2021 SZW TTW V2 Wagweu.docx.json, HB 5e editie 2024_1.json, CAO_CAR_arcering___wijz_AOW_LT.json</t>
+          <t>CAO_CAR_2015_2017.json, HB 5e editie 2024_2.json, CAO_CA_17_19.json, CAO Car 2021 2024b.json, HB 5e editie 2024.json, carrosserie_aangepast_cao_n_a__v_bed.json, CAO_CAR__TTW_JULI.json, M_T_Totaal_tekst.json, CAO_CAR_2017_2019_TTW_GP_nov_2017.json, M_en_T_Carrosseriebedrijf_cao_en_handboek_doc.json, CAO CARR 2019 2021 SZW TTW Wagweu art 64.docx.json, CAO CARR 2019 2021 SZW TTW V2 Wagweu.docx.json, HB 5e editie 2024_1.json, CAO_CAR_arcering___wijz_AOW_LT.json</t>
         </is>
       </c>
     </row>
@@ -2411,11 +2855,19 @@
       <c r="E62" t="n">
         <v>11</v>
       </c>
-      <c r="F62" t="inlineStr"/>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G62" t="n">
         <v>11</v>
       </c>
-      <c r="H62" t="inlineStr"/>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I62" t="n">
         <v>0</v>
       </c>
@@ -2443,17 +2895,25 @@
       <c r="E63" t="n">
         <v>1</v>
       </c>
-      <c r="F63" t="inlineStr"/>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G63" t="n">
         <v>1</v>
       </c>
-      <c r="H63" t="inlineStr"/>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I63" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>CAO_Tekst___CAO_Vast_2011___2012.json</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -2475,17 +2935,25 @@
       <c r="E64" t="n">
         <v>17</v>
       </c>
-      <c r="F64" t="inlineStr"/>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G64" t="n">
         <v>17</v>
       </c>
-      <c r="H64" t="inlineStr"/>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I64" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Cao_reisbranche_2016_2018_definitief_einddocument.json, cao Reisbranche 1jul2024-1jul2026 def1.json, 2019 Tekst cao-reisbranche 1 november 2018 - 1 september 2019 - versie 2.0.json, Tekst cao Reisbranche 1jul21-31dec21.json, Tekst cao Reisbranche 1jan-1jul2022.json, CAO_2015_2016_aanmelding.json, cao Reisbranche 1jul2024-1jul2026 def.json, CAO_teksten_voor_CAO_2013_2015_wijzigingen_def_R2.json, DEF_Tekst cao Reisbranche 1jan-1jul2022 - avv.docx.json, Tekst_cao_reisbranche_2016_2018_def_tekst.json, cao Reisbranche 1jul2022-1jul2024 - versie 2 sept 2022.json, 2019 Tekst cao-reisbranche 1 november 2018 - 1 september 2019.pdf .json, cao Reisbranche 1jul2022-1jul2024 concept versie.json, AWVN__487825_v1_DefCAO_ANVR_2011_2012.json, cao Reisbranche 1jul2024-1jul2026 def2.json, ANVR_CAO_2012_2013_Gecorrigeerde_tekst_def_R1.json, Tekst cao Reisbranche definitief.docx.json</t>
+          <t>Cao_reisbranche_2016_2018_definitief_einddocument.json, cao Reisbranche 1jul2024-1jul2026 def1.json, Tekst cao Reisbranche 1jul21-31dec21.json, CAO_2015_2016_aanmelding.json, DEF_Tekst cao Reisbranche 1jan-1jul2022 - avv.docx.json, Tekst_cao_reisbranche_2016_2018_def_tekst.json, cao Reisbranche 1jul2022-1jul2024 - versie 2 sept 2022.json, cao Reisbranche 1jul2022-1jul2024 concept versie.json, cao Reisbranche 1jul2024-1jul2026 def2.json, ANVR_CAO_2012_2013_Gecorrigeerde_tekst_def_R1.json, Tekst cao Reisbranche definitief.docx.json</t>
         </is>
       </c>
     </row>
@@ -2507,17 +2975,25 @@
       <c r="E65" t="n">
         <v>14</v>
       </c>
-      <c r="F65" t="inlineStr"/>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G65" t="n">
         <v>14</v>
       </c>
-      <c r="H65" t="inlineStr"/>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I65" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>CAO NWb 2018-2021-def.json, Cao_NWb_2015_2018_procesafspraken_30_03_2016.json, cao_Netwerkbedrijven_2_0_2011_2013.json, cao NWb 2021-2022.json, cao_NWb_2015_2018.json, cao NWb 2023 ondertekende versie.json, CAO NWb 2018 - 2021 - getekend.pdf .json, cao NWb 2024-2025_getekend.json, WEN25057_cao NWb-2026NL-FINAL zonder handtekening.json, Cao_NWb_2013_2015_met_aanpassing_DI.json, NWb_cao.json, CAO_NWb_2011_def.json, Cao_NWb_2013_1_mei.json, Cao_NWb_2013_2015_met_aanpassing_HNW_schoon.json</t>
+          <t>Cao_NWb_2015_2018_procesafspraken_30_03_2016.json, cao NWb 2021-2022.json, CAO NWb 2018 - 2021 - getekend.pdf .json, cao NWb 2024-2025_getekend.json, WEN25057_cao NWb-2026NL-FINAL zonder handtekening.json, NWb_cao.json, CAO_NWb_2011_def.json, Cao_NWb_2013_1_mei.json, Cao_NWb_2013_2015_met_aanpassing_HNW_schoon.json</t>
         </is>
       </c>
     </row>
@@ -2539,15 +3015,27 @@
       <c r="E66" t="n">
         <v>17</v>
       </c>
-      <c r="F66" t="inlineStr"/>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G66" t="n">
         <v>17</v>
       </c>
-      <c r="H66" t="inlineStr"/>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I66" t="n">
         <v>191</v>
       </c>
-      <c r="J66" t="inlineStr"/>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -2567,11 +3055,19 @@
       <c r="E67" t="n">
         <v>7</v>
       </c>
-      <c r="F67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G67" t="n">
         <v>7</v>
       </c>
-      <c r="H67" t="inlineStr"/>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I67" t="n">
         <v>0</v>
       </c>
@@ -2599,19 +3095,23 @@
       <c r="E68" t="n">
         <v>21</v>
       </c>
-      <c r="F68" t="inlineStr"/>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G68" t="n">
         <v>21</v>
       </c>
-      <c r="H68" t="inlineStr"/>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I68" t="n">
-        <v>0</v>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>CAO_Timmer_avv_27_3_2014.json, DEF_ARBVW_2011_2012.json, CAO_Timmer_1_apr___18_t_m__31_mrt__19_2e_vers_.json, CAO_Timmer_aanp_avv_14_4_2014.json, cao_nr__51_aug__18.json, INTEGRALE TEKST cao timmerindustrie 1 aug 2020 - 30 nov 2021.json, Cao Timmer 2024-2025 - incl bijlagen 28-06-2024.json, cao Timmerindustrie 1 dec 21 tt 1 mrt 2024_1.json, cao_Timmerindustrie_TTW_1_1_2015_tm_31_3_2017.json, Int_2__caoTimmer_TTW_1_1_15_tm_31_3_17.json, Cao Timmerindustrie 1 dec 21 tt 1 mrt 2024.json, Cao Timmerindustrie 1 apr 2019 tm 31 juli 2020.json, GEWIJZIGDE_april_DEF_ARBVW_2011_2012.json, Cao_Timmer_apr__2017__apr__2018.json, EINDVERSIE_CAO_TIMMERIND__2015_2017.json, cao Timmer nr 51 INTEGRAAL 1 aug 2020 - 30 nov 21.json, avv_REDACTIETEKST_ARBVW_2013_26sept.json, Minis_Cao_Timmer_apr__2017__apr__2018.json, CAO Timmerindustrie 1 apr 2019 tm 31 juli 2020 wijzigingen sept.19.json, Cao Timmer 2024-2025 - TTW .json, INTEGRALE cao Timmerindustrie 1 dec 21 tt 1 mrt 2024.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -2631,15 +3131,27 @@
       <c r="E69" t="n">
         <v>18</v>
       </c>
-      <c r="F69" t="inlineStr"/>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G69" t="n">
         <v>18</v>
       </c>
-      <c r="H69" t="inlineStr"/>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I69" t="n">
         <v>193</v>
       </c>
-      <c r="J69" t="inlineStr"/>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -2659,11 +3171,19 @@
       <c r="E70" t="n">
         <v>2</v>
       </c>
-      <c r="F70" t="inlineStr"/>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G70" t="n">
         <v>2</v>
       </c>
-      <c r="H70" t="inlineStr"/>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I70" t="n">
         <v>0</v>
       </c>
@@ -2691,11 +3211,19 @@
       <c r="E71" t="n">
         <v>11</v>
       </c>
-      <c r="F71" t="inlineStr"/>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G71" t="n">
         <v>11</v>
       </c>
-      <c r="H71" t="inlineStr"/>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I71" t="n">
         <v>0</v>
       </c>
@@ -2723,21 +3251,25 @@
       <c r="E72" t="n">
         <v>15</v>
       </c>
-      <c r="F72" t="inlineStr"/>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G72" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>VBZ_CAO_2012_2013__def.json</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I72" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>VBZ_cao_2017_def.json, Cao Zoetwarenindustrie 2023-2024.json, Cao na ttw Zoetwaren looptijd 1 januari 2023 tm 30 september 2024 (6 november 2023).json, VBZ_CAO_2012_2013__na_ttw_ivm_avv.json, VBZ_cao_2015_2016.json, Cao Zoetwarenindustrie 2021-2022 def.json, Zoetwarenindustrie_cao_2018.json, Cao Zoetwaren 2024-2026 na ttw (12 juni 2025).json, Herschreven cao Zoetwaren_finale versie (2 december 2024)_incl. IKB en akkoord cao-partijen (25 april 2025).json, VBZ_cao_2014.json, Zoetwaren_arbvoorw_CAO_2011_2012_.json, zoetwarindustrie cao 2019-2020 FINAAL.docx .json, Zoetwarenindustrie 2019-2020 na ttw ivm artikel 14 en 25 lid 3.pdf .json, Cao Zoetwarenindustrie 2021-2022 na correctie art 31.json</t>
+          <t>VBZ_cao_2017_def.json, Cao na ttw Zoetwaren looptijd 1 januari 2023 tm 30 september 2024 (6 november 2023).json, VBZ_CAO_2012_2013__na_ttw_ivm_avv.json, VBZ_cao_2015_2016.json, Cao Zoetwarenindustrie 2021-2022 def.json, Zoetwarenindustrie_cao_2018.json, Cao Zoetwaren 2024-2026 na ttw (12 juni 2025).json, Herschreven cao Zoetwaren_finale versie (2 december 2024)_incl. IKB en akkoord cao-partijen (25 april 2025).json, VBZ_CAO_2012_2013__def.json, Zoetwaren_arbvoorw_CAO_2011_2012_.json, zoetwarindustrie cao 2019-2020 FINAAL.docx .json, Cao Zoetwarenindustrie 2021-2022 na correctie art 31.json</t>
         </is>
       </c>
     </row>
@@ -2759,17 +3291,25 @@
       <c r="E73" t="n">
         <v>21</v>
       </c>
-      <c r="F73" t="inlineStr"/>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G73" t="n">
         <v>21</v>
       </c>
-      <c r="H73" t="inlineStr"/>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I73" t="n">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Cao MITT 2024-2025 versie 18 06112024 (003).json, SZW_CAOMITT2016_19_meld_2e_tussent__wijz__sch.json, CAO_MITT_2012_2014_schoon_dd__18_10_2012.json, CAOMITT_2014_2016_tussent_wijz_dec__2015_sch2.json, CAO MITT 2020 na ttw2 art. 1.3 en 6.3.json, SZW_CAO_MITT_2010_2012__wijziging_dec_2011_schoon.json, CAO MITT 2022-2023 definitief.json, SZW_CAO_MITT_2010_2012__wijziging_jan_2012_schoon.json, CAO MITT 2020 _1.json, SZW_CAOMITT2016_19_meld_3e_tussent__wijz__sch_.json, MITT cao 2019-2020.json, SZW_CAO_MITT_2012_2014_schoon_dd_6_9_2012.json, CAO MITT 2010-2012 -melding sept 2010-schoon.json, CAO_MITT_2014_2016_tussent__wijz__sch_szw.json, CAO MITT 2020 .json, CAO_MITT_2014_2016___schoon___niet_geel_gearceerd.json, CAO MITT 2021-2022.json, CAOMITT2014_16_tussent_wijz__juli_2017_sch_szw.json, CAO MITT 2023 versie 06072023.json, SZW_CAOMITT2016_19_melding__tussent__wijz__sch.json, SZW_CAOMITT2016_19_melding_schn_geen_wijz__zichtb_.json</t>
+          <t>SZW_CAOMITT2016_19_meld_2e_tussent__wijz__sch.json, CAOMITT_2014_2016_tussent_wijz_dec__2015_sch2.json, CAO MITT 2020 na ttw2 art. 1.3 en 6.3.json, SZW_CAO_MITT_2010_2012__wijziging_dec_2011_schoon.json, CAO MITT 2022-2023 definitief.json, SZW_CAO_MITT_2010_2012__wijziging_jan_2012_schoon.json, SZW_CAOMITT2016_19_meld_3e_tussent__wijz__sch_.json, MITT cao 2019-2020.json, SZW_CAO_MITT_2012_2014_schoon_dd_6_9_2012.json, CAO MITT 2010-2012 -melding sept 2010-schoon.json, CAO_MITT_2014_2016_tussent__wijz__sch_szw.json, CAO MITT 2020 .json, CAO_MITT_2014_2016___schoon___niet_geel_gearceerd.json, SZW_CAOMITT2016_19_melding_schn_geen_wijz__zichtb_.json</t>
         </is>
       </c>
     </row>
@@ -2791,17 +3331,25 @@
       <c r="E74" t="n">
         <v>13</v>
       </c>
-      <c r="F74" t="inlineStr"/>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G74" t="n">
         <v>13</v>
       </c>
-      <c r="H74" t="inlineStr"/>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I74" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Tekst CAO Boek en Kantoor 24 25 ongemark def.json, CAO_Kantoor_18_19_def_aanm.json, CAO_Kantoor_en_Boek_16_17_def.json, CAO_Kantoor_en_Boek_17_18_def.json, Boekhandel Kantoorvakhandel 2010-2012.json, Cao_Boekhandel_en_Kantoorvakhandel_2014_2016.json, Cao_Boekhandel_en_Kantoorvakhandel_2012_2014.json, Tekst CAO Boek en Kantoor 21 23 def.json, Cao_Boekh_en_Kantoorvakh_2012_2014_def.json, 070224_Tekst CAO Boek en Kantoor 23 24 ongemark def.json, Tekst CAO Boek en Kantoor 19 20 31-10-2019 ongemark def aanm.docx.json, CAO_Kantoor_en_Boek_17_18_nw_def.json, CAO_Kantoor_en_Boek_17_18_nw_sept.json</t>
+          <t>Tekst CAO Boek en Kantoor 24 25 ongemark def.json, CAO_Kantoor_en_Boek_16_17_def.json, Boekhandel Kantoorvakhandel 2010-2012.json, Cao_Boekhandel_en_Kantoorvakhandel_2014_2016.json, Cao_Boekhandel_en_Kantoorvakhandel_2012_2014.json, Tekst CAO Boek en Kantoor 21 23 def.json, Cao_Boekh_en_Kantoorvakh_2012_2014_def.json, 070224_Tekst CAO Boek en Kantoor 23 24 ongemark def.json, CAO_Kantoor_en_Boek_17_18_nw_def.json, CAO_Kantoor_en_Boek_17_18_nw_sept.json</t>
         </is>
       </c>
     </row>
@@ -2823,11 +3371,19 @@
       <c r="E75" t="n">
         <v>9</v>
       </c>
-      <c r="F75" t="inlineStr"/>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G75" t="n">
         <v>9</v>
       </c>
-      <c r="H75" t="inlineStr"/>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I75" t="n">
         <v>0</v>
       </c>
@@ -2855,17 +3411,25 @@
       <c r="E76" t="n">
         <v>18</v>
       </c>
-      <c r="F76" t="inlineStr"/>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G76" t="n">
         <v>18</v>
       </c>
-      <c r="H76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I76" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>cao_tekst_Tank_Was_2017_2019_v1.json, cao_tekst_Tank_Was_2017_2019_def.json, cao tekst Tank Was 2022-2023, definitief.json, cao tekst Tank Was 2020 2021 versie 20 juli 2020.doc.json, CAO_tekst_2013_2015.json, cao tekst Tank Was 2020 2021 versie 16 juli.doc.json, cao tekst Tank Was 2024 - 2025, definitief 21032024.json, cao_tekst_Tank_Was_def_3_juni_2016_1.json, cao_tekst_Tank_Was_2017_2019_def_1.json, cao tekst Tank Was 2024 - 2025, definitief 25012024.json, CAO_tekst_2013_2015_def.json, CAO_tekst_2011_2013.json, cao tekst Tank Was 2020 2021 versie 22 juni.doc.json, Ingediend bij SZW - Eindtekst cao Tankstations en Wasbedrijven 1 april 2025 - 31 december 2026.json, cao_tekst_Tank_Was_def_3_juni_2016.json, CAO_tekst_2011_2013__2_.json, cao tekst Tank Was 2022-2023, definitief 28032022.json, cao tekst Tank Was 2020 2021 versie 22 juli 2020.doc.json</t>
+          <t>cao_tekst_Tank_Was_2017_2019_v1.json, cao_tekst_Tank_Was_2017_2019_def.json, cao tekst Tank Was 2022-2023, definitief.json, cao tekst Tank Was 2020 2021 versie 20 juli 2020.doc.json, cao tekst Tank Was 2020 2021 versie 16 juli.doc.json, cao tekst Tank Was 2024 - 2025, definitief 21032024.json, cao_tekst_Tank_Was_def_3_juni_2016_1.json, cao_tekst_Tank_Was_2017_2019_def_1.json, cao tekst Tank Was 2024 - 2025, definitief 25012024.json, CAO_tekst_2011_2013.json, cao tekst Tank Was 2020 2021 versie 22 juni.doc.json, CAO_tekst_2011_2013__2_.json</t>
         </is>
       </c>
     </row>
@@ -2887,15 +3451,27 @@
       <c r="E77" t="n">
         <v>20</v>
       </c>
-      <c r="F77" t="inlineStr"/>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G77" t="n">
         <v>20</v>
       </c>
-      <c r="H77" t="inlineStr"/>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I77" t="n">
         <v>300</v>
       </c>
-      <c r="J77" t="inlineStr"/>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -2915,17 +3491,25 @@
       <c r="E78" t="n">
         <v>18</v>
       </c>
-      <c r="F78" t="inlineStr"/>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G78" t="n">
         <v>18</v>
       </c>
-      <c r="H78" t="inlineStr"/>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I78" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023 inclusief T.json, Cao_productiegerichte_dierhouderij_2014_2017.json, Eindtekst_cao_Dierhouderij_2012_2013_incl__ttw.json, cao_tekst_integraal.json, cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023.json, cao productiegerichte dierhouderij 2021 versie 30 januari 2021.docx.json, CAO_Dierhouderij_2010__2012.json, cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023_1.json, Eindtekst cao Productiegerichte Dierhouderij 1 januari 2024 - 31 december 2025.json, Eindtekst cao Productiegerichte Dierhouderij 1 januari 2024 - 31 december 2025 incl. 2e ttw per 1 januari 2025.json, Eindtekst cao Productiegerichte Dierhouderij 1 januari 2024 - 31 december 2025 incl. 1e ttw per 1 januari 2024.json, cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023 inclusief T_1.json, cao_Pg_Dierhouderij.json, Integrale tekst cao Productiegerichte Dierhouderij 2022 - 2023 (TTW per 1 juli 2023).json, cao_tekst_Pg_Dierhouderij.json, 20120967N_Eindtekst_cao_Dierhouderij_2012_2013.json, cao productiegerichte dierhouderij 2021 ttw 17 maart 2021.json, cao PGD integraal def.docx.json</t>
+          <t>cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023 inclusief T.json, Eindtekst_cao_Dierhouderij_2012_2013_incl__ttw.json, cao_tekst_integraal.json, cao productiegerichte dierhouderij 2021 versie 30 januari 2021.docx.json, CAO_Dierhouderij_2010__2012.json, cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023_1.json, Eindtekst cao Productiegerichte Dierhouderij 1 januari 2024 - 31 december 2025.json, Eindtekst cao Productiegerichte Dierhouderij 1 januari 2024 - 31 december 2025 incl. 2e ttw per 1 januari 2025.json, Eindtekst cao Productiegerichte Dierhouderij 1 januari 2024 - 31 december 2025 incl. 1e ttw per 1 januari 2024.json, cao Productiegerichte Dierhouderij 1 januari 2022 - 31 december 2023 inclusief T_1.json, cao_Pg_Dierhouderij.json, Integrale tekst cao Productiegerichte Dierhouderij 2022 - 2023 (TTW per 1 juli 2023).json, cao_tekst_Pg_Dierhouderij.json, 20120967N_Eindtekst_cao_Dierhouderij_2012_2013.json, cao productiegerichte dierhouderij 2021 ttw 17 maart 2021.json, cao PGD integraal def.docx.json</t>
         </is>
       </c>
     </row>
@@ -2947,17 +3531,25 @@
       <c r="E79" t="n">
         <v>10</v>
       </c>
-      <c r="F79" t="inlineStr"/>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G79" t="n">
         <v>10</v>
       </c>
-      <c r="H79" t="inlineStr"/>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I79" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>CAO_PLb_2013_caotekst.json, Sector-cao PLb 2025-2026 definitief.json, Cao PLb versie 5 juli 2021-signed.json, Productie__en_Leveringsbedrijven_cao_2011_2013.json, CAO tekst CAO PLb 2023-2024 ondertekend door cao-partijen.json, CAO_PLb_2013_def___ondertekend.json, CaoPLb_herstel_foute_verwijz_en_redac_wijz_tbvAVV.json, CAO PLb 2022-2023 definitief ondertekend.json, CAO PLb 2018 - 2020 ondertekend.pdf .json, CAO_PLb_2015___2018_definitief__30_juni_2016_.json</t>
+          <t>Sector-cao PLb 2025-2026 definitief.json, Cao PLb versie 5 juli 2021-signed.json, Productie__en_Leveringsbedrijven_cao_2011_2013.json, CAO tekst CAO PLb 2023-2024 ondertekend door cao-partijen.json, CAO_PLb_2013_def___ondertekend.json, CaoPLb_herstel_foute_verwijz_en_redac_wijz_tbvAVV.json, CAO PLb 2022-2023 definitief ondertekend.json, CAO PLb 2018 - 2020 ondertekend.pdf .json, CAO_PLb_2015___2018_definitief__30_juni_2016_.json</t>
         </is>
       </c>
     </row>
@@ -2979,11 +3571,19 @@
       <c r="E80" t="n">
         <v>3</v>
       </c>
-      <c r="F80" t="inlineStr"/>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G80" t="n">
         <v>3</v>
       </c>
-      <c r="H80" t="inlineStr"/>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
@@ -3011,17 +3611,25 @@
       <c r="E81" t="n">
         <v>14</v>
       </c>
-      <c r="F81" t="inlineStr"/>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G81" t="n">
         <v>14</v>
       </c>
-      <c r="H81" t="inlineStr"/>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I81" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>cao_Bloemenspeciaalzaken_16_8_2018.json, 1. 20250117 Def. cao Gesp. detailhandel bloemen en planten 2025-2026.json, cao_2011__2012_definitief.json, CAO_Gespec_Detailh_Bloemen_en_Planten_2018___2019.json, 2__Cao_Gesp___Detailh__in_Bloemen_en_Planten.json, Gewijzigde tekst 14 mei 2020 2.1.c Cao Gespecialiseerde detailhandel in bloemen.json, def. cao tekst Gespecialiseerde detailhandel in bloemen en planten 2023.json, 2024-02-15 Def. tekst tussentijds gewijzigde cao met wijzigingen bijgehouden cao Gespecialiseerde detailhandel in bloemen en planten 2024.json, def. cao tekst Gespecialiseerde detailhandel in bloemen en planten 2023_1.json, Cao_tekst_1.json, c. 20240403 (Schoon) Tekst tussentijds gewijzigde cao Gespecialiseerde detailhandel bloemen en planten.json, 2024-01-19 Def. tekst schoon cao Gespecialiseerde detailhandel in bloemen en planten 2024.json, Cao_tekst.json, 2.1.c Cao Gespecialiseerde detailhandel in bloemen en planten 2020 - 2022.docx.json</t>
+          <t>cao_Bloemenspeciaalzaken_16_8_2018.json, 1. 20250117 Def. cao Gesp. detailhandel bloemen en planten 2025-2026.json, cao_2011__2012_definitief.json, CAO_Gespec_Detailh_Bloemen_en_Planten_2018___2019.json, 2__Cao_Gesp___Detailh__in_Bloemen_en_Planten.json, Gewijzigde tekst 14 mei 2020 2.1.c Cao Gespecialiseerde detailhandel in bloemen.json, def. cao tekst Gespecialiseerde detailhandel in bloemen en planten 2023.json, 2024-02-15 Def. tekst tussentijds gewijzigde cao met wijzigingen bijgehouden cao Gespecialiseerde detailhandel in bloemen en planten 2024.json, Cao_tekst_1.json, c. 20240403 (Schoon) Tekst tussentijds gewijzigde cao Gespecialiseerde detailhandel bloemen en planten.json, 2024-01-19 Def. tekst schoon cao Gespecialiseerde detailhandel in bloemen en planten 2024.json, Cao_tekst.json, 2.1.c Cao Gespecialiseerde detailhandel in bloemen en planten 2020 - 2022.docx.json</t>
         </is>
       </c>
     </row>
@@ -3043,17 +3651,25 @@
       <c r="E82" t="n">
         <v>13</v>
       </c>
-      <c r="F82" t="inlineStr"/>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G82" t="n">
         <v>13</v>
       </c>
-      <c r="H82" t="inlineStr"/>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I82" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>CAO Waterbouw 2023-2024 schoon.json, CAO Waterbouw 2019-2020 definitief.docx .json, CAO Waterbouw 2021-2022 Integraal 03.12.2021.json, CAO_Waterbouw VERSIE 110329.json, CAO_VVW12.json, CAO Waterbouw 2022-2023_1.json, CAO Waterbouw 2024-2025 schoon.json, CAO Waterbouw 2022-2023.json, CAO_Waterbouw_2013_2014_def.json, CAO_Waterbouw__def_23_mei_2014_AVV.json, CAO Waterbouw 2025-2027 schoon-zn.json, CAO_Waterbouw_2018_2019_definitief.json, CAO_Waterbouw_2015_2018_def__8_juli_2015.json</t>
+          <t>CAO Waterbouw 2023-2024 schoon.json, CAO Waterbouw 2019-2020 definitief.docx .json, CAO Waterbouw 2021-2022 Integraal 03.12.2021.json, CAO_Waterbouw VERSIE 110329.json, CAO_VVW12.json, CAO Waterbouw 2024-2025 schoon.json, CAO Waterbouw 2022-2023.json, CAO_Waterbouw__def_23_mei_2014_AVV.json, CAO Waterbouw 2025-2027 schoon-zn.json, CAO_Waterbouw_2018_2019_definitief.json, CAO_Waterbouw_2015_2018_def__8_juli_2015.json</t>
         </is>
       </c>
     </row>
@@ -3075,17 +3691,25 @@
       <c r="E83" t="n">
         <v>14</v>
       </c>
-      <c r="F83" t="inlineStr"/>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G83" t="n">
         <v>14</v>
       </c>
-      <c r="H83" t="inlineStr"/>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Textielgroothandel_cao_2014_2016.json, Textielgroothandel_cao_ttw.json, Textielgroothandel_cao_2017_2018.json, Cao 2021-2023 na ttw.json, Textielgroothandel_CAO_2011_2012.json, Textielgroothandel_cao_2018_2020.json, cao_2016_2017_Textielgroothandel.json, Cao Textielgroothandel 2024-2026 versie 21-1-2025.json, Textielgroothandel_2012_2013.json, Cao Textielgroothandel 2023-2024 versie 19-7-2023.json, Cao Textielgroothandel 2023-2024 versie 21-8-2023.json, Textielgroothandel_CAO_2013_2014.json, cao 2021-2023.json, Textielgr__NVW_ttw_ivm_fkb_2012_2013_obv_1538864.json</t>
+          <t>Textielgroothandel_cao_2014_2016.json, Textielgroothandel_cao_2017_2018.json, Cao 2021-2023 na ttw.json, Textielgroothandel_cao_2018_2020.json, Cao Textielgroothandel 2024-2026 versie 21-1-2025.json, Textielgroothandel_2012_2013.json, Cao Textielgroothandel 2023-2024 versie 21-8-2023.json, Textielgroothandel_CAO_2013_2014.json</t>
         </is>
       </c>
     </row>
@@ -3107,19 +3731,23 @@
       <c r="E84" t="n">
         <v>13</v>
       </c>
-      <c r="F84" t="inlineStr"/>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G84" t="n">
         <v>13</v>
       </c>
-      <c r="H84" t="inlineStr"/>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I84" t="n">
-        <v>0</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>CAO_Sport_2016_2018_DEF.json, def__cao_WOS_01_01_2012_totmet_31_12_2012.json, WOS_cao_2013_definitief.json, CAO DEFINITIEF WOS.pdf .json, CAO_Sport_2015.json, Definitieve cao Sport 2022 - 2023.json, Sport cao 2024-2025.json, Sport-CAO 2019-2020 ttw.json, Sport 2021 definitief.json, CAO Sport 2022-2023 2.json, Sport_WOS_cao_2014.json, CAO 2009_2012_definitief.json, CAO_Sport_2016_2018_DEF_1.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -3139,17 +3767,25 @@
       <c r="E85" t="n">
         <v>21</v>
       </c>
-      <c r="F85" t="inlineStr"/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G85" t="n">
         <v>21</v>
       </c>
-      <c r="H85" t="inlineStr"/>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I85" t="n">
-        <v>45</v>
+        <v>188</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>cao 2022-2023 6 januari 2022 aanmelding.json, cao 2022-2023 ttw februari 2023 integraal.json, cao_afbouw_2011_12__integrale_cao.json, CAO_2015_2017_TTW_integrale_tekst.json, cao 2020-2021 integraal2.docx.json, 20241203 cao 2024-2025 ttw januari 2025 integraal.json, CAO_2013_2014_definitief_2.json, CAO_2018_2019_integraal_versie_8.json, CAO 2018-2019 integraal.docx .json, CAO_2015_2017_integrale_tekst2.json, cao afbouw 2022-2023 6 januari 2022 aanmelding 2.docx.json, cao 2020-2021 integraal.docx.json, cao 2024-2025, ttw augustus 2024, integraal.json, CAO_2015_2017_integrale_tekst.json, CAO_2013_2014_definitief.json, cao 2020-2021 ttw integraal.docx.json, CAO_2018_2019_integraal.json, cao 2024-2025, 18 april 2024 integraal.json, cao 2024-2025, 30 januari 2024 integraal.json</t>
+          <t>cao 2022-2023 ttw februari 2023 integraal.json, cao_afbouw_2011_12__integrale_cao.json, CAO_2015_2017_TTW_integrale_tekst.json, cao 2020-2021 integraal2.docx.json, CAO_2013_2014_definitief_2.json, CAO 2018-2019 integraal.docx .json, cao 2020-2021 integraal.docx.json, cao 2024-2025, ttw augustus 2024, integraal.json, CAO_2015_2017_integrale_tekst.json, CAO_2013_2014_definitief.json, cao 2020-2021 ttw integraal.docx.json, CAO_2018_2019_integraal.json, cao 2024-2025, 18 april 2024 integraal.json</t>
         </is>
       </c>
     </row>
@@ -3171,17 +3807,25 @@
       <c r="E86" t="n">
         <v>21</v>
       </c>
-      <c r="F86" t="inlineStr"/>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G86" t="n">
         <v>21</v>
       </c>
-      <c r="H86" t="inlineStr"/>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I86" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>15_00080a_NvW_Cao_OB_2015_2019_wijz_geaccepteerd.json, 2024-08-09 Cao OB gehele tekst met juiste opmaak_inhoudsopgave.json, Cao OB 1.7.2020 31.12.2022 ondertekend TUSSENTIJDSE TEKSTUELE WIJZIGINGEN GEAC.json, Cao_OB_2015_2019_salaristabel_1_juli_2017.json, Cao OB 2024 2026_incl gewijz Ontheffingsregeling.json, Cao_OB_2015_2019_invulling_loonruimte_2017.json, Cao OB_1.7.2019-1.7.2020.docx.json, Cao_OB_2015_2019_invulling_loonruimte_2016.json, 13_00052_Cao_OB_2014.json, 241129 Cao OB 2024 2026 tussentijdse wijzigingen.json, Cao_OB_verlenging_1_januari_2015_tot_15_juni_2015.json, CAO_2012_2013_def_incl_aanpassing_vakantiewet.json, Cao_OB_2015_2019_invulling_loonruimte_2019.json, Cao_OB_2015_2019_invulling_loonruimte_2018.json, Cao OB 1.7.2020 31.12.2022 ondertekend TUSSENTIJDSE WIJZIGING SALARISGARANTIE_GE.json, CAO 2010-2011.json, Cao_OB_2015_2019_WML_2018.json, 231122_wijz geaccepteerd_tussentijdse wijziging ivm avv_230428 cao OB 1.1.2023_31.3.2024_DEF.json, 230428 cao OB 1.1.2023_31.3.2024_DEF.json, Cao OB 1.7.2020 31.12.2022 ondertekend.json, Openbare_Bibliotheken_2012_2013.json</t>
+          <t>15_00080a_NvW_Cao_OB_2015_2019_wijz_geaccepteerd.json, 2024-08-09 Cao OB gehele tekst met juiste opmaak_inhoudsopgave.json, Cao OB 1.7.2020 31.12.2022 ondertekend TUSSENTIJDSE TEKSTUELE WIJZIGINGEN GEAC.json, Cao_OB_2015_2019_salaristabel_1_juli_2017.json, Cao OB 2024 2026_incl gewijz Ontheffingsregeling.json, Cao_OB_2015_2019_invulling_loonruimte_2017.json, Cao OB_1.7.2019-1.7.2020.docx.json, 13_00052_Cao_OB_2014.json, 241129 Cao OB 2024 2026 tussentijdse wijzigingen.json, Cao_OB_verlenging_1_januari_2015_tot_15_juni_2015.json, CAO_2012_2013_def_incl_aanpassing_vakantiewet.json, Cao_OB_2015_2019_invulling_loonruimte_2019.json, Cao_OB_2015_2019_invulling_loonruimte_2018.json, Cao OB 1.7.2020 31.12.2022 ondertekend TUSSENTIJDSE WIJZIGING SALARISGARANTIE_GE.json, CAO 2010-2011.json, Cao_OB_2015_2019_WML_2018.json, 231122_wijz geaccepteerd_tussentijdse wijziging ivm avv_230428 cao OB 1.1.2023_31.3.2024_DEF.json, Cao OB 1.7.2020 31.12.2022 ondertekend.json, Openbare_Bibliotheken_2012_2013.json</t>
         </is>
       </c>
     </row>
@@ -3203,15 +3847,27 @@
       <c r="E87" t="n">
         <v>20</v>
       </c>
-      <c r="F87" t="inlineStr"/>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G87" t="n">
         <v>20</v>
       </c>
-      <c r="H87" t="inlineStr"/>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I87" t="n">
         <v>374</v>
       </c>
-      <c r="J87" t="inlineStr"/>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -3231,15 +3887,27 @@
       <c r="E88" t="n">
         <v>0</v>
       </c>
-      <c r="F88" t="inlineStr"/>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G88" t="n">
         <v>0</v>
       </c>
-      <c r="H88" t="inlineStr"/>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I88" t="n">
         <v>0</v>
       </c>
-      <c r="J88" t="inlineStr"/>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -3259,17 +3927,25 @@
       <c r="E89" t="n">
         <v>14</v>
       </c>
-      <c r="F89" t="inlineStr"/>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G89" t="n">
         <v>14</v>
       </c>
-      <c r="H89" t="inlineStr"/>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I89" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Cao Betonproductenindustrie 2025-2026 versie 17-2-2025.json, Integrale_Cao_tekst_2017_2019_vs3.json, Cao Betonproductenindustrie 2023 versie 13-3-2023.json, Integrale_Cao_tekst_2017_2019_vs2.json, Cao Betonproductenindustrie 2021-2022 definitief.json, Cao Betonproductenindustrie 2019-2021 versie 08-04-2021.json, cao voor de betonproductenindustrie.json, CAO_2017_2019.json, Cao Betonproductenindustrie 2019-2021 na ttw versie 25-05-2021.json, Cao Betonproductenindustrie 2021-2022 na ttw definitief.json, CAO_voor_de_betonproductenindustrie_2011_2013.json, Cao_BPI_2014_2017_nieuwe_tekst.json, Cao Betonproductenindustrie 2024 versie 8-5-2024.json, cao_voor_de_betonproductenindustrie_2013__2014.json</t>
+          <t>Cao Betonproductenindustrie 2025-2026 versie 17-2-2025.json, Integrale_Cao_tekst_2017_2019_vs3.json, Cao Betonproductenindustrie 2023 versie 13-3-2023.json, Integrale_Cao_tekst_2017_2019_vs2.json, Cao Betonproductenindustrie 2021-2022 definitief.json, CAO_2017_2019.json, Cao Betonproductenindustrie 2019-2021 na ttw versie 25-05-2021.json, Cao Betonproductenindustrie 2021-2022 na ttw definitief.json, CAO_voor_de_betonproductenindustrie_2011_2013.json, Cao_BPI_2014_2017_nieuwe_tekst.json, Cao Betonproductenindustrie 2024 versie 8-5-2024.json</t>
         </is>
       </c>
     </row>
@@ -3291,15 +3967,27 @@
       <c r="E90" t="n">
         <v>0</v>
       </c>
-      <c r="F90" t="inlineStr"/>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G90" t="n">
         <v>0</v>
       </c>
-      <c r="H90" t="inlineStr"/>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I90" t="n">
         <v>0</v>
       </c>
-      <c r="J90" t="inlineStr"/>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -3319,17 +4007,25 @@
       <c r="E91" t="n">
         <v>14</v>
       </c>
-      <c r="F91" t="inlineStr"/>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G91" t="n">
         <v>14</v>
       </c>
-      <c r="H91" t="inlineStr"/>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I91" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>Cao Railinfrastructuur -staand DEFINITIEF periode 8-2025 voor AVV.json, Def tekst Cao 2021 versie 0.7_01062021.json, Rallinfra_CAO_2011_2012__definitief.json, Railinfra_CAO_2014_def_26042016.json, PDF Werkdocument Cao 2023 vers.02 01032023 (002).json, versie 2 def Cao Railinfrastructuur - DEFINITIEF juni 2024 - versie voor AVV - kopie.json, Cao Railinfrastructuur - 9 juli 2024.json, Rallinfra caotekst.json, railinfra_addendum_en_cao.json, Railinfra_CAO_2017_def_280917_1.json, Tekst Cao 2018.2019 def d.d. 22-05-2019 .pdf .json, Railinfra_CAO_2013__DEF_02_08_13.json, Cao Railinfrastructuur - DEFINITIEF 21 maart 2024 (002).json</t>
+          <t>Cao Railinfrastructuur -staand DEFINITIEF periode 8-2025 voor AVV.json, Def tekst Cao 2021 versie 0.7_01062021.json, Rallinfra_CAO_2011_2012__definitief.json, Railinfra_CAO_2014_def_26042016.json, PDF Werkdocument Cao 2023 vers.02 01032023 (002).json, versie 2 def Cao Railinfrastructuur - DEFINITIEF juni 2024 - versie voor AVV - kopie.json, Rallinfra caotekst.json, railinfra_addendum_en_cao.json, Railinfra_CAO_2017_def_280917_1.json, Tekst Cao 2018.2019 def d.d. 22-05-2019 .pdf .json, Railinfra_CAO_2013__DEF_02_08_13.json, Cao Railinfrastructuur - DEFINITIEF 21 maart 2024 (002).json</t>
         </is>
       </c>
     </row>
@@ -3351,21 +4047,25 @@
       <c r="E92" t="n">
         <v>15</v>
       </c>
-      <c r="F92" t="inlineStr"/>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G92" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>cao_arbeidsvoorwaarden_2018_2020_getekend.json</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I92" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>Cao_graan_be_en_verwerkende_bedrijven_2015___2017.json, cao tekst 2010 - 2012 per 1-4-2011.json, Cao Graanbe- en verwerkende bedrijven 2020 - 2022.json, x DEF Cao-teksten graanbe- en verwerkende bedrijven 2025.json, Cao_boekje_2012_2013.json, Cao Graanbe- en verwerkende Bedrijven 2024.pdf.json, CAO_boekje_2014___2015.json, cao_tekst_2013___2014.json, Tekst_cao_graan_2017__2018_def_MET_handtekening.json, cao_boekje_2015_2017.json, cao_arbeidsvoorwaarden_2018_2020_getekend_1.json, cao_tekst_2015___2017.json, Cao Graanbe- en verwerkende Bedrijven 2023 DEF.json, cao_tekst_2013___2014_DEF_Z_HT.json</t>
+          <t>cao_arbeidsvoorwaarden_2018_2020_getekend.json, Cao_graan_be_en_verwerkende_bedrijven_2015___2017.json, Cao Graanbe- en verwerkende bedrijven 2020 - 2022.json, x DEF Cao-teksten graanbe- en verwerkende bedrijven 2025.json, Cao Graanbe- en verwerkende Bedrijven 2024.pdf.json, CAO_boekje_2014___2015.json, cao_tekst_2013___2014.json, Tekst_cao_graan_2017__2018_def_MET_handtekening.json, cao_boekje_2015_2017.json, cao_arbeidsvoorwaarden_2018_2020_getekend_1.json, cao_tekst_2015___2017.json, cao_tekst_2013___2014_DEF_Z_HT.json</t>
         </is>
       </c>
     </row>
@@ -3387,17 +4087,25 @@
       <c r="E93" t="n">
         <v>13</v>
       </c>
-      <c r="F93" t="inlineStr"/>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G93" t="n">
         <v>13</v>
       </c>
-      <c r="H93" t="inlineStr"/>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I93" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>Nieuwe CAO 2018-2020 volledig.docx.json, AGF_detailhandel_in_Nieuwe_CAO_2018_2020.json, CAO_Aardapp__en_loont_.json, CAO_2016_2018_AGF_Detailhandel.json, CAO_2016_2018_AGF_Detailhandel_1.json, CAO_2014_2016_AGF_Detailhandel_zonder_bijlagen.json, Definitieve tekst CAO AGF Detailhandel 2024-2025_1.json, CAO AGF Detailhandel 2021-2024 def_.json, Definitieve tekst CAO AGF Detailhandel 2024-2025.json, CAO AGF Detailhandel 2021-2024 aanmelding.json, CAO AGF Detailhandel 2020-2021 volledig.docx.json, CAO AGF Detailhandel 2020-2021 volledig def.docx.json, cao 2010-2012 volledig.json</t>
+          <t>Nieuwe CAO 2018-2020 volledig.docx.json, AGF_detailhandel_in_Nieuwe_CAO_2018_2020.json, CAO_Aardapp__en_loont_.json, CAO_2016_2018_AGF_Detailhandel.json, CAO_2016_2018_AGF_Detailhandel_1.json, CAO_2014_2016_AGF_Detailhandel_zonder_bijlagen.json, Definitieve tekst CAO AGF Detailhandel 2024-2025.json, CAO AGF Detailhandel 2021-2024 aanmelding.json, CAO AGF Detailhandel 2020-2021 volledig.docx.json, CAO AGF Detailhandel 2020-2021 volledig def.docx.json, cao 2010-2012 volledig.json</t>
         </is>
       </c>
     </row>
@@ -3419,19 +4127,23 @@
       <c r="E94" t="n">
         <v>12</v>
       </c>
-      <c r="F94" t="inlineStr"/>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G94" t="n">
         <v>12</v>
       </c>
-      <c r="H94" t="inlineStr"/>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I94" t="n">
-        <v>0</v>
-      </c>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>sociale afspraken 2020 - 2023 geschoond.json, CAO Banden- en Wielenbranche 2023 na ttw 17-7-2023.json, sociale afspraken 2019 - 2020 geschoond.docx.json, CAO Banden- en Wielenbranche 2023 12-6-2023.json, sociale afspraken 2020 - 2023 geschoond_1.json, CAO Banden- en Wielenbranche 2024-2025 versie 9-4-2024 (2).json, cao_2016_2017_geschoond_26_07_16.json, sociale_afspraken_2018___2019_geschoond.json, CAO_2016___2017_geschoond.json, CAO_2010___2012_geschoond.json, CAO Banden- en Wielenbranche 2024-2025 na ttw2 versie 26-6-2024.json, CAO na ttw Banden- en Wielenbranche 2024-2025 versie 30-4-2024.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -3451,17 +4163,25 @@
       <c r="E95" t="n">
         <v>17</v>
       </c>
-      <c r="F95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G95" t="n">
         <v>17</v>
       </c>
-      <c r="H95" t="inlineStr"/>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I95" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>Zuivel cao I 2022 tussentijdse wijziging dec 2021.json, Zuivel I 2018-2020.pdf .json, Cao I zuivel 2022na ttw def.json, AWVN__534089_v1_Zuivel_CAO_I_2012_2014.json, Zuivel_cao_I_2016_2018.json, Zuivel I 2020.json, Zuivel cao I 2022.json, Zuivel_CAO_I_na_ttw2.json, Zuivel cao I 2021.json, Zuivel_2016_2018_cao_I.json, DEF cao I zuivel 1 april 2024 tot 1 april 2025.json, Zuivel I 2018-2020.docx .json, Zuivel_CAO_I_na_ttw_2012_2014_obv__1499987v0_2.json, Zuivelindustrie_tekst_nieuw_2014_2016.json, Cao I zuivel na ttw 1 januari 2023 tot en met 31 maart 2024.json, Zuivel cao I 1 januari 2023 tot en met 31 maart 2024.json, Zuivel_ttw_ivm_Arla_obv_481097.json</t>
+          <t>Zuivel cao I 2022 tussentijdse wijziging dec 2021.json, Zuivel I 2018-2020.pdf .json, Cao I zuivel 2022na ttw def.json, Zuivel_cao_I_2016_2018.json, Zuivel cao I 2022.json, Zuivel_CAO_I_na_ttw2.json, Zuivel_2016_2018_cao_I.json, DEF cao I zuivel 1 april 2024 tot 1 april 2025.json, Zuivel I 2018-2020.docx .json, Zuivel_CAO_I_na_ttw_2012_2014_obv__1499987v0_2.json, Zuivelindustrie_tekst_nieuw_2014_2016.json, Cao I zuivel na ttw 1 januari 2023 tot en met 31 maart 2024.json, Zuivel_ttw_ivm_Arla_obv_481097.json</t>
         </is>
       </c>
     </row>
@@ -3483,17 +4203,25 @@
       <c r="E96" t="n">
         <v>10</v>
       </c>
-      <c r="F96" t="inlineStr"/>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G96" t="n">
         <v>10</v>
       </c>
-      <c r="H96" t="inlineStr"/>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I96" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>tekst_CAO_01112010__01012012.json, CAO_Banken_2022.DefNL.json, NVB_CAO-boekje_2025_digitaal__redacted.json, NVB_CAO-boekje_2023_addendum.20240502.json, CAO__01012014_tot_01072014__CAO_tekst_14_jan_2014.json, NVB CAO-boekje 2021_14-04.json, NVB CAO-boekje 2023_digitaal-NL.json, CAO_Banken.json, OD18976_NVB CAO-boekje 2019_digitaal.pdf - CAO Banken_PDF digitaal NL versie.pdf .json, CAO_2017.json</t>
+          <t>CAO_Banken_2022.DefNL.json, NVB_CAO-boekje_2025_digitaal__redacted.json, NVB_CAO-boekje_2023_addendum.20240502.json, CAO__01012014_tot_01072014__CAO_tekst_14_jan_2014.json, NVB CAO-boekje 2021_14-04.json, NVB CAO-boekje 2023_digitaal-NL.json, CAO_Banken.json, OD18976_NVB CAO-boekje 2019_digitaal.pdf - CAO Banken_PDF digitaal NL versie.pdf .json, CAO_2017.json</t>
         </is>
       </c>
     </row>
@@ -3515,17 +4243,25 @@
       <c r="E97" t="n">
         <v>17</v>
       </c>
-      <c r="F97" t="inlineStr"/>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G97" t="n">
         <v>17</v>
       </c>
-      <c r="H97" t="inlineStr"/>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I97" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>ICK cao 2024-2025.json, ICK CAO 2022 v2.json, ICK-cao 2023.json, ICK CAO 2021_1.json, CAO 2019.json, ICK_CAO_2017.json, ICK-CAO 2018.pdf .json, ICK CAO 2021.json, ICK cao 2025-2026.json, Digitale_versie_ICK_CAO_2012.json, ICK_CAO_2016_definitief.json, Tekst_ICK_CAO_2011.json, ICK_CAO_2015___definitief.json, Definitieve_Tekst_ICK_CAO_2013_18_februari_2013_MV.json, Definitieve_tekst_ICK_CAO_2014_6_maart_2014.json, Cdef_ ICK CAO 2022.json, ICK CAO 2020_def.docx.json</t>
+          <t>ICK cao 2024-2025.json, ICK CAO 2022 v2.json, ICK-cao 2023.json, ICK CAO 2021_1.json, CAO 2019.json, ICK_CAO_2017.json, ICK-CAO 2018.pdf .json, ICK CAO 2021.json, ICK cao 2025-2026.json, Digitale_versie_ICK_CAO_2012.json, ICK_CAO_2015___definitief.json, Definitieve_Tekst_ICK_CAO_2013_18_februari_2013_MV.json, Definitieve_tekst_ICK_CAO_2014_6_maart_2014.json, ICK CAO 2020_def.docx.json</t>
         </is>
       </c>
     </row>
@@ -3547,15 +4283,27 @@
       <c r="E98" t="n">
         <v>0</v>
       </c>
-      <c r="F98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G98" t="n">
         <v>0</v>
       </c>
-      <c r="H98" t="inlineStr"/>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
-      <c r="J98" t="inlineStr"/>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -3575,17 +4323,25 @@
       <c r="E99" t="n">
         <v>18</v>
       </c>
-      <c r="F99" t="inlineStr"/>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G99" t="n">
         <v>18</v>
       </c>
-      <c r="H99" t="inlineStr"/>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I99" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>CAO_pluimvee_per_1_januari_2017.json, Cao pluimvee - cao 2021-2023 versie 7-9-2021.json, Cao pluimvee - 2019 na ttw2 ivm wijziging art 28.pdf .json, CAO_pluimvee_per_1_januari_2017_per_13_2_2017.json, Pluimvee cao 2019.pdf .json, Cao pluimvee - 2019 na ttw3 ivm wijziging art 25.docx .json, CAO_pluimvee_per_1_januari_2017_per_9_2_2017.json, CAO_pluimvee_per_1_januari_2017_per_23_3_2018.json, Cao pluimvee - cao 2020-2021 na ttw2 art 77 .json, Cao pluimvee - cao 2020-2021 na ttw art 31 52 77 78 79 bijlage 3 .json, pluimvee - 2019 na ttw ivm wijziging art 55.pdf .json, Cao pluimvee - cao 2023-2025 def.json, CAO_pluimvee_per_1_januari_2017_per_19_4_2018.json, Cao pluimvee - cao 2020-2021 .json, Cao pluimvee na ttw - cao 2023-2025.json, CAO_pluimvee_per_1_mei_2012.json, CAO_pluimvee_per_1_mei_2013.json, Cao pluimvee 2023-2025 na ttw 9-4-2024 (incl. gewijzigd functiehandboek).json</t>
+          <t>Cao pluimvee - cao 2021-2023 versie 7-9-2021.json, Cao pluimvee - 2019 na ttw2 ivm wijziging art 28.pdf .json, CAO_pluimvee_per_1_januari_2017_per_13_2_2017.json, Pluimvee cao 2019.pdf .json, Cao pluimvee - 2019 na ttw3 ivm wijziging art 25.docx .json, CAO_pluimvee_per_1_januari_2017_per_23_3_2018.json, Cao pluimvee - cao 2020-2021 na ttw art 31 52 77 78 79 bijlage 3 .json, pluimvee - 2019 na ttw ivm wijziging art 55.pdf .json, Cao pluimvee - cao 2023-2025 def.json, CAO_pluimvee_per_1_januari_2017_per_19_4_2018.json, Cao pluimvee na ttw - cao 2023-2025.json, CAO_pluimvee_per_1_mei_2013.json, Cao pluimvee 2023-2025 na ttw 9-4-2024 (incl. gewijzigd functiehandboek).json</t>
         </is>
       </c>
     </row>
@@ -3607,19 +4363,23 @@
       <c r="E100" t="n">
         <v>12</v>
       </c>
-      <c r="F100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G100" t="n">
         <v>12</v>
       </c>
-      <c r="H100" t="inlineStr"/>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I100" t="n">
-        <v>0</v>
-      </c>
-      <c r="J100" t="inlineStr">
-        <is>
-          <t>CAO Grondstoffen Energie en Omgeving Services 2022-2023-2024 - signed.json, Cao_GEO_PROCES_2018_2019.json, cao_GEO_vernieuwd_definitief.json, GEO_Cao.json, CAO GEO PROCES en SERVICES 2020.json, cao_afval_en_milieu_proces_2013_2014_met_handtek.json, cao_Afval_en_Milieu_Proces_2014_2015.json, Energiebedrijf_1471.json, Cao GEO SERVICES 2024-2026.json, Cao_Afval_en_Milieu_Proces_2016_2017.json, Cao 2022-2024 Proces - ondertekening.json, CAO Grondstoffen Energie en Omgeving PROCES 2021 20210503 ondertekend.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -3639,17 +4399,25 @@
       <c r="E101" t="n">
         <v>14</v>
       </c>
-      <c r="F101" t="inlineStr"/>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G101" t="n">
         <v>14</v>
       </c>
-      <c r="H101" t="inlineStr"/>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I101" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>Tuinzaadbedrijven 1 januari 2023 - 31 december 2023 definitief.json, Cao_Tuinzaadbedrijven_20180101___20191231.json, Afspraken cao Tuinzaadbedrijven 2020 versie definitief.json, Tekst CAO Tuinzaadbedrijven 1 januari 2024 - 31 december 2025 def.json, Plantum___CAO_2011____2014.json, Tuinzaadbedrijven 2021 - 2022 TTW augustus 2022.json, CAO_Tuinzaadbedrijven_1_jan_2018_tm_31_dec_2019.json, Plantum___definitieve_CAO_2011___2014.json, defintieve tekst CAO Tuinzaadbedrijven 2021 - 2022.json, Tuinzaadbedrijven 2021 - 2022 TTW2.json, CAO_Tuinzaden_2016_2017.json, Tuinzaden_cao_2014_2016.json, 2e__gem_t_t_w__1_10_2011___01_01_2014.json, Plantum_ttw_CAO_2011_2014.json</t>
+          <t>Tuinzaadbedrijven 1 januari 2023 - 31 december 2023 definitief.json, Cao_Tuinzaadbedrijven_20180101___20191231.json, Afspraken cao Tuinzaadbedrijven 2020 versie definitief.json, Plantum___CAO_2011____2014.json, Tuinzaadbedrijven 2021 - 2022 TTW augustus 2022.json, CAO_Tuinzaadbedrijven_1_jan_2018_tm_31_dec_2019.json, defintieve tekst CAO Tuinzaadbedrijven 2021 - 2022.json, Tuinzaadbedrijven 2021 - 2022 TTW2.json, CAO_Tuinzaden_2016_2017.json, Tuinzaden_cao_2014_2016.json, 2e__gem_t_t_w__1_10_2011___01_01_2014.json, Plantum_ttw_CAO_2011_2014.json</t>
         </is>
       </c>
     </row>
@@ -3671,15 +4439,27 @@
       <c r="E102" t="n">
         <v>2</v>
       </c>
-      <c r="F102" t="inlineStr"/>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G102" t="n">
         <v>2</v>
       </c>
-      <c r="H102" t="inlineStr"/>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I102" t="n">
         <v>28</v>
       </c>
-      <c r="J102" t="inlineStr"/>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -3699,11 +4479,19 @@
       <c r="E103" t="n">
         <v>2</v>
       </c>
-      <c r="F103" t="inlineStr"/>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G103" t="n">
         <v>2</v>
       </c>
-      <c r="H103" t="inlineStr"/>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I103" t="n">
         <v>0</v>
       </c>
@@ -3731,17 +4519,25 @@
       <c r="E104" t="n">
         <v>17</v>
       </c>
-      <c r="F104" t="inlineStr"/>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G104" t="n">
         <v>17</v>
       </c>
-      <c r="H104" t="inlineStr"/>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I104" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>2024_31okt_tekstcaotbvavvschoon_MvD.json, 2022jun30_HWi_CAOtekst_1apr2022-31mrt2023_Cao-Aanmelden_exclCaoFondsOOA.json, 2024Mrt25_schonetekstcao.json, CAOtekst_2014_PvL_6mei2014.json, CAOtekst_1apr2019-31dec2019_PvL_6mei2019.pdf .json, CAOtekst_1apr2017_31mrt2019_PvL_30mei2018.json, 2021nov12_HWi_CAOtekst_1apr2020-31mrt2022.json, CAOtekst_2012_2013_PvL_5jun2012.json, 2024jan30_CAOHH2023-2024.json, CAOtekst_1apr2017_31mrt2019.json, 2020jan8_PvL_CAOtekst_1apr2019-31mrt2020.json, CAOtekst_2012_2013_PvL_26jul2012.json, 2020feb3_PvL_CAOtekst_1apr2019-31mrt2020.json, 2024_17dec_schone_tekstcaotbvavv_MvD4.json, 2025_14jan_schone_tekstcaotbvavv_MvD.json, 2021dec17_HWi_CAOtekst-tbv-Cao-aanmelden_1apr2020-31mrt2022_exclCaoFondsOOA_v2.d.json, CAOtekst_2015_31mrt2017_PvL_11sep2015.json</t>
+          <t>2024_31okt_tekstcaotbvavvschoon_MvD.json, 2022jun30_HWi_CAOtekst_1apr2022-31mrt2023_Cao-Aanmelden_exclCaoFondsOOA.json, 2024Mrt25_schonetekstcao.json, CAOtekst_1apr2019-31dec2019_PvL_6mei2019.pdf .json, 2021nov12_HWi_CAOtekst_1apr2020-31mrt2022.json, CAOtekst_2012_2013_PvL_5jun2012.json, CAOtekst_1apr2017_31mrt2019.json, 2020jan8_PvL_CAOtekst_1apr2019-31mrt2020.json, CAOtekst_2012_2013_PvL_26jul2012.json, 2020feb3_PvL_CAOtekst_1apr2019-31mrt2020.json, 2025_14jan_schone_tekstcaotbvavv_MvD.json, 2021dec17_HWi_CAOtekst-tbv-Cao-aanmelden_1apr2020-31mrt2022_exclCaoFondsOOA_v2.d.json, CAOtekst_2015_31mrt2017_PvL_11sep2015.json</t>
         </is>
       </c>
     </row>
@@ -3763,17 +4559,25 @@
       <c r="E105" t="n">
         <v>14</v>
       </c>
-      <c r="F105" t="inlineStr"/>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G105" t="n">
         <v>14</v>
       </c>
-      <c r="H105" t="inlineStr"/>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>20240725 CAO Particulier Kaaspakhuis 01-01-2024- 1-05-2025 wijzigingen bijgehouden.json, 20072021 CAO-boekje 2021-2022.json, CAO Particulier Kaaspakhuis 01-01-2024 definitief.json, CAO-tekst definitief.docx_1.json, CAO_tekst_integraal.json, CAO_tekst_definitief.json, CAO 2010-2012 tekst.json, CAO-tekst definitief.docx.json, CAO Particulier Kaaspakhuis 2023 versie 17-7-2023.json, CAO Particulier Kaaspakhuis 2023 na ttw versie 1-8-2023.json, CAOtekst_AVV__integraal_.json, CAOtekst_AVV__integraal__verlenging.json, CAO_tekst_integraal1.json, CAO-tekst 2021-2022 OKT schoon.json</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -3795,19 +4599,23 @@
       <c r="E106" t="n">
         <v>13</v>
       </c>
-      <c r="F106" t="inlineStr"/>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G106" t="n">
         <v>13</v>
       </c>
-      <c r="H106" t="inlineStr"/>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I106" t="n">
-        <v>0</v>
-      </c>
-      <c r="J106" t="inlineStr">
-        <is>
-          <t>CAO visdetailhandel 2019-2020 definitieve versie aangeboden aan ministerie.docx .json, cao_tkst_AVV_na_gesprek_ministerie_1.json, Integrale cao-tekst visdetailhandel 2025 geschoond.json, CAO visdetailhandel 2021-2023 def voor ministerie na controle wg.json, Integrale cao-tekst visdetailhandel 2024 .json, Cao visdetailhandel 2025 tussentijdse wijzigingen juni 2025.json, Integrale cao-tekst visdetailhandel 2021-2023.json, Integrale cao-tekst visdetailhandel 2024 (definitieve versie 21 februari 2024).json, VNV_cao_boekje_A5_2015_408280_C.json, CAO_visdetailhandel_per_1__1__2015_org__getekend.json, cao_tkst_AVV_na_gesprek_ministerie.json, visdetailhandel cao en bijlagen.json, Cao_Visdetailhandel_2017_2018.json</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -3827,11 +4635,19 @@
       <c r="E107" t="n">
         <v>12</v>
       </c>
-      <c r="F107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G107" t="n">
         <v>12</v>
       </c>
-      <c r="H107" t="inlineStr"/>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I107" t="n">
         <v>0</v>
       </c>
@@ -3859,11 +4675,19 @@
       <c r="E108" t="n">
         <v>2</v>
       </c>
-      <c r="F108" t="inlineStr"/>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G108" t="n">
         <v>2</v>
       </c>
-      <c r="H108" t="inlineStr"/>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I108" t="n">
         <v>0</v>
       </c>
@@ -3891,17 +4715,25 @@
       <c r="E109" t="n">
         <v>18</v>
       </c>
-      <c r="F109" t="inlineStr"/>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G109" t="n">
         <v>18</v>
       </c>
-      <c r="H109" t="inlineStr"/>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I109" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>HB 5e editie 2024_2.json, m_en_t_islollatiebedrijf_kvo.json, CAO_ISO_2017_2019__TTW.json, CAO ISO 2019 2021 SZW TTW V2 wagweu.docx.json, CAO_ISO_arcering___wijz_AOW_LT.json, CAO_ISO_17_19.json, CAO ISO 2021 2024_1.json, CAO ISO 2021 2024.json, HB 5e editie 2024.json, CAO_ISO_2017_2019__TTW_GP_nov_2017.json, CAO ISO 2021 2024b.json, M_T_Isolatie_Cao___Handboek.json, CAO_ISO_TTW_JULI.json, CAO_ISO_2017_2019__TTW_LL_nov_2018.json, CAO_ISO.json, CAO ISO 2019 2021 SZW TTW wagweu art 64.docx.json, Isolatie_cao_en_handboek.json, HB 5e editie 2024_1.json</t>
+          <t>CAO_ISO_2017_2019__TTW.json, CAO ISO 2019 2021 SZW TTW V2 wagweu.docx.json, CAO_ISO_arcering___wijz_AOW_LT.json, CAO ISO 2021 2024_1.json, CAO ISO 2021 2024.json, HB 5e editie 2024.json, CAO_ISO_2017_2019__TTW_GP_nov_2017.json, CAO ISO 2021 2024b.json, M_T_Isolatie_Cao___Handboek.json, CAO_ISO_TTW_JULI.json, CAO_ISO_2017_2019__TTW_LL_nov_2018.json, CAO_ISO.json, CAO ISO 2019 2021 SZW TTW wagweu art 64.docx.json, Isolatie_cao_en_handboek.json</t>
         </is>
       </c>
     </row>

</xml_diff>